<commit_message>
Refactor - final stages - preparing for release.
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D197E81F-7A5A-2F40-A3B1-AC82485487E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2436B5C8-EB2C-C445-8600-A3553B56AFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="500" windowWidth="34680" windowHeight="20940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="500" windowWidth="21080" windowHeight="23880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -4659,9 +4659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactor, build AA trees and update website
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2436B5C8-EB2C-C445-8600-A3553B56AFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBB099-D07B-924C-A206-1CE67AC7146A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="500" windowWidth="21080" windowHeight="23880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="500" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -4660,8 +4660,8 @@
   <dimension ref="A1:O165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5956,7 +5956,7 @@
         <v>538</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7" t="s">
@@ -6001,7 +6001,7 @@
         <v>538</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7" t="s">
@@ -6046,7 +6046,7 @@
         <v>538</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7" t="s">
@@ -6091,7 +6091,7 @@
         <v>538</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
@@ -6136,7 +6136,7 @@
         <v>538</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
@@ -6181,7 +6181,7 @@
         <v>538</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
@@ -6226,7 +6226,7 @@
         <v>538</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
@@ -6271,7 +6271,7 @@
         <v>538</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
@@ -6316,7 +6316,7 @@
         <v>538</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
@@ -6361,7 +6361,7 @@
         <v>538</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
@@ -6406,7 +6406,7 @@
         <v>538</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7" t="s">
@@ -6451,7 +6451,7 @@
         <v>538</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7" t="s">
@@ -6494,7 +6494,7 @@
         <v>538</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7" t="s">
@@ -6539,7 +6539,7 @@
         <v>538</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7" t="s">
@@ -6584,7 +6584,7 @@
         <v>538</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7" t="s">
@@ -6629,7 +6629,7 @@
         <v>538</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7" t="s">
@@ -6673,8 +6673,8 @@
       <c r="G45" s="28" t="s">
         <v>538</v>
       </c>
-      <c r="H45" s="28" t="s">
-        <v>820</v>
+      <c r="H45" s="7" t="s">
+        <v>501</v>
       </c>
       <c r="I45" s="28"/>
       <c r="J45" s="7" t="s">
@@ -6719,7 +6719,7 @@
         <v>538</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="7" t="s">
@@ -6764,7 +6764,7 @@
         <v>538</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7" t="s">
@@ -6809,7 +6809,7 @@
         <v>538</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7" t="s">
@@ -6854,7 +6854,7 @@
         <v>538</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7" t="s">
@@ -6899,7 +6899,7 @@
         <v>538</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="7" t="s">
@@ -6944,7 +6944,7 @@
         <v>538</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7" t="s">
@@ -6989,7 +6989,7 @@
         <v>538</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7" t="s">
@@ -7034,7 +7034,7 @@
         <v>538</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7" t="s">
@@ -7079,7 +7079,7 @@
         <v>538</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="7" t="s">
@@ -7124,7 +7124,7 @@
         <v>538</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="7" t="s">
@@ -7169,7 +7169,7 @@
         <v>538</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>820</v>
+        <v>501</v>
       </c>
       <c r="I56" s="7"/>
       <c r="J56" s="7" t="s">
@@ -7214,7 +7214,7 @@
         <v>538</v>
       </c>
       <c r="H57" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I57" s="31"/>
       <c r="J57" s="31" t="s">
@@ -7259,7 +7259,7 @@
         <v>538</v>
       </c>
       <c r="H58" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I58" s="31"/>
       <c r="J58" s="31" t="s">
@@ -7304,7 +7304,7 @@
         <v>538</v>
       </c>
       <c r="H59" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I59" s="31"/>
       <c r="J59" s="31" t="s">
@@ -7349,7 +7349,7 @@
         <v>538</v>
       </c>
       <c r="H60" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I60" s="31"/>
       <c r="J60" s="31" t="s">
@@ -7394,7 +7394,7 @@
         <v>538</v>
       </c>
       <c r="H61" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I61" s="31"/>
       <c r="J61" s="31" t="s">
@@ -7439,7 +7439,7 @@
         <v>538</v>
       </c>
       <c r="H62" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I62" s="31"/>
       <c r="J62" s="31" t="s">
@@ -7484,7 +7484,7 @@
         <v>538</v>
       </c>
       <c r="H63" s="31" t="s">
-        <v>820</v>
+        <v>401</v>
       </c>
       <c r="I63" s="31"/>
       <c r="J63" s="31" t="s">
@@ -7531,7 +7531,7 @@
       <c r="H64" s="34" t="s">
         <v>820</v>
       </c>
-      <c r="I64" s="24"/>
+      <c r="I64" s="34"/>
       <c r="J64" s="24" t="s">
         <v>505</v>
       </c>
@@ -8026,7 +8026,7 @@
       <c r="H75" s="34" t="s">
         <v>820</v>
       </c>
-      <c r="I75" s="58"/>
+      <c r="I75" s="34"/>
       <c r="J75" s="58" t="s">
         <v>801</v>
       </c>

</xml_diff>

<commit_message>
AA tree-builds for subgenera
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBB099-D07B-924C-A206-1CE67AC7146A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93267EA0-9DC5-3D42-B441-AF8E29643F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="500" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25120" yWindow="4180" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -4660,8 +4660,8 @@
   <dimension ref="A1:O165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="A1:O164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8388,10 +8388,10 @@
       </c>
       <c r="I83" s="38"/>
       <c r="J83" s="38" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="K83" s="38" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="L83" s="38" t="s">
         <v>639</v>
@@ -8433,10 +8433,10 @@
       </c>
       <c r="I84" s="38"/>
       <c r="J84" s="38" t="s">
-        <v>79</v>
+        <v>617</v>
       </c>
       <c r="K84" s="38" t="s">
-        <v>79</v>
+        <v>617</v>
       </c>
       <c r="L84" s="38" t="s">
         <v>639</v>

</xml_diff>

<commit_message>
Refactor - add Mupulungu virus
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27151FA5-30EC-4742-90DB-9A6970400EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D3B359-35FA-3548-8F64-FBF23F5F49BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9920" yWindow="1540" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="removed" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$N$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$N$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="824">
   <si>
     <t>AY632538</t>
   </si>
@@ -2495,6 +2495,21 @@
   </si>
   <si>
     <t>TBFV</t>
+  </si>
+  <si>
+    <t>LC582740</t>
+  </si>
+  <si>
+    <t>Mpulungu flavivirus</t>
+  </si>
+  <si>
+    <t>Mpulungu</t>
+  </si>
+  <si>
+    <t>Rhipicephalus muhsamae</t>
+  </si>
+  <si>
+    <t>ZT17-1078</t>
   </si>
 </sst>
 </file>
@@ -4641,11 +4656,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O163"/>
+  <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4661,7 +4676,7 @@
     <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
     <col min="15" max="15" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8346,59 +8361,59 @@
       </c>
     </row>
     <row r="83" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A83" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B83" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="C83" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="D83" s="40" t="s">
-        <v>734</v>
-      </c>
-      <c r="E83" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="F83" s="40" t="s">
+      <c r="A83" s="37" t="s">
+        <v>819</v>
+      </c>
+      <c r="B83" s="38" t="s">
+        <v>820</v>
+      </c>
+      <c r="C83" s="38" t="s">
+        <v>821</v>
+      </c>
+      <c r="D83" s="38" t="s">
+        <v>734</v>
+      </c>
+      <c r="E83" s="38" t="s">
+        <v>659</v>
+      </c>
+      <c r="F83" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="G83" s="40" t="s">
-        <v>818</v>
-      </c>
-      <c r="H83" s="40" t="s">
-        <v>817</v>
-      </c>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40" t="s">
-        <v>515</v>
-      </c>
-      <c r="K83" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="L83" s="40" t="s">
-        <v>620</v>
-      </c>
-      <c r="M83" s="16" t="s">
-        <v>460</v>
-      </c>
-      <c r="N83" s="16" t="s">
-        <v>475</v>
+      <c r="G83" s="38" t="s">
+        <v>821</v>
+      </c>
+      <c r="H83" s="38" t="s">
+        <v>817</v>
+      </c>
+      <c r="I83" s="38"/>
+      <c r="J83" s="38" t="s">
+        <v>617</v>
+      </c>
+      <c r="K83" s="38" t="s">
+        <v>617</v>
+      </c>
+      <c r="L83" s="38" t="s">
+        <v>822</v>
+      </c>
+      <c r="M83" s="15" t="s">
+        <v>823</v>
+      </c>
+      <c r="N83" s="13" t="s">
+        <v>474</v>
       </c>
       <c r="O83" s="16" t="s">
-        <v>152</v>
+        <v>822</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C84" s="40" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D84" s="40" t="s">
         <v>734</v>
@@ -8417,33 +8432,33 @@
       </c>
       <c r="I84" s="40"/>
       <c r="J84" s="40" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K84" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L84" s="40" t="s">
-        <v>621</v>
-      </c>
-      <c r="M84" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="N84" s="13" t="s">
-        <v>474</v>
+        <v>620</v>
+      </c>
+      <c r="M84" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="N84" s="16" t="s">
+        <v>475</v>
       </c>
       <c r="O84" s="16" t="s">
-        <v>462</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
-        <v>258</v>
+        <v>60</v>
       </c>
       <c r="B85" s="40" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>417</v>
+        <v>461</v>
       </c>
       <c r="D85" s="40" t="s">
         <v>734</v>
@@ -8462,33 +8477,33 @@
       </c>
       <c r="I85" s="40"/>
       <c r="J85" s="40" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="K85" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L85" s="40" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="M85" s="15" t="s">
-        <v>1</v>
+        <v>463</v>
       </c>
       <c r="N85" s="13" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="O85" s="16" t="s">
-        <v>154</v>
+        <v>462</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A86" s="39" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="B86" s="40" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="C86" s="40" t="s">
-        <v>313</v>
+        <v>417</v>
       </c>
       <c r="D86" s="40" t="s">
         <v>734</v>
@@ -8507,33 +8522,33 @@
       </c>
       <c r="I86" s="40"/>
       <c r="J86" s="40" t="s">
-        <v>640</v>
+        <v>515</v>
       </c>
       <c r="K86" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L86" s="40" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="M86" s="15" t="s">
         <v>1</v>
       </c>
       <c r="N86" s="13" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="O86" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A87" s="39" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="C87" s="40" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="D87" s="40" t="s">
         <v>734</v>
@@ -8552,7 +8567,7 @@
       </c>
       <c r="I87" s="40"/>
       <c r="J87" s="40" t="s">
-        <v>515</v>
+        <v>640</v>
       </c>
       <c r="K87" s="40" t="s">
         <v>190</v>
@@ -8561,24 +8576,24 @@
         <v>612</v>
       </c>
       <c r="M87" s="15" t="s">
-        <v>363</v>
+        <v>1</v>
       </c>
       <c r="N87" s="13" t="s">
         <v>471</v>
       </c>
       <c r="O87" s="16" t="s">
-        <v>362</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="39" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C88" s="40" t="s">
-        <v>202</v>
+        <v>361</v>
       </c>
       <c r="D88" s="40" t="s">
         <v>734</v>
@@ -8603,27 +8618,27 @@
         <v>190</v>
       </c>
       <c r="L88" s="40" t="s">
-        <v>641</v>
+        <v>612</v>
       </c>
       <c r="M88" s="15" t="s">
-        <v>1</v>
+        <v>363</v>
       </c>
       <c r="N88" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="O88" s="16" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
-        <v>58</v>
+        <v>220</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>186</v>
+        <v>101</v>
       </c>
       <c r="C89" s="40" t="s">
-        <v>456</v>
+        <v>202</v>
       </c>
       <c r="D89" s="40" t="s">
         <v>734</v>
@@ -8642,33 +8657,33 @@
       </c>
       <c r="I89" s="40"/>
       <c r="J89" s="40" t="s">
-        <v>618</v>
+        <v>515</v>
       </c>
       <c r="K89" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L89" s="40" t="s">
-        <v>620</v>
+        <v>641</v>
       </c>
       <c r="M89" s="15" t="s">
-        <v>458</v>
+        <v>1</v>
       </c>
       <c r="N89" s="13" t="s">
         <v>473</v>
       </c>
       <c r="O89" s="16" t="s">
-        <v>457</v>
+        <v>345</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
-        <v>237</v>
+        <v>58</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>120</v>
+        <v>186</v>
       </c>
       <c r="C90" s="40" t="s">
-        <v>372</v>
+        <v>456</v>
       </c>
       <c r="D90" s="40" t="s">
         <v>734</v>
@@ -8687,33 +8702,33 @@
       </c>
       <c r="I90" s="40"/>
       <c r="J90" s="40" t="s">
-        <v>558</v>
+        <v>618</v>
       </c>
       <c r="K90" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L90" s="40" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="M90" s="15" t="s">
-        <v>373</v>
+        <v>458</v>
       </c>
       <c r="N90" s="13" t="s">
         <v>473</v>
       </c>
       <c r="O90" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="39" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B91" s="40" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C91" s="40" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="D91" s="40" t="s">
         <v>734</v>
@@ -8732,7 +8747,7 @@
       </c>
       <c r="I91" s="40"/>
       <c r="J91" s="40" t="s">
-        <v>515</v>
+        <v>558</v>
       </c>
       <c r="K91" s="40" t="s">
         <v>190</v>
@@ -8741,10 +8756,10 @@
         <v>612</v>
       </c>
       <c r="M91" s="15" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="N91" s="13" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="O91" s="16" t="s">
         <v>118</v>
@@ -8752,13 +8767,13 @@
     </row>
     <row r="92" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A92" s="39" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B92" s="40" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>294</v>
+        <v>359</v>
       </c>
       <c r="D92" s="40" t="s">
         <v>734</v>
@@ -8777,33 +8792,33 @@
       </c>
       <c r="I92" s="40"/>
       <c r="J92" s="40" t="s">
-        <v>619</v>
+        <v>515</v>
       </c>
       <c r="K92" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L92" s="40" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="M92" s="15" t="s">
-        <v>296</v>
+        <v>360</v>
       </c>
       <c r="N92" s="13" t="s">
-        <v>471</v>
-      </c>
-      <c r="O92" s="42" t="s">
-        <v>295</v>
+        <v>472</v>
+      </c>
+      <c r="O92" s="16" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>61</v>
+        <v>212</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="C93" s="40" t="s">
-        <v>464</v>
+        <v>294</v>
       </c>
       <c r="D93" s="40" t="s">
         <v>734</v>
@@ -8822,33 +8837,33 @@
       </c>
       <c r="I93" s="40"/>
       <c r="J93" s="40" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="K93" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L93" s="40" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="M93" s="15" t="s">
-        <v>465</v>
+        <v>296</v>
       </c>
       <c r="N93" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="O93" s="16" t="s">
-        <v>208</v>
+        <v>471</v>
+      </c>
+      <c r="O93" s="42" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A94" s="39" t="s">
-        <v>269</v>
+        <v>61</v>
       </c>
       <c r="B94" s="40" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C94" s="40" t="s">
-        <v>431</v>
+        <v>464</v>
       </c>
       <c r="D94" s="40" t="s">
         <v>734</v>
@@ -8867,33 +8882,33 @@
       </c>
       <c r="I94" s="40"/>
       <c r="J94" s="40" t="s">
-        <v>515</v>
+        <v>618</v>
       </c>
       <c r="K94" s="40" t="s">
         <v>190</v>
       </c>
       <c r="L94" s="40" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="M94" s="15" t="s">
-        <v>48</v>
+        <v>465</v>
       </c>
       <c r="N94" s="13" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="O94" s="16" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A95" s="39" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="B95" s="40" t="s">
-        <v>99</v>
+        <v>174</v>
       </c>
       <c r="C95" s="40" t="s">
-        <v>342</v>
+        <v>431</v>
       </c>
       <c r="D95" s="40" t="s">
         <v>734</v>
@@ -8918,27 +8933,27 @@
         <v>190</v>
       </c>
       <c r="L95" s="40" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="M95" s="15" t="s">
-        <v>343</v>
+        <v>48</v>
       </c>
       <c r="N95" s="13" t="s">
         <v>473</v>
       </c>
       <c r="O95" s="16" t="s">
-        <v>1</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="39" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>191</v>
+        <v>99</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>297</v>
+        <v>342</v>
       </c>
       <c r="D96" s="40" t="s">
         <v>734</v>
@@ -8963,13 +8978,13 @@
         <v>190</v>
       </c>
       <c r="L96" s="40" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="M96" s="15" t="s">
-        <v>298</v>
+        <v>343</v>
       </c>
       <c r="N96" s="13" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="O96" s="16" t="s">
         <v>1</v>
@@ -8977,13 +8992,13 @@
     </row>
     <row r="97" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="39" t="s">
-        <v>257</v>
+        <v>4</v>
       </c>
       <c r="B97" s="40" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>415</v>
+        <v>297</v>
       </c>
       <c r="D97" s="40" t="s">
         <v>734</v>
@@ -9008,72 +9023,72 @@
         <v>190</v>
       </c>
       <c r="L97" s="40" t="s">
+        <v>616</v>
+      </c>
+      <c r="M97" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="N97" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="O97" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="B98" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C98" s="40" t="s">
+        <v>415</v>
+      </c>
+      <c r="D98" s="40" t="s">
+        <v>734</v>
+      </c>
+      <c r="E98" s="40" t="s">
+        <v>659</v>
+      </c>
+      <c r="F98" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="G98" s="40" t="s">
+        <v>818</v>
+      </c>
+      <c r="H98" s="40" t="s">
+        <v>817</v>
+      </c>
+      <c r="I98" s="40"/>
+      <c r="J98" s="40" t="s">
+        <v>515</v>
+      </c>
+      <c r="K98" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="L98" s="40" t="s">
         <v>620</v>
       </c>
-      <c r="M97" s="15" t="s">
+      <c r="M98" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="N97" s="13" t="s">
+      <c r="N98" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="O97" s="16" t="s">
+      <c r="O98" s="16" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A98" s="47" t="s">
-        <v>550</v>
-      </c>
-      <c r="B98" s="48" t="s">
-        <v>553</v>
-      </c>
-      <c r="C98" s="49" t="s">
-        <v>600</v>
-      </c>
-      <c r="D98" s="49" t="s">
-        <v>734</v>
-      </c>
-      <c r="E98" s="49" t="s">
-        <v>659</v>
-      </c>
-      <c r="F98" s="49" t="s">
-        <v>479</v>
-      </c>
-      <c r="G98" s="49" t="s">
-        <v>779</v>
-      </c>
-      <c r="H98" s="49" t="s">
-        <v>817</v>
-      </c>
-      <c r="I98" s="49"/>
-      <c r="J98" s="49" t="s">
-        <v>558</v>
-      </c>
-      <c r="K98" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L98" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M98" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N98" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="O98" s="16" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="47" t="s">
-        <v>478</v>
+        <v>550</v>
       </c>
       <c r="B99" s="48" t="s">
-        <v>485</v>
+        <v>553</v>
       </c>
       <c r="C99" s="49" t="s">
-        <v>482</v>
+        <v>600</v>
       </c>
       <c r="D99" s="49" t="s">
         <v>734</v>
@@ -9092,7 +9107,7 @@
       </c>
       <c r="I99" s="49"/>
       <c r="J99" s="49" t="s">
-        <v>537</v>
+        <v>558</v>
       </c>
       <c r="K99" s="14" t="s">
         <v>195</v>
@@ -9106,19 +9121,19 @@
       <c r="N99" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O99" s="46" t="s">
-        <v>536</v>
+      <c r="O99" s="16" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="47" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B100" s="48" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="C100" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D100" s="49" t="s">
         <v>734</v>
@@ -9137,7 +9152,7 @@
       </c>
       <c r="I100" s="49"/>
       <c r="J100" s="49" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="K100" s="14" t="s">
         <v>195</v>
@@ -9152,18 +9167,18 @@
         <v>1</v>
       </c>
       <c r="O100" s="46" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="101" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A101" s="47" t="s">
-        <v>622</v>
+        <v>483</v>
       </c>
       <c r="B101" s="48" t="s">
-        <v>623</v>
+        <v>480</v>
       </c>
       <c r="C101" s="49" t="s">
-        <v>794</v>
+        <v>481</v>
       </c>
       <c r="D101" s="49" t="s">
         <v>734</v>
@@ -9182,7 +9197,7 @@
       </c>
       <c r="I101" s="49"/>
       <c r="J101" s="49" t="s">
-        <v>624</v>
+        <v>535</v>
       </c>
       <c r="K101" s="14" t="s">
         <v>195</v>
@@ -9196,17 +9211,19 @@
       <c r="N101" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O101" s="46"/>
+      <c r="O101" s="46" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="102" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A102" s="47" t="s">
-        <v>769</v>
+        <v>622</v>
       </c>
       <c r="B102" s="48" t="s">
-        <v>770</v>
+        <v>623</v>
       </c>
       <c r="C102" s="49" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D102" s="49" t="s">
         <v>734</v>
@@ -9224,23 +9241,32 @@
         <v>817</v>
       </c>
       <c r="I102" s="49"/>
-      <c r="J102" s="49"/>
+      <c r="J102" s="49" t="s">
+        <v>624</v>
+      </c>
       <c r="K102" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L102" s="14" t="s">
         <v>195</v>
       </c>
+      <c r="M102" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N102" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O102" s="46"/>
     </row>
     <row r="103" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A103" s="47" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B103" s="48" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C103" s="49" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="D103" s="49" t="s">
         <v>734</v>
@@ -9268,13 +9294,13 @@
     </row>
     <row r="104" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A104" s="47" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B104" s="48" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C104" s="49" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="D104" s="49" t="s">
         <v>734</v>
@@ -9302,13 +9328,13 @@
     </row>
     <row r="105" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A105" s="47" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B105" s="48" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C105" s="49" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D105" s="49" t="s">
         <v>734</v>
@@ -9333,19 +9359,16 @@
       <c r="L105" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="O105" s="46" t="s">
-        <v>782</v>
-      </c>
     </row>
     <row r="106" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A106" s="47" t="s">
-        <v>606</v>
+        <v>777</v>
       </c>
       <c r="B106" s="48" t="s">
-        <v>484</v>
+        <v>778</v>
       </c>
       <c r="C106" s="49" t="s">
-        <v>601</v>
+        <v>797</v>
       </c>
       <c r="D106" s="49" t="s">
         <v>734</v>
@@ -9357,40 +9380,32 @@
         <v>479</v>
       </c>
       <c r="G106" s="49" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H106" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I106" s="49"/>
-      <c r="J106" s="49" t="s">
-        <v>526</v>
-      </c>
+      <c r="J106" s="49"/>
       <c r="K106" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L106" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M106" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N106" s="15" t="s">
-        <v>1</v>
-      </c>
       <c r="O106" s="46" t="s">
-        <v>487</v>
+        <v>782</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A107" s="47" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B107" s="48" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C107" s="49" t="s">
-        <v>660</v>
+        <v>601</v>
       </c>
       <c r="D107" s="49" t="s">
         <v>734</v>
@@ -9409,7 +9424,7 @@
       </c>
       <c r="I107" s="49"/>
       <c r="J107" s="49" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K107" s="14" t="s">
         <v>195</v>
@@ -9424,18 +9439,18 @@
         <v>1</v>
       </c>
       <c r="O107" s="46" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A108" s="47" t="s">
-        <v>773</v>
+        <v>607</v>
       </c>
       <c r="B108" s="48" t="s">
-        <v>774</v>
+        <v>486</v>
       </c>
       <c r="C108" s="49" t="s">
-        <v>792</v>
+        <v>660</v>
       </c>
       <c r="D108" s="49" t="s">
         <v>734</v>
@@ -9453,23 +9468,34 @@
         <v>817</v>
       </c>
       <c r="I108" s="49"/>
-      <c r="J108" s="49"/>
+      <c r="J108" s="49" t="s">
+        <v>527</v>
+      </c>
       <c r="K108" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L108" s="14" t="s">
         <v>195</v>
+      </c>
+      <c r="M108" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N108" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O108" s="46" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A109" s="47" t="s">
-        <v>551</v>
+        <v>773</v>
       </c>
       <c r="B109" s="48" t="s">
-        <v>552</v>
+        <v>774</v>
       </c>
       <c r="C109" s="49" t="s">
-        <v>602</v>
+        <v>792</v>
       </c>
       <c r="D109" s="49" t="s">
         <v>734</v>
@@ -9481,40 +9507,29 @@
         <v>479</v>
       </c>
       <c r="G109" s="49" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H109" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I109" s="49"/>
-      <c r="J109" s="49" t="s">
-        <v>560</v>
-      </c>
+      <c r="J109" s="49"/>
       <c r="K109" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L109" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="M109" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N109" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="O109" s="16" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A110" s="47" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B110" s="48" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C110" s="49" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D110" s="49" t="s">
         <v>734</v>
@@ -9533,7 +9548,7 @@
       </c>
       <c r="I110" s="49"/>
       <c r="J110" s="49" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="K110" s="14" t="s">
         <v>195</v>
@@ -9548,18 +9563,18 @@
         <v>1</v>
       </c>
       <c r="O110" s="16" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A111" s="47" t="s">
-        <v>216</v>
+        <v>549</v>
       </c>
       <c r="B111" s="48" t="s">
-        <v>93</v>
+        <v>554</v>
       </c>
       <c r="C111" s="49" t="s">
-        <v>333</v>
+        <v>599</v>
       </c>
       <c r="D111" s="49" t="s">
         <v>734</v>
@@ -9568,17 +9583,17 @@
         <v>659</v>
       </c>
       <c r="F111" s="49" t="s">
-        <v>323</v>
+        <v>479</v>
       </c>
       <c r="G111" s="49" t="s">
-        <v>541</v>
+        <v>781</v>
       </c>
       <c r="H111" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I111" s="49"/>
       <c r="J111" s="49" t="s">
-        <v>518</v>
+        <v>556</v>
       </c>
       <c r="K111" s="14" t="s">
         <v>195</v>
@@ -9593,18 +9608,18 @@
         <v>1</v>
       </c>
       <c r="O111" s="16" t="s">
-        <v>135</v>
+        <v>555</v>
       </c>
     </row>
     <row r="112" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A112" s="47" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B112" s="48" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C112" s="49" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="D112" s="49" t="s">
         <v>734</v>
@@ -9616,7 +9631,7 @@
         <v>323</v>
       </c>
       <c r="G112" s="49" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H112" s="49" t="s">
         <v>817</v>
@@ -9632,10 +9647,10 @@
         <v>195</v>
       </c>
       <c r="M112" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="N112" s="13" t="s">
-        <v>472</v>
+        <v>1</v>
+      </c>
+      <c r="N112" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="O112" s="16" t="s">
         <v>135</v>
@@ -9643,13 +9658,13 @@
     </row>
     <row r="113" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A113" s="47" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B113" s="48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C113" s="49" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D113" s="49" t="s">
         <v>734</v>
@@ -9661,14 +9676,14 @@
         <v>323</v>
       </c>
       <c r="G113" s="49" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H113" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I113" s="49"/>
       <c r="J113" s="49" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="K113" s="14" t="s">
         <v>195</v>
@@ -9677,24 +9692,24 @@
         <v>195</v>
       </c>
       <c r="M113" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="N113" s="13" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O113" s="16" t="s">
-        <v>490</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A114" s="47" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B114" s="48" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C114" s="49" t="s">
-        <v>589</v>
+        <v>349</v>
       </c>
       <c r="D114" s="49" t="s">
         <v>734</v>
@@ -9706,14 +9721,14 @@
         <v>323</v>
       </c>
       <c r="G114" s="49" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="H114" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I114" s="49"/>
       <c r="J114" s="49" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="K114" s="14" t="s">
         <v>195</v>
@@ -9722,24 +9737,24 @@
         <v>195</v>
       </c>
       <c r="M114" s="15" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="N114" s="13" t="s">
         <v>1</v>
       </c>
       <c r="O114" s="16" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A115" s="47" t="s">
-        <v>284</v>
+        <v>230</v>
       </c>
       <c r="B115" s="48" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="C115" s="49" t="s">
-        <v>420</v>
+        <v>589</v>
       </c>
       <c r="D115" s="49" t="s">
         <v>734</v>
@@ -9751,14 +9766,14 @@
         <v>323</v>
       </c>
       <c r="G115" s="49" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="H115" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I115" s="49"/>
       <c r="J115" s="49" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="K115" s="14" t="s">
         <v>195</v>
@@ -9767,24 +9782,24 @@
         <v>195</v>
       </c>
       <c r="M115" s="15" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="N115" s="13" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O115" s="16" t="s">
-        <v>489</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A116" s="47" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="B116" s="48" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C116" s="49" t="s">
-        <v>590</v>
+        <v>420</v>
       </c>
       <c r="D116" s="49" t="s">
         <v>734</v>
@@ -9796,14 +9811,14 @@
         <v>323</v>
       </c>
       <c r="G116" s="49" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="H116" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I116" s="49"/>
       <c r="J116" s="49" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="K116" s="14" t="s">
         <v>195</v>
@@ -9812,24 +9827,24 @@
         <v>195</v>
       </c>
       <c r="M116" s="15" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="N116" s="13" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="O116" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A117" s="47" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="B117" s="48" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
       <c r="C117" s="49" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D117" s="49" t="s">
         <v>734</v>
@@ -9841,14 +9856,14 @@
         <v>323</v>
       </c>
       <c r="G117" s="49" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="H117" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I117" s="49"/>
       <c r="J117" s="49" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K117" s="14" t="s">
         <v>195</v>
@@ -9857,24 +9872,24 @@
         <v>195</v>
       </c>
       <c r="M117" s="15" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="N117" s="13" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="O117" s="16" t="s">
-        <v>110</v>
+        <v>490</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A118" s="47" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C118" s="49" t="s">
-        <v>407</v>
+        <v>593</v>
       </c>
       <c r="D118" s="49" t="s">
         <v>734</v>
@@ -9886,14 +9901,14 @@
         <v>323</v>
       </c>
       <c r="G118" s="49" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="H118" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I118" s="49"/>
       <c r="J118" s="49" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="K118" s="14" t="s">
         <v>195</v>
@@ -9902,24 +9917,24 @@
         <v>195</v>
       </c>
       <c r="M118" s="15" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="N118" s="13" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="O118" s="16" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A119" s="47" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B119" s="48" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="C119" s="49" t="s">
-        <v>591</v>
+        <v>407</v>
       </c>
       <c r="D119" s="49" t="s">
         <v>734</v>
@@ -9931,14 +9946,14 @@
         <v>323</v>
       </c>
       <c r="G119" s="49" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H119" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I119" s="49"/>
       <c r="J119" s="49" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="K119" s="14" t="s">
         <v>195</v>
@@ -9953,18 +9968,18 @@
         <v>471</v>
       </c>
       <c r="O119" s="16" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A120" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="B120" s="49" t="s">
-        <v>166</v>
+        <v>251</v>
+      </c>
+      <c r="B120" s="48" t="s">
+        <v>142</v>
       </c>
       <c r="C120" s="49" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D120" s="49" t="s">
         <v>734</v>
@@ -9976,14 +9991,14 @@
         <v>323</v>
       </c>
       <c r="G120" s="49" t="s">
-        <v>643</v>
+        <v>546</v>
       </c>
       <c r="H120" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I120" s="49"/>
       <c r="J120" s="49" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="K120" s="14" t="s">
         <v>195</v>
@@ -9992,24 +10007,24 @@
         <v>195</v>
       </c>
       <c r="M120" s="15" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="N120" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O120" s="16" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A121" s="47" t="s">
-        <v>644</v>
+        <v>263</v>
       </c>
       <c r="B121" s="49" t="s">
-        <v>645</v>
+        <v>166</v>
       </c>
       <c r="C121" s="49" t="s">
-        <v>646</v>
+        <v>592</v>
       </c>
       <c r="D121" s="49" t="s">
         <v>734</v>
@@ -10021,14 +10036,14 @@
         <v>323</v>
       </c>
       <c r="G121" s="49" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="H121" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I121" s="49"/>
       <c r="J121" s="49" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="K121" s="14" t="s">
         <v>195</v>
@@ -10037,24 +10052,24 @@
         <v>195</v>
       </c>
       <c r="M121" s="15" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="N121" s="13" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O121" s="16" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
     </row>
     <row r="122" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A122" s="47" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
       <c r="B122" s="49" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="C122" s="49" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D122" s="49" t="s">
         <v>734</v>
@@ -10065,74 +10080,84 @@
       <c r="F122" s="49" t="s">
         <v>323</v>
       </c>
-      <c r="G122" s="49"/>
+      <c r="G122" s="49" t="s">
+        <v>647</v>
+      </c>
       <c r="H122" s="49" t="s">
         <v>817</v>
       </c>
       <c r="I122" s="49"/>
       <c r="J122" s="49" t="s">
+        <v>523</v>
+      </c>
+      <c r="K122" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L122" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M122" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N122" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O122" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A123" s="47" t="s">
+        <v>656</v>
+      </c>
+      <c r="B123" s="49" t="s">
+        <v>625</v>
+      </c>
+      <c r="C123" s="49" t="s">
+        <v>648</v>
+      </c>
+      <c r="D123" s="49" t="s">
+        <v>734</v>
+      </c>
+      <c r="E123" s="49" t="s">
+        <v>659</v>
+      </c>
+      <c r="F123" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="G123" s="49"/>
+      <c r="H123" s="49" t="s">
+        <v>817</v>
+      </c>
+      <c r="I123" s="49"/>
+      <c r="J123" s="49" t="s">
         <v>617</v>
       </c>
-      <c r="K122" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L122" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M122" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N122" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O122" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A123" s="59" t="s">
-        <v>747</v>
-      </c>
-      <c r="B123" s="43" t="s">
-        <v>752</v>
-      </c>
-      <c r="C123" s="43" t="s">
-        <v>756</v>
-      </c>
-      <c r="D123" s="43" t="s">
-        <v>734</v>
-      </c>
-      <c r="E123" s="43" t="s">
-        <v>659</v>
-      </c>
-      <c r="F123" s="43" t="s">
-        <v>609</v>
-      </c>
-      <c r="G123" s="43" t="s">
-        <v>768</v>
-      </c>
-      <c r="H123" s="43" t="s">
-        <v>817</v>
-      </c>
-      <c r="I123" s="43"/>
-      <c r="J123" s="43"/>
       <c r="K123" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L123" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M123" s="50"/>
+      <c r="M123" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N123" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O123" s="16" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A124" s="59" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="B124" s="43" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C124" s="43" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D124" s="43" t="s">
         <v>734</v>
@@ -10157,16 +10182,17 @@
       <c r="L124" s="14" t="s">
         <v>195</v>
       </c>
+      <c r="M124" s="50"/>
     </row>
     <row r="125" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A125" s="59" t="s">
-        <v>233</v>
+        <v>750</v>
       </c>
       <c r="B125" s="43" t="s">
-        <v>114</v>
+        <v>754</v>
       </c>
       <c r="C125" s="43" t="s">
-        <v>364</v>
+        <v>757</v>
       </c>
       <c r="D125" s="43" t="s">
         <v>734</v>
@@ -10178,40 +10204,29 @@
         <v>609</v>
       </c>
       <c r="G125" s="43" t="s">
-        <v>364</v>
+        <v>768</v>
       </c>
       <c r="H125" s="43" t="s">
         <v>817</v>
       </c>
       <c r="I125" s="43"/>
-      <c r="J125" s="43" t="s">
-        <v>511</v>
-      </c>
+      <c r="J125" s="43"/>
       <c r="K125" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L125" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="M125" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="N125" s="13" t="s">
-        <v>472</v>
-      </c>
-      <c r="O125" s="16" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A126" s="59" t="s">
-        <v>493</v>
+        <v>233</v>
       </c>
       <c r="B126" s="43" t="s">
-        <v>498</v>
+        <v>114</v>
       </c>
       <c r="C126" s="43" t="s">
-        <v>598</v>
+        <v>364</v>
       </c>
       <c r="D126" s="43" t="s">
         <v>734</v>
@@ -10222,13 +10237,15 @@
       <c r="F126" s="43" t="s">
         <v>609</v>
       </c>
-      <c r="G126" s="43"/>
+      <c r="G126" s="43" t="s">
+        <v>364</v>
+      </c>
       <c r="H126" s="43" t="s">
         <v>817</v>
       </c>
       <c r="I126" s="43"/>
       <c r="J126" s="43" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="K126" s="14" t="s">
         <v>195</v>
@@ -10237,24 +10254,24 @@
         <v>195</v>
       </c>
       <c r="M126" s="15" t="s">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="N126" s="13" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O126" s="16" t="s">
-        <v>499</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A127" s="59" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B127" s="43" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="C127" s="43" t="s">
-        <v>791</v>
+        <v>598</v>
       </c>
       <c r="D127" s="43" t="s">
         <v>734</v>
@@ -10271,7 +10288,7 @@
       </c>
       <c r="I127" s="43"/>
       <c r="J127" s="43" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="K127" s="14" t="s">
         <v>195</v>
@@ -10286,18 +10303,18 @@
         <v>1</v>
       </c>
       <c r="O127" s="16" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="128" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A128" s="59" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B128" s="43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C128" s="43" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D128" s="43" t="s">
         <v>734</v>
@@ -10314,76 +10331,76 @@
       </c>
       <c r="I128" s="43"/>
       <c r="J128" s="43" t="s">
+        <v>512</v>
+      </c>
+      <c r="K128" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L128" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M128" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N128" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O128" s="16" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A129" s="59" t="s">
+        <v>492</v>
+      </c>
+      <c r="B129" s="43" t="s">
+        <v>495</v>
+      </c>
+      <c r="C129" s="43" t="s">
+        <v>790</v>
+      </c>
+      <c r="D129" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E129" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F129" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="G129" s="43"/>
+      <c r="H129" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I129" s="43"/>
+      <c r="J129" s="43" t="s">
         <v>513</v>
       </c>
-      <c r="K128" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L128" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M128" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N128" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O128" s="16" t="s">
+      <c r="K129" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L129" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M129" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N129" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O129" s="16" t="s">
         <v>496</v>
-      </c>
-    </row>
-    <row r="129" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A129" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B129" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="C129" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="D129" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="E129" s="24" t="s">
-        <v>745</v>
-      </c>
-      <c r="F129" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="G129" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="H129" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="I129" s="24"/>
-      <c r="J129" s="24" t="s">
-        <v>613</v>
-      </c>
-      <c r="K129" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L129" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M129" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="N129" s="13"/>
-      <c r="O129" s="16" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A130" s="25" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>585</v>
+        <v>205</v>
       </c>
       <c r="D130" s="24" t="s">
         <v>734</v>
@@ -10394,13 +10411,15 @@
       <c r="F130" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G130" s="24"/>
+      <c r="G130" s="24" t="s">
+        <v>206</v>
+      </c>
       <c r="H130" s="24" t="s">
         <v>817</v>
       </c>
       <c r="I130" s="24"/>
       <c r="J130" s="24" t="s">
-        <v>518</v>
+        <v>613</v>
       </c>
       <c r="K130" s="14" t="s">
         <v>195</v>
@@ -10409,24 +10428,22 @@
         <v>195</v>
       </c>
       <c r="M130" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="N130" s="13" t="s">
-        <v>474</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="N130" s="13"/>
       <c r="O130" s="16" t="s">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A131" s="25" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>604</v>
+        <v>173</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D131" s="24" t="s">
         <v>734</v>
@@ -10443,7 +10460,7 @@
       </c>
       <c r="I131" s="24"/>
       <c r="J131" s="24" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K131" s="14" t="s">
         <v>195</v>
@@ -10451,25 +10468,25 @@
       <c r="L131" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M131" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="N131" s="58" t="s">
-        <v>471</v>
+      <c r="M131" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N131" s="13" t="s">
+        <v>474</v>
       </c>
       <c r="O131" s="16" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A132" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B132" s="26" t="s">
-        <v>163</v>
+        <v>604</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D132" s="24" t="s">
         <v>734</v>
@@ -10486,7 +10503,7 @@
       </c>
       <c r="I132" s="24"/>
       <c r="J132" s="24" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K132" s="14" t="s">
         <v>195</v>
@@ -10495,24 +10512,24 @@
         <v>195</v>
       </c>
       <c r="M132" s="58" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="N132" s="58" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O132" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A133" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B133" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D133" s="24" t="s">
         <v>734</v>
@@ -10538,7 +10555,7 @@
         <v>195</v>
       </c>
       <c r="M133" s="58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N133" s="58" t="s">
         <v>472</v>
@@ -10549,13 +10566,13 @@
     </row>
     <row r="134" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A134" s="25" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B134" s="26" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>32</v>
+        <v>588</v>
       </c>
       <c r="D134" s="24" t="s">
         <v>734</v>
@@ -10572,7 +10589,7 @@
       </c>
       <c r="I134" s="24"/>
       <c r="J134" s="24" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="K134" s="14" t="s">
         <v>195</v>
@@ -10581,24 +10598,24 @@
         <v>195</v>
       </c>
       <c r="M134" s="58" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="N134" s="58" t="s">
         <v>472</v>
       </c>
       <c r="O134" s="16" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
     </row>
     <row r="135" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A135" s="25" t="s">
-        <v>665</v>
+        <v>254</v>
       </c>
       <c r="B135" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C135" s="26" t="s">
-        <v>661</v>
+      <c r="C135" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D135" s="24" t="s">
         <v>734</v>
@@ -10606,16 +10623,16 @@
       <c r="E135" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="F135" s="26" t="s">
+      <c r="F135" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G135" s="26"/>
-      <c r="H135" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="I135" s="26"/>
-      <c r="J135" s="26" t="s">
-        <v>710</v>
+      <c r="G135" s="24"/>
+      <c r="H135" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="I135" s="24"/>
+      <c r="J135" s="24" t="s">
+        <v>508</v>
       </c>
       <c r="K135" s="14" t="s">
         <v>195</v>
@@ -10624,21 +10641,24 @@
         <v>195</v>
       </c>
       <c r="M135" s="58" t="s">
-        <v>709</v>
+        <v>32</v>
       </c>
       <c r="N135" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
+      </c>
+      <c r="O135" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A136" s="25" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>707</v>
+        <v>146</v>
       </c>
       <c r="C136" s="26" t="s">
-        <v>735</v>
+        <v>661</v>
       </c>
       <c r="D136" s="24" t="s">
         <v>734</v>
@@ -10655,7 +10675,7 @@
       </c>
       <c r="I136" s="26"/>
       <c r="J136" s="26" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="K136" s="14" t="s">
         <v>195</v>
@@ -10664,7 +10684,7 @@
         <v>195</v>
       </c>
       <c r="M136" s="58" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="N136" s="58" t="s">
         <v>1</v>
@@ -10672,13 +10692,13 @@
     </row>
     <row r="137" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A137" s="25" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>694</v>
+        <v>707</v>
       </c>
       <c r="C137" s="26" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="D137" s="24" t="s">
         <v>734</v>
@@ -10695,7 +10715,7 @@
       </c>
       <c r="I137" s="26"/>
       <c r="J137" s="26" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K137" s="14" t="s">
         <v>195</v>
@@ -10704,7 +10724,7 @@
         <v>195</v>
       </c>
       <c r="M137" s="58" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="N137" s="58" t="s">
         <v>1</v>
@@ -10712,13 +10732,13 @@
     </row>
     <row r="138" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>714</v>
+        <v>694</v>
       </c>
       <c r="C138" s="26" t="s">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="D138" s="24" t="s">
         <v>734</v>
@@ -10735,7 +10755,7 @@
       </c>
       <c r="I138" s="26"/>
       <c r="J138" s="26" t="s">
-        <v>695</v>
+        <v>712</v>
       </c>
       <c r="K138" s="14" t="s">
         <v>195</v>
@@ -10744,22 +10764,21 @@
         <v>195</v>
       </c>
       <c r="M138" s="58" t="s">
-        <v>1</v>
+        <v>713</v>
       </c>
       <c r="N138" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O138" s="16"/>
     </row>
     <row r="139" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>696</v>
+        <v>714</v>
       </c>
       <c r="C139" s="26" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D139" s="24" t="s">
         <v>734</v>
@@ -10776,7 +10795,7 @@
       </c>
       <c r="I139" s="26"/>
       <c r="J139" s="26" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="K139" s="14" t="s">
         <v>195</v>
@@ -10785,7 +10804,7 @@
         <v>195</v>
       </c>
       <c r="M139" s="58" t="s">
-        <v>715</v>
+        <v>1</v>
       </c>
       <c r="N139" s="58" t="s">
         <v>1</v>
@@ -10794,13 +10813,13 @@
     </row>
     <row r="140" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C140" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D140" s="24" t="s">
         <v>734</v>
@@ -10817,7 +10836,7 @@
       </c>
       <c r="I140" s="26"/>
       <c r="J140" s="26" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="K140" s="14" t="s">
         <v>195</v>
@@ -10826,7 +10845,7 @@
         <v>195</v>
       </c>
       <c r="M140" s="58" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N140" s="58" t="s">
         <v>1</v>
@@ -10835,13 +10854,13 @@
     </row>
     <row r="141" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D141" s="24" t="s">
         <v>734</v>
@@ -10858,7 +10877,7 @@
       </c>
       <c r="I141" s="26"/>
       <c r="J141" s="26" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="K141" s="14" t="s">
         <v>195</v>
@@ -10867,7 +10886,7 @@
         <v>195</v>
       </c>
       <c r="M141" s="58" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="N141" s="58" t="s">
         <v>1</v>
@@ -10876,13 +10895,13 @@
     </row>
     <row r="142" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B142" s="26" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="C142" s="26" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D142" s="24" t="s">
         <v>734</v>
@@ -10899,7 +10918,7 @@
       </c>
       <c r="I142" s="26"/>
       <c r="J142" s="26" t="s">
-        <v>731</v>
+        <v>701</v>
       </c>
       <c r="K142" s="14" t="s">
         <v>195</v>
@@ -10908,7 +10927,7 @@
         <v>195</v>
       </c>
       <c r="M142" s="58" t="s">
-        <v>706</v>
+        <v>717</v>
       </c>
       <c r="N142" s="58" t="s">
         <v>1</v>
@@ -10917,13 +10936,13 @@
     </row>
     <row r="143" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C143" s="26" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D143" s="24" t="s">
         <v>734</v>
@@ -10932,7 +10951,7 @@
         <v>745</v>
       </c>
       <c r="F143" s="26" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G143" s="26"/>
       <c r="H143" s="26" t="s">
@@ -10940,7 +10959,7 @@
       </c>
       <c r="I143" s="26"/>
       <c r="J143" s="26" t="s">
-        <v>118</v>
+        <v>731</v>
       </c>
       <c r="K143" s="14" t="s">
         <v>195</v>
@@ -10949,24 +10968,22 @@
         <v>195</v>
       </c>
       <c r="M143" s="58" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="N143" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O143" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="O143" s="16"/>
     </row>
     <row r="144" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A144" s="25" t="s">
-        <v>252</v>
+        <v>673</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>143</v>
+        <v>703</v>
       </c>
       <c r="C144" s="26" t="s">
-        <v>597</v>
+        <v>742</v>
       </c>
       <c r="D144" s="24" t="s">
         <v>734</v>
@@ -10983,7 +11000,7 @@
       </c>
       <c r="I144" s="26"/>
       <c r="J144" s="26" t="s">
-        <v>519</v>
+        <v>118</v>
       </c>
       <c r="K144" s="14" t="s">
         <v>195</v>
@@ -10992,24 +11009,24 @@
         <v>195</v>
       </c>
       <c r="M144" s="58" t="s">
-        <v>30</v>
+        <v>704</v>
       </c>
       <c r="N144" s="58" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O144" s="16" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A145" s="25" t="s">
-        <v>219</v>
+        <v>252</v>
       </c>
       <c r="B145" s="26" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C145" s="26" t="s">
-        <v>344</v>
+        <v>597</v>
       </c>
       <c r="D145" s="24" t="s">
         <v>734</v>
@@ -11026,7 +11043,7 @@
       </c>
       <c r="I145" s="26"/>
       <c r="J145" s="26" t="s">
-        <v>581</v>
+        <v>519</v>
       </c>
       <c r="K145" s="14" t="s">
         <v>195</v>
@@ -11035,24 +11052,24 @@
         <v>195</v>
       </c>
       <c r="M145" s="58" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N145" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O145" s="16" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="25" t="s">
-        <v>285</v>
+        <v>219</v>
       </c>
       <c r="B146" s="26" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="C146" s="26" t="s">
-        <v>435</v>
+        <v>344</v>
       </c>
       <c r="D146" s="24" t="s">
         <v>734</v>
@@ -11078,24 +11095,24 @@
         <v>195</v>
       </c>
       <c r="M146" s="58" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="N146" s="58" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O146" s="16" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="25" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="B147" s="26" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C147" s="26" t="s">
-        <v>596</v>
+        <v>435</v>
       </c>
       <c r="D147" s="24" t="s">
         <v>734</v>
@@ -11112,7 +11129,7 @@
       </c>
       <c r="I147" s="26"/>
       <c r="J147" s="26" t="s">
-        <v>520</v>
+        <v>581</v>
       </c>
       <c r="K147" s="14" t="s">
         <v>195</v>
@@ -11121,24 +11138,24 @@
         <v>195</v>
       </c>
       <c r="M147" s="58" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="N147" s="58" t="s">
         <v>472</v>
       </c>
       <c r="O147" s="16" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="148" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A148" s="25" t="s">
-        <v>221</v>
+        <v>264</v>
       </c>
       <c r="B148" s="26" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="C148" s="26" t="s">
-        <v>346</v>
+        <v>596</v>
       </c>
       <c r="D148" s="24" t="s">
         <v>734</v>
@@ -11155,7 +11172,7 @@
       </c>
       <c r="I148" s="26"/>
       <c r="J148" s="26" t="s">
-        <v>581</v>
+        <v>520</v>
       </c>
       <c r="K148" s="14" t="s">
         <v>195</v>
@@ -11164,24 +11181,24 @@
         <v>195</v>
       </c>
       <c r="M148" s="58" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="N148" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O148" s="16" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
     </row>
     <row r="149" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A149" s="25" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="B149" s="26" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="C149" s="26" t="s">
-        <v>595</v>
+        <v>346</v>
       </c>
       <c r="D149" s="24" t="s">
         <v>734</v>
@@ -11198,7 +11215,7 @@
       </c>
       <c r="I149" s="26"/>
       <c r="J149" s="26" t="s">
-        <v>521</v>
+        <v>581</v>
       </c>
       <c r="K149" s="14" t="s">
         <v>195</v>
@@ -11207,24 +11224,24 @@
         <v>195</v>
       </c>
       <c r="M149" s="58" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="N149" s="58" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O149" s="16" t="s">
-        <v>149</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="25" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D150" s="24" t="s">
         <v>734</v>
@@ -11241,7 +11258,7 @@
       </c>
       <c r="I150" s="26"/>
       <c r="J150" s="26" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K150" s="14" t="s">
         <v>195</v>
@@ -11250,24 +11267,24 @@
         <v>195</v>
       </c>
       <c r="M150" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N150" s="58" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O150" s="16" t="s">
-        <v>813</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A151" s="25" t="s">
-        <v>672</v>
+        <v>259</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>702</v>
+        <v>160</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>741</v>
+        <v>594</v>
       </c>
       <c r="D151" s="24" t="s">
         <v>734</v>
@@ -11284,78 +11301,76 @@
       </c>
       <c r="I151" s="26"/>
       <c r="J151" s="26" t="s">
+        <v>522</v>
+      </c>
+      <c r="K151" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L151" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M151" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="N151" s="58" t="s">
+        <v>474</v>
+      </c>
+      <c r="O151" s="16" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A152" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="B152" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="C152" s="26" t="s">
+        <v>741</v>
+      </c>
+      <c r="D152" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="E152" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="F152" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="G152" s="26"/>
+      <c r="H152" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="I152" s="26"/>
+      <c r="J152" s="26" t="s">
         <v>730</v>
       </c>
-      <c r="K151" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L151" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M151" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="N151" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O151" s="16" t="s">
+      <c r="K152" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L152" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M152" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="N152" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="O152" s="16" t="s">
         <v>730</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A152" s="44" t="s">
-        <v>801</v>
-      </c>
-      <c r="B152" s="45" t="s">
-        <v>567</v>
-      </c>
-      <c r="C152" s="45" t="s">
-        <v>801</v>
-      </c>
-      <c r="D152" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="E152" s="45" t="s">
-        <v>659</v>
-      </c>
-      <c r="F152" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="G152" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="H152" s="45" t="s">
-        <v>817</v>
-      </c>
-      <c r="I152" s="45"/>
-      <c r="J152" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="K152" s="14" t="s">
-        <v>638</v>
-      </c>
-      <c r="L152" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="M152" s="58" t="s">
-        <v>655</v>
-      </c>
-      <c r="N152" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O152" s="16" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="153" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A153" s="44" t="s">
-        <v>566</v>
+        <v>801</v>
       </c>
       <c r="B153" s="45" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C153" s="45" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="D153" s="45" t="s">
         <v>662</v>
@@ -11372,9 +11387,7 @@
       <c r="H153" s="45" t="s">
         <v>817</v>
       </c>
-      <c r="I153" s="45">
-        <v>1</v>
-      </c>
+      <c r="I153" s="45"/>
       <c r="J153" s="45" t="s">
         <v>515</v>
       </c>
@@ -11396,13 +11409,13 @@
     </row>
     <row r="154" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B154" s="45" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C154" s="45" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="D154" s="45" t="s">
         <v>662</v>
@@ -11423,33 +11436,33 @@
         <v>1</v>
       </c>
       <c r="J154" s="45" t="s">
-        <v>573</v>
+        <v>515</v>
       </c>
       <c r="K154" s="14" t="s">
-        <v>195</v>
+        <v>638</v>
       </c>
       <c r="L154" s="14" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="M154" s="58" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="N154" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O154" s="16" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="155" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A155" s="44" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B155" s="45" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C155" s="45" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D155" s="45" t="s">
         <v>662</v>
@@ -11470,7 +11483,7 @@
         <v>1</v>
       </c>
       <c r="J155" s="45" t="s">
-        <v>401</v>
+        <v>573</v>
       </c>
       <c r="K155" s="14" t="s">
         <v>195</v>
@@ -11479,24 +11492,24 @@
         <v>195</v>
       </c>
       <c r="M155" s="58" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="N155" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O155" s="16" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
     </row>
     <row r="156" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="44" t="s">
-        <v>650</v>
+        <v>563</v>
       </c>
       <c r="B156" s="45" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C156" s="45" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
       <c r="D156" s="45" t="s">
         <v>662</v>
@@ -11517,33 +11530,33 @@
         <v>1</v>
       </c>
       <c r="J156" s="45" t="s">
-        <v>516</v>
+        <v>401</v>
       </c>
       <c r="K156" s="14" t="s">
-        <v>638</v>
+        <v>195</v>
       </c>
       <c r="L156" s="14" t="s">
-        <v>621</v>
+        <v>195</v>
       </c>
       <c r="M156" s="58" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="N156" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O156" s="16" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="157" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="44" t="s">
-        <v>565</v>
+        <v>650</v>
       </c>
       <c r="B157" s="45" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C157" s="45" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="D157" s="45" t="s">
         <v>662</v>
@@ -11564,33 +11577,33 @@
         <v>1</v>
       </c>
       <c r="J157" s="45" t="s">
-        <v>575</v>
+        <v>516</v>
       </c>
       <c r="K157" s="14" t="s">
-        <v>195</v>
+        <v>638</v>
       </c>
       <c r="L157" s="14" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="M157" s="58" t="s">
-        <v>1</v>
+        <v>652</v>
       </c>
       <c r="N157" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O157" s="16" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="158" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="s">
-        <v>629</v>
+        <v>565</v>
       </c>
       <c r="B158" s="45" t="s">
-        <v>628</v>
+        <v>570</v>
       </c>
       <c r="C158" s="45" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="D158" s="45" t="s">
         <v>662</v>
@@ -11611,7 +11624,7 @@
         <v>1</v>
       </c>
       <c r="J158" s="45" t="s">
-        <v>664</v>
+        <v>575</v>
       </c>
       <c r="K158" s="14" t="s">
         <v>195</v>
@@ -11626,18 +11639,18 @@
         <v>1</v>
       </c>
       <c r="O158" s="16" t="s">
-        <v>1</v>
+        <v>574</v>
       </c>
     </row>
     <row r="159" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="s">
-        <v>651</v>
+        <v>629</v>
       </c>
       <c r="B159" s="45" t="s">
-        <v>567</v>
+        <v>628</v>
       </c>
       <c r="C159" s="45" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="D159" s="45" t="s">
         <v>662</v>
@@ -11655,36 +11668,36 @@
         <v>817</v>
       </c>
       <c r="I159" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J159" s="45" t="s">
-        <v>516</v>
+        <v>664</v>
       </c>
       <c r="K159" s="14" t="s">
-        <v>638</v>
+        <v>195</v>
       </c>
       <c r="L159" s="14" t="s">
-        <v>621</v>
+        <v>195</v>
       </c>
       <c r="M159" s="58" t="s">
-        <v>652</v>
+        <v>1</v>
       </c>
       <c r="N159" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O159" s="16" t="s">
-        <v>578</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="s">
-        <v>798</v>
+        <v>651</v>
       </c>
       <c r="B160" s="45" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C160" s="45" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D160" s="45" t="s">
         <v>662</v>
@@ -11705,31 +11718,33 @@
         <v>3</v>
       </c>
       <c r="J160" s="45" t="s">
-        <v>573</v>
+        <v>516</v>
       </c>
       <c r="K160" s="14" t="s">
-        <v>195</v>
+        <v>638</v>
       </c>
       <c r="L160" s="14" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="M160" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="N160" s="58"/>
+        <v>652</v>
+      </c>
+      <c r="N160" s="58" t="s">
+        <v>1</v>
+      </c>
       <c r="O160" s="16" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="161" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B161" s="45" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C161" s="45" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D161" s="45" t="s">
         <v>662</v>
@@ -11750,7 +11765,7 @@
         <v>3</v>
       </c>
       <c r="J161" s="45" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K161" s="14" t="s">
         <v>195</v>
@@ -11759,22 +11774,22 @@
         <v>195</v>
       </c>
       <c r="M161" s="58" t="s">
-        <v>1</v>
+        <v>654</v>
       </c>
       <c r="N161" s="58"/>
       <c r="O161" s="16" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="162" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B162" s="45" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C162" s="45" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D162" s="45" t="s">
         <v>662</v>
@@ -11795,7 +11810,7 @@
         <v>3</v>
       </c>
       <c r="J162" s="45" t="s">
-        <v>401</v>
+        <v>575</v>
       </c>
       <c r="K162" s="14" t="s">
         <v>195</v>
@@ -11804,22 +11819,67 @@
         <v>195</v>
       </c>
       <c r="M162" s="58" t="s">
-        <v>653</v>
+        <v>1</v>
       </c>
       <c r="N162" s="58"/>
       <c r="O162" s="16" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A163" s="44" t="s">
+        <v>800</v>
+      </c>
+      <c r="B163" s="45" t="s">
+        <v>568</v>
+      </c>
+      <c r="C163" s="45" t="s">
+        <v>805</v>
+      </c>
+      <c r="D163" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="E163" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="F163" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="G163" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="H163" s="45" t="s">
+        <v>817</v>
+      </c>
+      <c r="I163" s="45">
+        <v>3</v>
+      </c>
+      <c r="J163" s="45" t="s">
+        <v>401</v>
+      </c>
+      <c r="K163" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L163" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M163" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="N163" s="58"/>
+      <c r="O163" s="16" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A163" s="1"/>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A164" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O162">
-    <sortCondition ref="D2:D162"/>
-    <sortCondition ref="E2:E162"/>
-    <sortCondition ref="F2:F162"/>
-    <sortCondition ref="G2:G162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O163">
+    <sortCondition ref="D2:D163"/>
+    <sortCondition ref="E2:E163"/>
+    <sortCondition ref="F2:F163"/>
+    <sortCondition ref="G2:G163"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B60" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Refactoring - separate build and analysis logic
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC5E011-8256-8949-9A47-FA8E06BC5299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5505F332-3964-7949-8674-8B93C9CF48E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="1540" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17640" yWindow="520" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="843">
   <si>
     <t>AY632538</t>
   </si>
@@ -2510,6 +2510,63 @@
   </si>
   <si>
     <t>ZT17-1078</t>
+  </si>
+  <si>
+    <t>MT075326</t>
+  </si>
+  <si>
+    <t>Salmon flavivirus</t>
+  </si>
+  <si>
+    <t>SFV</t>
+  </si>
+  <si>
+    <t>Oncorhynchus tshawytscha</t>
+  </si>
+  <si>
+    <t>DnFV</t>
+  </si>
+  <si>
+    <t>Dianemobius nigrofasciatus flavivirus</t>
+  </si>
+  <si>
+    <t>Dianemobius nigrofasciatus</t>
+  </si>
+  <si>
+    <t>MW208755</t>
+  </si>
+  <si>
+    <t>Coleopteran flavi-related virus</t>
+  </si>
+  <si>
+    <t>ColFlaV</t>
+  </si>
+  <si>
+    <t>MW208759</t>
+  </si>
+  <si>
+    <t>Embiopteran flavi-related virus</t>
+  </si>
+  <si>
+    <t>EmbFlaV</t>
+  </si>
+  <si>
+    <t>Plectopteran flavi-related virus</t>
+  </si>
+  <si>
+    <t>MW208760</t>
+  </si>
+  <si>
+    <t>PleFlaV</t>
+  </si>
+  <si>
+    <t>Perla marginata</t>
+  </si>
+  <si>
+    <t>Antipaluria urichi</t>
+  </si>
+  <si>
+    <t>Pempsamacra sp.</t>
   </si>
 </sst>
 </file>
@@ -4656,11 +4713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O165"/>
+  <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I131" sqref="I131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10307,31 +10364,51 @@
       </c>
     </row>
     <row r="128" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A128" s="59"/>
-      <c r="B128" s="43"/>
-      <c r="C128" s="43"/>
-      <c r="D128" s="43"/>
-      <c r="E128" s="43"/>
-      <c r="F128" s="43"/>
+      <c r="A128" s="59" t="s">
+        <v>824</v>
+      </c>
+      <c r="B128" s="43" t="s">
+        <v>825</v>
+      </c>
+      <c r="C128" s="43" t="s">
+        <v>826</v>
+      </c>
+      <c r="D128" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E128" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F128" s="43" t="s">
+        <v>609</v>
+      </c>
       <c r="G128" s="43"/>
-      <c r="H128" s="43"/>
+      <c r="H128" s="43" t="s">
+        <v>817</v>
+      </c>
       <c r="I128" s="43"/>
       <c r="J128" s="43"/>
-      <c r="K128" s="14"/>
-      <c r="L128" s="14"/>
+      <c r="K128" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L128" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="M128" s="15"/>
       <c r="N128" s="13"/>
-      <c r="O128" s="16"/>
+      <c r="O128" s="16" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="129" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A129" s="59" t="s">
-        <v>491</v>
+        <v>828</v>
       </c>
       <c r="B129" s="43" t="s">
-        <v>494</v>
+        <v>829</v>
       </c>
       <c r="C129" s="43" t="s">
-        <v>791</v>
+        <v>828</v>
       </c>
       <c r="D129" s="43" t="s">
         <v>734</v>
@@ -10347,34 +10424,28 @@
         <v>817</v>
       </c>
       <c r="I129" s="43"/>
-      <c r="J129" s="43" t="s">
-        <v>512</v>
-      </c>
+      <c r="J129" s="43"/>
       <c r="K129" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L129" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M129" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N129" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="M129" s="15"/>
+      <c r="N129" s="13"/>
       <c r="O129" s="16" t="s">
-        <v>497</v>
+        <v>830</v>
       </c>
     </row>
     <row r="130" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A130" s="59" t="s">
-        <v>492</v>
+        <v>831</v>
       </c>
       <c r="B130" s="43" t="s">
-        <v>495</v>
+        <v>832</v>
       </c>
       <c r="C130" s="43" t="s">
-        <v>790</v>
+        <v>833</v>
       </c>
       <c r="D130" s="43" t="s">
         <v>734</v>
@@ -10390,180 +10461,162 @@
         <v>817</v>
       </c>
       <c r="I130" s="43"/>
-      <c r="J130" s="43" t="s">
-        <v>513</v>
-      </c>
+      <c r="J130" s="43"/>
       <c r="K130" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L130" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M130" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N130" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="M130" s="15"/>
+      <c r="N130" s="13"/>
       <c r="O130" s="16" t="s">
-        <v>496</v>
+        <v>842</v>
       </c>
     </row>
     <row r="131" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A131" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B131" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="C131" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="D131" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="E131" s="24" t="s">
-        <v>745</v>
-      </c>
-      <c r="F131" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="G131" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="H131" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="I131" s="24"/>
-      <c r="J131" s="24" t="s">
-        <v>613</v>
-      </c>
+      <c r="A131" s="59" t="s">
+        <v>838</v>
+      </c>
+      <c r="B131" s="43" t="s">
+        <v>837</v>
+      </c>
+      <c r="C131" s="43" t="s">
+        <v>839</v>
+      </c>
+      <c r="D131" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E131" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F131" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="G131" s="43"/>
+      <c r="H131" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I131" s="43"/>
+      <c r="J131" s="43"/>
       <c r="K131" s="14" t="s">
         <v>195</v>
       </c>
       <c r="L131" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M131" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="M131" s="15"/>
       <c r="N131" s="13"/>
       <c r="O131" s="16" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A132" s="59" t="s">
+        <v>834</v>
+      </c>
+      <c r="B132" s="43" t="s">
+        <v>835</v>
+      </c>
+      <c r="C132" s="43" t="s">
+        <v>836</v>
+      </c>
+      <c r="D132" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E132" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F132" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="G132" s="43"/>
+      <c r="H132" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I132" s="43"/>
+      <c r="J132" s="43"/>
+      <c r="K132" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L132" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M132" s="15"/>
+      <c r="N132" s="13"/>
+      <c r="O132" s="16" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A133" s="59" t="s">
+        <v>491</v>
+      </c>
+      <c r="B133" s="43" t="s">
+        <v>494</v>
+      </c>
+      <c r="C133" s="43" t="s">
+        <v>791</v>
+      </c>
+      <c r="D133" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E133" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F133" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="G133" s="43"/>
+      <c r="H133" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I133" s="43"/>
+      <c r="J133" s="43" t="s">
+        <v>512</v>
+      </c>
+      <c r="K133" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L133" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M133" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B132" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="C132" s="24" t="s">
-        <v>585</v>
-      </c>
-      <c r="D132" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="E132" s="24" t="s">
-        <v>745</v>
-      </c>
-      <c r="F132" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="G132" s="24"/>
-      <c r="H132" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="I132" s="24"/>
-      <c r="J132" s="24" t="s">
-        <v>518</v>
-      </c>
-      <c r="K132" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L132" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M132" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="N132" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="O132" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="133" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A133" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="B133" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="C133" s="24" t="s">
-        <v>586</v>
-      </c>
-      <c r="D133" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="E133" s="24" t="s">
-        <v>745</v>
-      </c>
-      <c r="F133" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="G133" s="24"/>
-      <c r="H133" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="I133" s="24"/>
-      <c r="J133" s="24" t="s">
-        <v>519</v>
-      </c>
-      <c r="K133" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L133" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M133" s="58" t="s">
+      <c r="N133" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N133" s="58" t="s">
-        <v>471</v>
-      </c>
       <c r="O133" s="16" t="s">
-        <v>162</v>
+        <v>497</v>
       </c>
     </row>
     <row r="134" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A134" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="B134" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="C134" s="24" t="s">
-        <v>587</v>
-      </c>
-      <c r="D134" s="24" t="s">
-        <v>734</v>
-      </c>
-      <c r="E134" s="24" t="s">
-        <v>745</v>
-      </c>
-      <c r="F134" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="G134" s="24"/>
-      <c r="H134" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="I134" s="24"/>
-      <c r="J134" s="24" t="s">
-        <v>520</v>
+      <c r="A134" s="59" t="s">
+        <v>492</v>
+      </c>
+      <c r="B134" s="43" t="s">
+        <v>495</v>
+      </c>
+      <c r="C134" s="43" t="s">
+        <v>790</v>
+      </c>
+      <c r="D134" s="43" t="s">
+        <v>734</v>
+      </c>
+      <c r="E134" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F134" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="G134" s="43"/>
+      <c r="H134" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I134" s="43"/>
+      <c r="J134" s="43" t="s">
+        <v>513</v>
       </c>
       <c r="K134" s="14" t="s">
         <v>195</v>
@@ -10571,25 +10624,25 @@
       <c r="L134" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M134" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="N134" s="58" t="s">
-        <v>472</v>
+      <c r="M134" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N134" s="13" t="s">
+        <v>1</v>
       </c>
       <c r="O134" s="16" t="s">
-        <v>164</v>
+        <v>496</v>
       </c>
     </row>
     <row r="135" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A135" s="25" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>588</v>
+        <v>205</v>
       </c>
       <c r="D135" s="24" t="s">
         <v>734</v>
@@ -10600,13 +10653,15 @@
       <c r="F135" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G135" s="24"/>
+      <c r="G135" s="24" t="s">
+        <v>206</v>
+      </c>
       <c r="H135" s="24" t="s">
         <v>817</v>
       </c>
       <c r="I135" s="24"/>
       <c r="J135" s="24" t="s">
-        <v>520</v>
+        <v>613</v>
       </c>
       <c r="K135" s="14" t="s">
         <v>195</v>
@@ -10614,25 +10669,23 @@
       <c r="L135" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M135" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="N135" s="58" t="s">
-        <v>472</v>
-      </c>
+      <c r="M135" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N135" s="13"/>
       <c r="O135" s="16" t="s">
-        <v>164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A136" s="25" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>32</v>
+        <v>585</v>
       </c>
       <c r="D136" s="24" t="s">
         <v>734</v>
@@ -10649,7 +10702,7 @@
       </c>
       <c r="I136" s="24"/>
       <c r="J136" s="24" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="K136" s="14" t="s">
         <v>195</v>
@@ -10657,25 +10710,25 @@
       <c r="L136" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="M136" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="N136" s="58" t="s">
-        <v>472</v>
+      <c r="M136" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N136" s="13" t="s">
+        <v>474</v>
       </c>
       <c r="O136" s="16" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A137" s="25" t="s">
-        <v>665</v>
+        <v>260</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C137" s="26" t="s">
-        <v>661</v>
+        <v>604</v>
+      </c>
+      <c r="C137" s="24" t="s">
+        <v>586</v>
       </c>
       <c r="D137" s="24" t="s">
         <v>734</v>
@@ -10683,16 +10736,16 @@
       <c r="E137" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="F137" s="26" t="s">
+      <c r="F137" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G137" s="26"/>
-      <c r="H137" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="I137" s="26"/>
-      <c r="J137" s="26" t="s">
-        <v>710</v>
+      <c r="G137" s="24"/>
+      <c r="H137" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="I137" s="24"/>
+      <c r="J137" s="24" t="s">
+        <v>519</v>
       </c>
       <c r="K137" s="14" t="s">
         <v>195</v>
@@ -10701,21 +10754,24 @@
         <v>195</v>
       </c>
       <c r="M137" s="58" t="s">
-        <v>709</v>
+        <v>1</v>
       </c>
       <c r="N137" s="58" t="s">
-        <v>1</v>
+        <v>471</v>
+      </c>
+      <c r="O137" s="16" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>666</v>
+        <v>261</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>707</v>
-      </c>
-      <c r="C138" s="26" t="s">
-        <v>735</v>
+        <v>163</v>
+      </c>
+      <c r="C138" s="24" t="s">
+        <v>587</v>
       </c>
       <c r="D138" s="24" t="s">
         <v>734</v>
@@ -10723,16 +10779,16 @@
       <c r="E138" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="F138" s="26" t="s">
+      <c r="F138" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G138" s="26"/>
-      <c r="H138" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="I138" s="26"/>
-      <c r="J138" s="26" t="s">
-        <v>711</v>
+      <c r="G138" s="24"/>
+      <c r="H138" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="I138" s="24"/>
+      <c r="J138" s="24" t="s">
+        <v>520</v>
       </c>
       <c r="K138" s="14" t="s">
         <v>195</v>
@@ -10741,21 +10797,24 @@
         <v>195</v>
       </c>
       <c r="M138" s="58" t="s">
-        <v>708</v>
+        <v>43</v>
       </c>
       <c r="N138" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
+      </c>
+      <c r="O138" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>667</v>
+        <v>262</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>694</v>
-      </c>
-      <c r="C139" s="26" t="s">
-        <v>743</v>
+        <v>165</v>
+      </c>
+      <c r="C139" s="24" t="s">
+        <v>588</v>
       </c>
       <c r="D139" s="24" t="s">
         <v>734</v>
@@ -10763,16 +10822,16 @@
       <c r="E139" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="F139" s="26" t="s">
+      <c r="F139" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G139" s="26"/>
-      <c r="H139" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="I139" s="26"/>
-      <c r="J139" s="26" t="s">
-        <v>712</v>
+      <c r="G139" s="24"/>
+      <c r="H139" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="I139" s="24"/>
+      <c r="J139" s="24" t="s">
+        <v>520</v>
       </c>
       <c r="K139" s="14" t="s">
         <v>195</v>
@@ -10781,21 +10840,24 @@
         <v>195</v>
       </c>
       <c r="M139" s="58" t="s">
-        <v>713</v>
+        <v>44</v>
       </c>
       <c r="N139" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
+      </c>
+      <c r="O139" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>668</v>
+        <v>254</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>714</v>
-      </c>
-      <c r="C140" s="26" t="s">
-        <v>736</v>
+        <v>146</v>
+      </c>
+      <c r="C140" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D140" s="24" t="s">
         <v>734</v>
@@ -10803,16 +10865,16 @@
       <c r="E140" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="F140" s="26" t="s">
+      <c r="F140" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="G140" s="26"/>
-      <c r="H140" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="I140" s="26"/>
-      <c r="J140" s="26" t="s">
-        <v>695</v>
+      <c r="G140" s="24"/>
+      <c r="H140" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="I140" s="24"/>
+      <c r="J140" s="24" t="s">
+        <v>508</v>
       </c>
       <c r="K140" s="14" t="s">
         <v>195</v>
@@ -10821,22 +10883,24 @@
         <v>195</v>
       </c>
       <c r="M140" s="58" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="N140" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O140" s="16"/>
+        <v>472</v>
+      </c>
+      <c r="O140" s="16" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="141" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>696</v>
+        <v>146</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>737</v>
+        <v>661</v>
       </c>
       <c r="D141" s="24" t="s">
         <v>734</v>
@@ -10853,7 +10917,7 @@
       </c>
       <c r="I141" s="26"/>
       <c r="J141" s="26" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
       <c r="K141" s="14" t="s">
         <v>195</v>
@@ -10862,22 +10926,21 @@
         <v>195</v>
       </c>
       <c r="M141" s="58" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="N141" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O141" s="16"/>
     </row>
     <row r="142" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B142" s="26" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="C142" s="26" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D142" s="24" t="s">
         <v>734</v>
@@ -10894,7 +10957,7 @@
       </c>
       <c r="I142" s="26"/>
       <c r="J142" s="26" t="s">
-        <v>699</v>
+        <v>711</v>
       </c>
       <c r="K142" s="14" t="s">
         <v>195</v>
@@ -10903,22 +10966,21 @@
         <v>195</v>
       </c>
       <c r="M142" s="58" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="N142" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O142" s="16"/>
     </row>
     <row r="143" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="C143" s="26" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="D143" s="24" t="s">
         <v>734</v>
@@ -10935,7 +10997,7 @@
       </c>
       <c r="I143" s="26"/>
       <c r="J143" s="26" t="s">
-        <v>701</v>
+        <v>712</v>
       </c>
       <c r="K143" s="14" t="s">
         <v>195</v>
@@ -10944,22 +11006,21 @@
         <v>195</v>
       </c>
       <c r="M143" s="58" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="N143" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O143" s="16"/>
     </row>
     <row r="144" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A144" s="25" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="C144" s="26" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D144" s="24" t="s">
         <v>734</v>
@@ -10976,7 +11037,7 @@
       </c>
       <c r="I144" s="26"/>
       <c r="J144" s="26" t="s">
-        <v>731</v>
+        <v>695</v>
       </c>
       <c r="K144" s="14" t="s">
         <v>195</v>
@@ -10985,7 +11046,7 @@
         <v>195</v>
       </c>
       <c r="M144" s="58" t="s">
-        <v>706</v>
+        <v>1</v>
       </c>
       <c r="N144" s="58" t="s">
         <v>1</v>
@@ -10994,13 +11055,13 @@
     </row>
     <row r="145" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A145" s="25" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B145" s="26" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="C145" s="26" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="D145" s="24" t="s">
         <v>734</v>
@@ -11009,7 +11070,7 @@
         <v>745</v>
       </c>
       <c r="F145" s="26" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G145" s="26"/>
       <c r="H145" s="26" t="s">
@@ -11017,7 +11078,7 @@
       </c>
       <c r="I145" s="26"/>
       <c r="J145" s="26" t="s">
-        <v>118</v>
+        <v>697</v>
       </c>
       <c r="K145" s="14" t="s">
         <v>195</v>
@@ -11026,24 +11087,22 @@
         <v>195</v>
       </c>
       <c r="M145" s="58" t="s">
-        <v>704</v>
+        <v>715</v>
       </c>
       <c r="N145" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O145" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="O145" s="16"/>
     </row>
     <row r="146" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="25" t="s">
-        <v>252</v>
+        <v>670</v>
       </c>
       <c r="B146" s="26" t="s">
-        <v>143</v>
+        <v>698</v>
       </c>
       <c r="C146" s="26" t="s">
-        <v>597</v>
+        <v>738</v>
       </c>
       <c r="D146" s="24" t="s">
         <v>734</v>
@@ -11052,7 +11111,7 @@
         <v>745</v>
       </c>
       <c r="F146" s="26" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G146" s="26"/>
       <c r="H146" s="26" t="s">
@@ -11060,7 +11119,7 @@
       </c>
       <c r="I146" s="26"/>
       <c r="J146" s="26" t="s">
-        <v>519</v>
+        <v>699</v>
       </c>
       <c r="K146" s="14" t="s">
         <v>195</v>
@@ -11069,24 +11128,22 @@
         <v>195</v>
       </c>
       <c r="M146" s="58" t="s">
-        <v>30</v>
+        <v>716</v>
       </c>
       <c r="N146" s="58" t="s">
-        <v>472</v>
-      </c>
-      <c r="O146" s="16" t="s">
-        <v>162</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O146" s="16"/>
     </row>
     <row r="147" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="25" t="s">
-        <v>219</v>
+        <v>671</v>
       </c>
       <c r="B147" s="26" t="s">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="C147" s="26" t="s">
-        <v>344</v>
+        <v>739</v>
       </c>
       <c r="D147" s="24" t="s">
         <v>734</v>
@@ -11095,7 +11152,7 @@
         <v>745</v>
       </c>
       <c r="F147" s="26" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G147" s="26"/>
       <c r="H147" s="26" t="s">
@@ -11103,7 +11160,7 @@
       </c>
       <c r="I147" s="26"/>
       <c r="J147" s="26" t="s">
-        <v>581</v>
+        <v>701</v>
       </c>
       <c r="K147" s="14" t="s">
         <v>195</v>
@@ -11112,24 +11169,22 @@
         <v>195</v>
       </c>
       <c r="M147" s="58" t="s">
-        <v>1</v>
+        <v>717</v>
       </c>
       <c r="N147" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="O147" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="O147" s="16"/>
     </row>
     <row r="148" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A148" s="25" t="s">
-        <v>285</v>
+        <v>674</v>
       </c>
       <c r="B148" s="26" t="s">
-        <v>178</v>
+        <v>705</v>
       </c>
       <c r="C148" s="26" t="s">
-        <v>435</v>
+        <v>740</v>
       </c>
       <c r="D148" s="24" t="s">
         <v>734</v>
@@ -11138,7 +11193,7 @@
         <v>745</v>
       </c>
       <c r="F148" s="26" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G148" s="26"/>
       <c r="H148" s="26" t="s">
@@ -11146,7 +11201,7 @@
       </c>
       <c r="I148" s="26"/>
       <c r="J148" s="26" t="s">
-        <v>581</v>
+        <v>731</v>
       </c>
       <c r="K148" s="14" t="s">
         <v>195</v>
@@ -11155,24 +11210,22 @@
         <v>195</v>
       </c>
       <c r="M148" s="58" t="s">
-        <v>51</v>
+        <v>706</v>
       </c>
       <c r="N148" s="58" t="s">
-        <v>472</v>
-      </c>
-      <c r="O148" s="16" t="s">
-        <v>118</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O148" s="16"/>
     </row>
     <row r="149" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A149" s="25" t="s">
-        <v>264</v>
+        <v>673</v>
       </c>
       <c r="B149" s="26" t="s">
-        <v>167</v>
+        <v>703</v>
       </c>
       <c r="C149" s="26" t="s">
-        <v>596</v>
+        <v>742</v>
       </c>
       <c r="D149" s="24" t="s">
         <v>734</v>
@@ -11189,7 +11242,7 @@
       </c>
       <c r="I149" s="26"/>
       <c r="J149" s="26" t="s">
-        <v>520</v>
+        <v>118</v>
       </c>
       <c r="K149" s="14" t="s">
         <v>195</v>
@@ -11198,24 +11251,24 @@
         <v>195</v>
       </c>
       <c r="M149" s="58" t="s">
-        <v>46</v>
+        <v>704</v>
       </c>
       <c r="N149" s="58" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O149" s="16" t="s">
-        <v>164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="25" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>346</v>
+        <v>597</v>
       </c>
       <c r="D150" s="24" t="s">
         <v>734</v>
@@ -11232,7 +11285,7 @@
       </c>
       <c r="I150" s="26"/>
       <c r="J150" s="26" t="s">
-        <v>581</v>
+        <v>519</v>
       </c>
       <c r="K150" s="14" t="s">
         <v>195</v>
@@ -11241,24 +11294,24 @@
         <v>195</v>
       </c>
       <c r="M150" s="58" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N150" s="58" t="s">
-        <v>1</v>
+        <v>472</v>
       </c>
       <c r="O150" s="16" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
     </row>
     <row r="151" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A151" s="25" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>595</v>
+        <v>344</v>
       </c>
       <c r="D151" s="24" t="s">
         <v>734</v>
@@ -11275,7 +11328,7 @@
       </c>
       <c r="I151" s="26"/>
       <c r="J151" s="26" t="s">
-        <v>521</v>
+        <v>581</v>
       </c>
       <c r="K151" s="14" t="s">
         <v>195</v>
@@ -11284,24 +11337,24 @@
         <v>195</v>
       </c>
       <c r="M151" s="58" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="N151" s="58" t="s">
-        <v>472</v>
+        <v>1</v>
       </c>
       <c r="O151" s="16" t="s">
-        <v>149</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A152" s="25" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="B152" s="26" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>594</v>
+        <v>435</v>
       </c>
       <c r="D152" s="24" t="s">
         <v>734</v>
@@ -11318,7 +11371,7 @@
       </c>
       <c r="I152" s="26"/>
       <c r="J152" s="26" t="s">
-        <v>522</v>
+        <v>581</v>
       </c>
       <c r="K152" s="14" t="s">
         <v>195</v>
@@ -11327,24 +11380,24 @@
         <v>195</v>
       </c>
       <c r="M152" s="58" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="N152" s="58" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O152" s="16" t="s">
-        <v>813</v>
+        <v>118</v>
       </c>
     </row>
     <row r="153" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A153" s="25" t="s">
-        <v>672</v>
+        <v>264</v>
       </c>
       <c r="B153" s="26" t="s">
-        <v>702</v>
+        <v>167</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>741</v>
+        <v>596</v>
       </c>
       <c r="D153" s="24" t="s">
         <v>734</v>
@@ -11361,7 +11414,7 @@
       </c>
       <c r="I153" s="26"/>
       <c r="J153" s="26" t="s">
-        <v>730</v>
+        <v>520</v>
       </c>
       <c r="K153" s="14" t="s">
         <v>195</v>
@@ -11370,210 +11423,196 @@
         <v>195</v>
       </c>
       <c r="M153" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="N153" s="58" t="s">
+        <v>472</v>
+      </c>
+      <c r="O153" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A154" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="B154" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C154" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="D154" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="E154" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="F154" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="G154" s="26"/>
+      <c r="H154" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="I154" s="26"/>
+      <c r="J154" s="26" t="s">
+        <v>581</v>
+      </c>
+      <c r="K154" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L154" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M154" s="58" t="s">
         <v>1</v>
-      </c>
-      <c r="N153" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O153" s="16" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="154" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A154" s="44" t="s">
-        <v>801</v>
-      </c>
-      <c r="B154" s="45" t="s">
-        <v>567</v>
-      </c>
-      <c r="C154" s="45" t="s">
-        <v>801</v>
-      </c>
-      <c r="D154" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="E154" s="45" t="s">
-        <v>659</v>
-      </c>
-      <c r="F154" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="G154" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="H154" s="45" t="s">
-        <v>817</v>
-      </c>
-      <c r="I154" s="45"/>
-      <c r="J154" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="K154" s="14" t="s">
-        <v>638</v>
-      </c>
-      <c r="L154" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="M154" s="58" t="s">
-        <v>655</v>
       </c>
       <c r="N154" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O154" s="16" t="s">
-        <v>578</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A155" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="B155" s="45" t="s">
-        <v>571</v>
-      </c>
-      <c r="C155" s="45" t="s">
-        <v>811</v>
-      </c>
-      <c r="D155" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="E155" s="45" t="s">
-        <v>659</v>
-      </c>
-      <c r="F155" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="G155" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="H155" s="45" t="s">
-        <v>817</v>
-      </c>
-      <c r="I155" s="45">
+      <c r="A155" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="B155" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C155" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="D155" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="F155" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="G155" s="26"/>
+      <c r="H155" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="I155" s="26"/>
+      <c r="J155" s="26" t="s">
+        <v>521</v>
+      </c>
+      <c r="K155" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L155" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M155" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="N155" s="58" t="s">
+        <v>472</v>
+      </c>
+      <c r="O155" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A156" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="B156" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C156" s="26" t="s">
+        <v>594</v>
+      </c>
+      <c r="D156" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="E156" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="F156" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="G156" s="26"/>
+      <c r="H156" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="I156" s="26"/>
+      <c r="J156" s="26" t="s">
+        <v>522</v>
+      </c>
+      <c r="K156" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L156" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M156" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="N156" s="58" t="s">
+        <v>474</v>
+      </c>
+      <c r="O156" s="16" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A157" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="B157" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="C157" s="26" t="s">
+        <v>741</v>
+      </c>
+      <c r="D157" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="E157" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="F157" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="G157" s="26"/>
+      <c r="H157" s="26" t="s">
+        <v>817</v>
+      </c>
+      <c r="I157" s="26"/>
+      <c r="J157" s="26" t="s">
+        <v>730</v>
+      </c>
+      <c r="K157" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L157" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M157" s="58" t="s">
         <v>1</v>
-      </c>
-      <c r="J155" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="K155" s="14" t="s">
-        <v>638</v>
-      </c>
-      <c r="L155" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="M155" s="58" t="s">
-        <v>655</v>
-      </c>
-      <c r="N155" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O155" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A156" s="44" t="s">
-        <v>564</v>
-      </c>
-      <c r="B156" s="45" t="s">
-        <v>569</v>
-      </c>
-      <c r="C156" s="45" t="s">
-        <v>810</v>
-      </c>
-      <c r="D156" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="E156" s="45" t="s">
-        <v>659</v>
-      </c>
-      <c r="F156" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="G156" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="H156" s="45" t="s">
-        <v>817</v>
-      </c>
-      <c r="I156" s="45">
-        <v>1</v>
-      </c>
-      <c r="J156" s="45" t="s">
-        <v>573</v>
-      </c>
-      <c r="K156" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L156" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M156" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="N156" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="O156" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="157" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A157" s="44" t="s">
-        <v>563</v>
-      </c>
-      <c r="B157" s="45" t="s">
-        <v>568</v>
-      </c>
-      <c r="C157" s="45" t="s">
-        <v>812</v>
-      </c>
-      <c r="D157" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="E157" s="45" t="s">
-        <v>659</v>
-      </c>
-      <c r="F157" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="G157" s="45" t="s">
-        <v>662</v>
-      </c>
-      <c r="H157" s="45" t="s">
-        <v>817</v>
-      </c>
-      <c r="I157" s="45">
-        <v>1</v>
-      </c>
-      <c r="J157" s="45" t="s">
-        <v>401</v>
-      </c>
-      <c r="K157" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L157" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M157" s="58" t="s">
-        <v>653</v>
       </c>
       <c r="N157" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O157" s="16" t="s">
-        <v>572</v>
+        <v>730</v>
       </c>
     </row>
     <row r="158" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="s">
-        <v>650</v>
+        <v>801</v>
       </c>
       <c r="B158" s="45" t="s">
         <v>567</v>
       </c>
       <c r="C158" s="45" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D158" s="45" t="s">
         <v>662</v>
@@ -11590,11 +11629,9 @@
       <c r="H158" s="45" t="s">
         <v>817</v>
       </c>
-      <c r="I158" s="45">
-        <v>1</v>
-      </c>
+      <c r="I158" s="45"/>
       <c r="J158" s="45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K158" s="14" t="s">
         <v>638</v>
@@ -11603,24 +11640,24 @@
         <v>621</v>
       </c>
       <c r="M158" s="58" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="N158" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O158" s="16" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="159" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B159" s="45" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C159" s="45" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="D159" s="45" t="s">
         <v>662</v>
@@ -11641,33 +11678,33 @@
         <v>1</v>
       </c>
       <c r="J159" s="45" t="s">
-        <v>575</v>
+        <v>515</v>
       </c>
       <c r="K159" s="14" t="s">
-        <v>195</v>
+        <v>638</v>
       </c>
       <c r="L159" s="14" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="M159" s="58" t="s">
-        <v>1</v>
+        <v>655</v>
       </c>
       <c r="N159" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O159" s="16" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="160" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="s">
-        <v>629</v>
+        <v>564</v>
       </c>
       <c r="B160" s="45" t="s">
-        <v>628</v>
+        <v>569</v>
       </c>
       <c r="C160" s="45" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="D160" s="45" t="s">
         <v>662</v>
@@ -11688,7 +11725,7 @@
         <v>1</v>
       </c>
       <c r="J160" s="45" t="s">
-        <v>664</v>
+        <v>573</v>
       </c>
       <c r="K160" s="14" t="s">
         <v>195</v>
@@ -11697,24 +11734,24 @@
         <v>195</v>
       </c>
       <c r="M160" s="58" t="s">
-        <v>1</v>
+        <v>654</v>
       </c>
       <c r="N160" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O160" s="16" t="s">
-        <v>1</v>
+        <v>577</v>
       </c>
     </row>
     <row r="161" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="s">
-        <v>651</v>
+        <v>563</v>
       </c>
       <c r="B161" s="45" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C161" s="45" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="D161" s="45" t="s">
         <v>662</v>
@@ -11732,36 +11769,36 @@
         <v>817</v>
       </c>
       <c r="I161" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J161" s="45" t="s">
-        <v>516</v>
+        <v>401</v>
       </c>
       <c r="K161" s="14" t="s">
-        <v>638</v>
+        <v>195</v>
       </c>
       <c r="L161" s="14" t="s">
-        <v>621</v>
+        <v>195</v>
       </c>
       <c r="M161" s="58" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="N161" s="58" t="s">
         <v>1</v>
       </c>
       <c r="O161" s="16" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="162" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="s">
-        <v>798</v>
+        <v>650</v>
       </c>
       <c r="B162" s="45" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C162" s="45" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D162" s="45" t="s">
         <v>662</v>
@@ -11779,34 +11816,36 @@
         <v>817</v>
       </c>
       <c r="I162" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J162" s="45" t="s">
-        <v>573</v>
+        <v>516</v>
       </c>
       <c r="K162" s="14" t="s">
-        <v>195</v>
+        <v>638</v>
       </c>
       <c r="L162" s="14" t="s">
-        <v>195</v>
+        <v>621</v>
       </c>
       <c r="M162" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="N162" s="58"/>
+        <v>652</v>
+      </c>
+      <c r="N162" s="58" t="s">
+        <v>1</v>
+      </c>
       <c r="O162" s="16" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="163" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="s">
-        <v>799</v>
+        <v>565</v>
       </c>
       <c r="B163" s="45" t="s">
         <v>570</v>
       </c>
       <c r="C163" s="45" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="D163" s="45" t="s">
         <v>662</v>
@@ -11824,7 +11863,7 @@
         <v>817</v>
       </c>
       <c r="I163" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J163" s="45" t="s">
         <v>575</v>
@@ -11838,20 +11877,22 @@
       <c r="M163" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="N163" s="58"/>
+      <c r="N163" s="58" t="s">
+        <v>1</v>
+      </c>
       <c r="O163" s="16" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="164" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="s">
-        <v>800</v>
+        <v>629</v>
       </c>
       <c r="B164" s="45" t="s">
-        <v>568</v>
+        <v>628</v>
       </c>
       <c r="C164" s="45" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D164" s="45" t="s">
         <v>662</v>
@@ -11869,34 +11910,218 @@
         <v>817</v>
       </c>
       <c r="I164" s="45">
+        <v>1</v>
+      </c>
+      <c r="J164" s="45" t="s">
+        <v>664</v>
+      </c>
+      <c r="K164" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L164" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M164" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="N164" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="O164" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A165" s="44" t="s">
+        <v>651</v>
+      </c>
+      <c r="B165" s="45" t="s">
+        <v>567</v>
+      </c>
+      <c r="C165" s="45" t="s">
+        <v>803</v>
+      </c>
+      <c r="D165" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="E165" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="F165" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="G165" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="H165" s="45" t="s">
+        <v>817</v>
+      </c>
+      <c r="I165" s="45">
         <v>3</v>
       </c>
-      <c r="J164" s="45" t="s">
+      <c r="J165" s="45" t="s">
+        <v>516</v>
+      </c>
+      <c r="K165" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="L165" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="M165" s="58" t="s">
+        <v>652</v>
+      </c>
+      <c r="N165" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="O165" s="16" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A166" s="44" t="s">
+        <v>798</v>
+      </c>
+      <c r="B166" s="45" t="s">
+        <v>569</v>
+      </c>
+      <c r="C166" s="45" t="s">
+        <v>804</v>
+      </c>
+      <c r="D166" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="E166" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="F166" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="G166" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="H166" s="45" t="s">
+        <v>817</v>
+      </c>
+      <c r="I166" s="45">
+        <v>3</v>
+      </c>
+      <c r="J166" s="45" t="s">
+        <v>573</v>
+      </c>
+      <c r="K166" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L166" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M166" s="58" t="s">
+        <v>654</v>
+      </c>
+      <c r="N166" s="58"/>
+      <c r="O166" s="16" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A167" s="44" t="s">
+        <v>799</v>
+      </c>
+      <c r="B167" s="45" t="s">
+        <v>570</v>
+      </c>
+      <c r="C167" s="45" t="s">
+        <v>806</v>
+      </c>
+      <c r="D167" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="E167" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="F167" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="G167" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="H167" s="45" t="s">
+        <v>817</v>
+      </c>
+      <c r="I167" s="45">
+        <v>3</v>
+      </c>
+      <c r="J167" s="45" t="s">
+        <v>575</v>
+      </c>
+      <c r="K167" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L167" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M167" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="N167" s="58"/>
+      <c r="O167" s="16" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A168" s="44" t="s">
+        <v>800</v>
+      </c>
+      <c r="B168" s="45" t="s">
+        <v>568</v>
+      </c>
+      <c r="C168" s="45" t="s">
+        <v>805</v>
+      </c>
+      <c r="D168" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="E168" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="F168" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="G168" s="45" t="s">
+        <v>662</v>
+      </c>
+      <c r="H168" s="45" t="s">
+        <v>817</v>
+      </c>
+      <c r="I168" s="45">
+        <v>3</v>
+      </c>
+      <c r="J168" s="45" t="s">
         <v>401</v>
       </c>
-      <c r="K164" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="L164" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="M164" s="58" t="s">
+      <c r="K168" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="L168" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M168" s="58" t="s">
         <v>653</v>
       </c>
-      <c r="N164" s="58"/>
-      <c r="O164" s="16" t="s">
+      <c r="N168" s="58"/>
+      <c r="O168" s="16" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A169" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O164">
-    <sortCondition ref="D2:D164"/>
-    <sortCondition ref="E2:E164"/>
-    <sortCondition ref="F2:F164"/>
-    <sortCondition ref="G2:G164"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O168">
+    <sortCondition ref="D2:D168"/>
+    <sortCondition ref="E2:E168"/>
+    <sortCondition ref="F2:F168"/>
+    <sortCondition ref="G2:G168"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B60" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Introduced LGF (Large-genome flavivirus) lineage into taxonomic schema
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B348C4-D420-1149-B5D0-A409E135AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB917C21-47FD-D34F-907F-B414BC3D909D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23120" yWindow="940" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4740,8 +4740,8 @@
   <dimension ref="A1:P169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated tabular data for new species references
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317A397-50A5-4A4E-B41E-34C92A9636BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45167AB6-678F-684C-A84D-F3068019D589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23120" yWindow="940" windowWidth="23260" windowHeight="24280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$O$120</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -38,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3016" uniqueCount="1050">
   <si>
     <t>AY632538</t>
   </si>
@@ -2576,19 +2567,630 @@
   </si>
   <si>
     <t>Chondricthyes</t>
+  </si>
+  <si>
+    <t>Guereza hepacivirus</t>
+  </si>
+  <si>
+    <t>NC_031950</t>
+  </si>
+  <si>
+    <t>Hepacivirus I</t>
+  </si>
+  <si>
+    <t>NC_038428</t>
+  </si>
+  <si>
+    <t>GuHV</t>
+  </si>
+  <si>
+    <t>HVI</t>
+  </si>
+  <si>
+    <t>Rodent (Rhabdomys pumilio)</t>
+  </si>
+  <si>
+    <t>Hepacivirus F</t>
+  </si>
+  <si>
+    <t>NC_038427</t>
+  </si>
+  <si>
+    <t>Rodent (Myodes glareolus)</t>
+  </si>
+  <si>
+    <t>HVF</t>
+  </si>
+  <si>
+    <t>Hepacivirus J</t>
+  </si>
+  <si>
+    <t>NC_038429</t>
+  </si>
+  <si>
+    <t>HVJ</t>
+  </si>
+  <si>
+    <t>NC_040815</t>
+  </si>
+  <si>
+    <t>Hepacivirus P</t>
+  </si>
+  <si>
+    <t>HVP</t>
+  </si>
+  <si>
+    <t>Rodent (Citellus dauricus Brandt)</t>
+  </si>
+  <si>
+    <t>NC_031947</t>
+  </si>
+  <si>
+    <t>Bat Hepacivirus</t>
+  </si>
+  <si>
+    <t>BHV</t>
+  </si>
+  <si>
+    <t>Bat (Otomops martiensseni)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_038432 </t>
+  </si>
+  <si>
+    <t>Hepacivirus N</t>
+  </si>
+  <si>
+    <t>HVN</t>
+  </si>
+  <si>
+    <t>Hepacivirus K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_038430 </t>
+  </si>
+  <si>
+    <t>HVK</t>
+  </si>
+  <si>
+    <t>Bat (Hipposideros vittatus)</t>
+  </si>
+  <si>
+    <t>NC_038426</t>
+  </si>
+  <si>
+    <t>Hepacivirus B</t>
+  </si>
+  <si>
+    <t>Primate (Tamarin)</t>
+  </si>
+  <si>
+    <t>HVB</t>
+  </si>
+  <si>
+    <t>NC_031916</t>
+  </si>
+  <si>
+    <t>Hepacivirus L</t>
+  </si>
+  <si>
+    <t>HVL</t>
+  </si>
+  <si>
+    <t>Hepacivirus M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_038431 </t>
+  </si>
+  <si>
+    <t>HVM</t>
+  </si>
+  <si>
+    <t>GBVB</t>
+  </si>
+  <si>
+    <t>Hepatitis GB virus B</t>
+  </si>
+  <si>
+    <t>NC_001655</t>
+  </si>
+  <si>
+    <t>BK013349</t>
+  </si>
+  <si>
+    <t>Bat Hepacivirus PM_01</t>
+  </si>
+  <si>
+    <t>BHV-PM_01</t>
+  </si>
+  <si>
+    <t>Bat (Peropteryx_macrotis)</t>
+  </si>
+  <si>
+    <t>Sloths (Bradypus variegatus)</t>
+  </si>
+  <si>
+    <t>MH844500</t>
+  </si>
+  <si>
+    <t>Sloth hepacivirus</t>
+  </si>
+  <si>
+    <t>SHV</t>
+  </si>
+  <si>
+    <t>MZ393518</t>
+  </si>
+  <si>
+    <t>Ringtail Racoon Hepacivirus</t>
+  </si>
+  <si>
+    <t>RRHV</t>
+  </si>
+  <si>
+    <t>Racoon (Bassariscus astutus)</t>
+  </si>
+  <si>
+    <t>Jogalong Hepacivirus</t>
+  </si>
+  <si>
+    <t>JHV</t>
+  </si>
+  <si>
+    <t>MN133813</t>
+  </si>
+  <si>
+    <t>Sifaka Hepacivirus</t>
+  </si>
+  <si>
+    <t>Primate (Lemur)</t>
+  </si>
+  <si>
+    <t>MK026585</t>
+  </si>
+  <si>
+    <t>Collins Beach Virus</t>
+  </si>
+  <si>
+    <t>CBV</t>
+  </si>
+  <si>
+    <t>Insect (Ixodes holocyclus)?</t>
+  </si>
+  <si>
+    <t>Insect (culex annulirostris)?</t>
+  </si>
+  <si>
+    <t>Canine Hepacivirus</t>
+  </si>
+  <si>
+    <t>CHV</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Sigmodontinae hepacivirus</t>
+  </si>
+  <si>
+    <t>Rodent (oligoryzomys nigripes)</t>
+  </si>
+  <si>
+    <t>Chinese softshell turtle hepacivirus</t>
+  </si>
+  <si>
+    <t>MG599999</t>
+  </si>
+  <si>
+    <t>STHV</t>
+  </si>
+  <si>
+    <t>Turtle (Pelodiscus sinensis)</t>
+  </si>
+  <si>
+    <t>Guangxi houndshark hepacivirus</t>
+  </si>
+  <si>
+    <t>GHHV</t>
+  </si>
+  <si>
+    <t>Shark (Mustelus manazo)</t>
+  </si>
+  <si>
+    <t>Xiamen sepia Stingray hepacivirus</t>
+  </si>
+  <si>
+    <t>XSSHV</t>
+  </si>
+  <si>
+    <t>Ray (Urolophus aurantiacus)</t>
+  </si>
+  <si>
+    <t>Bald Eagle Hepacivirus</t>
+  </si>
+  <si>
+    <t>Eagle (Haliaeetus leucocephalus)</t>
+  </si>
+  <si>
+    <t>Duck Hepacivirus</t>
+  </si>
+  <si>
+    <t>Duck</t>
+  </si>
+  <si>
+    <t>African Lungfish Hepacivirus</t>
+  </si>
+  <si>
+    <t>BEHV</t>
+  </si>
+  <si>
+    <t>DHV</t>
+  </si>
+  <si>
+    <t>ALHV</t>
+  </si>
+  <si>
+    <t>Lung Fish</t>
+  </si>
+  <si>
+    <t>Nanhai dogfish shark hepacivirus</t>
+  </si>
+  <si>
+    <t>NDSHV</t>
+  </si>
+  <si>
+    <t>Dogfish Shark</t>
+  </si>
+  <si>
+    <t>Guangxi chinese leopard gecko hepacivirus</t>
+  </si>
+  <si>
+    <t>LPHV</t>
+  </si>
+  <si>
+    <t>Leopard Gecko</t>
+  </si>
+  <si>
+    <t>Gecko (Teratoscincus roborowskii)</t>
+  </si>
+  <si>
+    <t>YTRHV</t>
+  </si>
+  <si>
+    <t>MT371443</t>
+  </si>
+  <si>
+    <t>Koala Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371442</t>
+  </si>
+  <si>
+    <t>Pelican Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371441</t>
+  </si>
+  <si>
+    <t>Magpie Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371440</t>
+  </si>
+  <si>
+    <t>Bandicoot Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371439</t>
+  </si>
+  <si>
+    <t>Gecko Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371437</t>
+  </si>
+  <si>
+    <t>Marmoset Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371436</t>
+  </si>
+  <si>
+    <t>Blue Tit Hepacivirus</t>
+  </si>
+  <si>
+    <t>MT371434</t>
+  </si>
+  <si>
+    <t>Bush Baby Hepacivirus</t>
+  </si>
+  <si>
+    <t>KHV</t>
+  </si>
+  <si>
+    <t>PHV</t>
+  </si>
+  <si>
+    <t>MHV</t>
+  </si>
+  <si>
+    <t>GHV</t>
+  </si>
+  <si>
+    <t>MpHV</t>
+  </si>
+  <si>
+    <t>BcHV</t>
+  </si>
+  <si>
+    <t>BTHV</t>
+  </si>
+  <si>
+    <t>BBHV</t>
+  </si>
+  <si>
+    <t>Koala</t>
+  </si>
+  <si>
+    <t>Pelican</t>
+  </si>
+  <si>
+    <t>Magpie</t>
+  </si>
+  <si>
+    <t>Bandicoot</t>
+  </si>
+  <si>
+    <t>Gecko</t>
+  </si>
+  <si>
+    <t>Marmoset</t>
+  </si>
+  <si>
+    <t>Blue Tit</t>
+  </si>
+  <si>
+    <t>Bush Baby</t>
+  </si>
+  <si>
+    <t>Bat Pegivirus</t>
+  </si>
+  <si>
+    <t>BPV</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Pegivirus B/GB-Virus D</t>
+  </si>
+  <si>
+    <t>GBVD</t>
+  </si>
+  <si>
+    <t>Pegivirus I</t>
+  </si>
+  <si>
+    <t>PVI</t>
+  </si>
+  <si>
+    <t>Bat (sturnira lilium)</t>
+  </si>
+  <si>
+    <t>Porcine Pegivirus</t>
+  </si>
+  <si>
+    <t>PPV</t>
+  </si>
+  <si>
+    <t>Pegivirus K</t>
+  </si>
+  <si>
+    <t>PVK</t>
+  </si>
+  <si>
+    <t>Dophin Pegivirus</t>
+  </si>
+  <si>
+    <t>DPV</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>NC_038434</t>
+  </si>
+  <si>
+    <t>Pegivirus F</t>
+  </si>
+  <si>
+    <t>Bat (Carollia perspicillata)</t>
+  </si>
+  <si>
+    <t>PVF</t>
+  </si>
+  <si>
+    <t>Pegivirus G</t>
+  </si>
+  <si>
+    <t>PVG</t>
+  </si>
+  <si>
+    <t>Bat (Scotophilus dinganii)</t>
+  </si>
+  <si>
+    <t>Goose Pegivirus</t>
+  </si>
+  <si>
+    <t>GPV</t>
+  </si>
+  <si>
+    <t>Geese (Anser cygnoides)</t>
+  </si>
+  <si>
+    <t>Bat Pestivirus V4</t>
+  </si>
+  <si>
+    <t>BPVV4</t>
+  </si>
+  <si>
+    <t>Bat Pestivirus V3</t>
+  </si>
+  <si>
+    <t>BPVV3</t>
+  </si>
+  <si>
+    <t>Bat Pestivirus V1</t>
+  </si>
+  <si>
+    <t>BPVV1</t>
+  </si>
+  <si>
+    <t>Rodent Pestivirus Nn</t>
+  </si>
+  <si>
+    <t>RPVNn</t>
+  </si>
+  <si>
+    <t>Rodent Pestivirus Ad</t>
+  </si>
+  <si>
+    <t>RPVAd</t>
+  </si>
+  <si>
+    <t>Rodent Pestivirus Ap</t>
+  </si>
+  <si>
+    <t>RPVAp</t>
+  </si>
+  <si>
+    <t>Rodent Pestivirus Ne</t>
+  </si>
+  <si>
+    <t>RPVNe</t>
+  </si>
+  <si>
+    <t>Rodent</t>
+  </si>
+  <si>
+    <t>Giraffe Pestivirus</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>NC_035432</t>
+  </si>
+  <si>
+    <t>Linda Virus</t>
+  </si>
+  <si>
+    <t>LPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_018713 </t>
+  </si>
+  <si>
+    <t>Aydin Virus</t>
+  </si>
+  <si>
+    <t>APV</t>
+  </si>
+  <si>
+    <t>MT513216</t>
+  </si>
+  <si>
+    <t>Southwest bike trail virus</t>
+  </si>
+  <si>
+    <t>SOBV</t>
+  </si>
+  <si>
+    <t>primate (Aotus trivirgatus)</t>
+  </si>
+  <si>
+    <t>NC_038435</t>
+  </si>
+  <si>
+    <t>MW091548</t>
+  </si>
+  <si>
+    <t>MH282911</t>
+  </si>
+  <si>
+    <t>MH282910</t>
+  </si>
+  <si>
+    <t>MH282908</t>
+  </si>
+  <si>
+    <t>KY370103</t>
+  </si>
+  <si>
+    <t>KY370102</t>
+  </si>
+  <si>
+    <t>KY370100</t>
+  </si>
+  <si>
+    <t>KY370099</t>
+  </si>
+  <si>
+    <t>MG599995</t>
+  </si>
+  <si>
+    <t>MG599988</t>
+  </si>
+  <si>
+    <t>MG599994</t>
+  </si>
+  <si>
+    <t>MG599992</t>
+  </si>
+  <si>
+    <t>KU351670</t>
+  </si>
+  <si>
+    <t>MK059751</t>
+  </si>
+  <si>
+    <t>MH824541</t>
+  </si>
+  <si>
+    <t>JQ181558</t>
+  </si>
+  <si>
+    <t>MH370348</t>
+  </si>
+  <si>
+    <t>MN062427</t>
+  </si>
+  <si>
+    <t>MK737641</t>
+  </si>
+  <si>
+    <t>KC796073</t>
+  </si>
+  <si>
+    <t>NC_030291</t>
+  </si>
+  <si>
+    <t>KC796088</t>
+  </si>
+  <si>
+    <t>NC_034442</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2660,6 +3262,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="25">
@@ -2817,7 +3449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="725">
+  <cellStyleXfs count="776">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3543,8 +4175,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3674,8 +4357,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="725">
+  <cellStyles count="776">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4090,6 +4794,57 @@
     <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4737,11 +5492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P169"/>
+  <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B133" sqref="A1:P168"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B197" sqref="A1:P225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12665,8 +13420,1859 @@
         <v>729</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A169" s="1"/>
+    <row r="169" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C169" s="26" t="s">
+        <v>850</v>
+      </c>
+      <c r="D169" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E169" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F169" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G169" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H169" s="26"/>
+      <c r="I169" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K169" s="26" t="s">
+        <v>580</v>
+      </c>
+      <c r="L169" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M169" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A170" s="65" t="s">
+        <v>849</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C170" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E170" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F170" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G170" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H170" s="26"/>
+      <c r="I170" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K170" s="26" t="s">
+        <v>852</v>
+      </c>
+      <c r="L170" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M170" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A171" s="65" t="s">
+        <v>854</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C171" s="26" t="s">
+        <v>856</v>
+      </c>
+      <c r="D171" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E171" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F171" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G171" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H171" s="26"/>
+      <c r="I171" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K171" s="26" t="s">
+        <v>855</v>
+      </c>
+      <c r="L171" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M171" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A172" s="65" t="s">
+        <v>858</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C172" s="26" t="s">
+        <v>859</v>
+      </c>
+      <c r="D172" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F172" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G172" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H172" s="26"/>
+      <c r="I172" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K172" s="26" t="s">
+        <v>855</v>
+      </c>
+      <c r="L172" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M172" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A173" s="65" t="s">
+        <v>860</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C173" s="26" t="s">
+        <v>862</v>
+      </c>
+      <c r="D173" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F173" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G173" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H173" s="26"/>
+      <c r="I173" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K173" s="26" t="s">
+        <v>863</v>
+      </c>
+      <c r="L173" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M173" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A174" s="65" t="s">
+        <v>864</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C174" s="26" t="s">
+        <v>866</v>
+      </c>
+      <c r="D174" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F174" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G174" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H174" s="26"/>
+      <c r="I174" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K174" s="26" t="s">
+        <v>867</v>
+      </c>
+      <c r="L174" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M174" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A175" s="65" t="s">
+        <v>868</v>
+      </c>
+      <c r="B175" s="65" t="s">
+        <v>869</v>
+      </c>
+      <c r="C175" s="26" t="s">
+        <v>870</v>
+      </c>
+      <c r="D175" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F175" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G175" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H175" s="26"/>
+      <c r="I175" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K175" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="L175" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M175" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A176" s="65" t="s">
+        <v>872</v>
+      </c>
+      <c r="B176" s="65" t="s">
+        <v>871</v>
+      </c>
+      <c r="C176" s="26" t="s">
+        <v>873</v>
+      </c>
+      <c r="D176" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E176" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F176" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G176" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H176" s="26"/>
+      <c r="I176" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K176" s="26" t="s">
+        <v>874</v>
+      </c>
+      <c r="L176" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M176" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A177" s="65" t="s">
+        <v>875</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="C177" s="26" t="s">
+        <v>878</v>
+      </c>
+      <c r="D177" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E177" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F177" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G177" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H177" s="26"/>
+      <c r="I177" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K177" s="26" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A178" s="65" t="s">
+        <v>879</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C178" s="26" t="s">
+        <v>881</v>
+      </c>
+      <c r="D178" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E178" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F178" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G178" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H178" s="26"/>
+      <c r="I178" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K178" s="26" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A179" s="65" t="s">
+        <v>883</v>
+      </c>
+      <c r="B179" s="65" t="s">
+        <v>882</v>
+      </c>
+      <c r="C179" s="26" t="s">
+        <v>884</v>
+      </c>
+      <c r="D179" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E179" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F179" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G179" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H179" s="26"/>
+      <c r="I179" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K179" s="26" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A180" s="65" t="s">
+        <v>887</v>
+      </c>
+      <c r="B180" s="65" t="s">
+        <v>886</v>
+      </c>
+      <c r="C180" s="26" t="s">
+        <v>885</v>
+      </c>
+      <c r="D180" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F180" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G180" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H180" s="26"/>
+      <c r="I180" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K180" s="26" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A181" s="65" t="s">
+        <v>888</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C181" s="26" t="s">
+        <v>890</v>
+      </c>
+      <c r="D181" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E181" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F181" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G181" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H181" s="26"/>
+      <c r="I181" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K181" s="26" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A182" s="65" t="s">
+        <v>893</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C182" s="26" t="s">
+        <v>895</v>
+      </c>
+      <c r="D182" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F182" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G182" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H182" s="26"/>
+      <c r="I182" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K182" s="26" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A183" s="65" t="s">
+        <v>896</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C183" s="26" t="s">
+        <v>898</v>
+      </c>
+      <c r="D183" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E183" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F183" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G183" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H183" s="26"/>
+      <c r="I183" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K183" s="65" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A184" s="65" t="s">
+        <v>902</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="C184" s="26" t="s">
+        <v>901</v>
+      </c>
+      <c r="D184" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E184" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F184" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G184" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H184" s="26"/>
+      <c r="I184" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K184" s="26" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A185" s="73" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B185" s="70" t="s">
+        <v>903</v>
+      </c>
+      <c r="C185" s="71" t="s">
+        <v>895</v>
+      </c>
+      <c r="D185" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E185" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F185" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G185" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H185" s="71"/>
+      <c r="I185" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K185" s="71" t="s">
+        <v>904</v>
+      </c>
+      <c r="L185" s="70"/>
+      <c r="M185" s="70"/>
+      <c r="N185" s="70"/>
+    </row>
+    <row r="186" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A186" s="65" t="s">
+        <v>905</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C186" s="26" t="s">
+        <v>907</v>
+      </c>
+      <c r="D186" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E186" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F186" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G186" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H186" s="26"/>
+      <c r="I186" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K186" s="26" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A187" s="73" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B187" s="70" t="s">
+        <v>910</v>
+      </c>
+      <c r="C187" s="71" t="s">
+        <v>911</v>
+      </c>
+      <c r="D187" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E187" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F187" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G187" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H187" s="71"/>
+      <c r="I187" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K187" s="71" t="s">
+        <v>912</v>
+      </c>
+      <c r="L187" s="70"/>
+      <c r="M187" s="70"/>
+      <c r="N187" s="70"/>
+    </row>
+    <row r="188" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A188" s="73" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B188" s="73" t="s">
+        <v>913</v>
+      </c>
+      <c r="C188" s="71" t="s">
+        <v>895</v>
+      </c>
+      <c r="D188" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E188" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F188" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G188" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H188" s="71"/>
+      <c r="I188" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K188" s="71" t="s">
+        <v>914</v>
+      </c>
+      <c r="L188" s="70"/>
+      <c r="M188" s="70"/>
+      <c r="N188" s="70"/>
+    </row>
+    <row r="189" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A189" s="66" t="s">
+        <v>916</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C189" s="26" t="s">
+        <v>917</v>
+      </c>
+      <c r="D189" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E189" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G189" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H189" s="26"/>
+      <c r="I189" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K189" s="26" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A190" s="69" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B190" s="70" t="s">
+        <v>919</v>
+      </c>
+      <c r="C190" s="71" t="s">
+        <v>920</v>
+      </c>
+      <c r="D190" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E190" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F190" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G190" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H190" s="71"/>
+      <c r="I190" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K190" s="71" t="s">
+        <v>921</v>
+      </c>
+      <c r="L190" s="70"/>
+      <c r="M190" s="70"/>
+      <c r="N190" s="70"/>
+    </row>
+    <row r="191" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A191" s="69" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B191" s="70" t="s">
+        <v>922</v>
+      </c>
+      <c r="C191" s="71" t="s">
+        <v>923</v>
+      </c>
+      <c r="D191" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E191" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F191" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G191" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H191" s="71"/>
+      <c r="I191" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K191" s="71" t="s">
+        <v>924</v>
+      </c>
+      <c r="L191" s="70"/>
+      <c r="M191" s="70"/>
+      <c r="N191" s="70"/>
+    </row>
+    <row r="192" spans="1:14" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A192" s="73" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B192" s="70" t="s">
+        <v>925</v>
+      </c>
+      <c r="C192" s="71" t="s">
+        <v>930</v>
+      </c>
+      <c r="D192" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E192" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F192" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G192" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H192" s="71"/>
+      <c r="I192" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K192" s="71" t="s">
+        <v>926</v>
+      </c>
+      <c r="L192" s="70"/>
+      <c r="M192" s="70"/>
+      <c r="N192" s="70"/>
+    </row>
+    <row r="193" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A193" s="73" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B193" s="70" t="s">
+        <v>927</v>
+      </c>
+      <c r="C193" s="71" t="s">
+        <v>931</v>
+      </c>
+      <c r="D193" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E193" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F193" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G193" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H193" s="71"/>
+      <c r="I193" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K193" s="71" t="s">
+        <v>928</v>
+      </c>
+      <c r="L193" s="70"/>
+      <c r="M193" s="70"/>
+      <c r="N193" s="70"/>
+    </row>
+    <row r="194" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A194" s="69" t="s">
+        <v>669</v>
+      </c>
+      <c r="B194" s="70" t="s">
+        <v>929</v>
+      </c>
+      <c r="C194" s="71" t="s">
+        <v>932</v>
+      </c>
+      <c r="D194" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E194" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F194" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G194" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H194" s="71"/>
+      <c r="I194" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K194" s="71" t="s">
+        <v>933</v>
+      </c>
+      <c r="L194" s="70"/>
+      <c r="M194" s="70"/>
+      <c r="N194" s="70"/>
+    </row>
+    <row r="195" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A195" s="69" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B195" s="73" t="s">
+        <v>934</v>
+      </c>
+      <c r="C195" s="71" t="s">
+        <v>935</v>
+      </c>
+      <c r="D195" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E195" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F195" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G195" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H195" s="71"/>
+      <c r="I195" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K195" s="71" t="s">
+        <v>936</v>
+      </c>
+      <c r="L195" s="70"/>
+      <c r="M195" s="70"/>
+      <c r="N195" s="70"/>
+    </row>
+    <row r="196" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A196" s="69" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B196" s="73" t="s">
+        <v>937</v>
+      </c>
+      <c r="C196" s="71" t="s">
+        <v>938</v>
+      </c>
+      <c r="D196" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E196" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F196" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G196" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H196" s="71"/>
+      <c r="I196" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K196" s="71" t="s">
+        <v>939</v>
+      </c>
+      <c r="L196" s="70"/>
+      <c r="M196" s="70"/>
+      <c r="N196" s="70"/>
+    </row>
+    <row r="197" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A197" s="69" t="s">
+        <v>665</v>
+      </c>
+      <c r="B197" s="73" t="s">
+        <v>706</v>
+      </c>
+      <c r="C197" s="71" t="s">
+        <v>941</v>
+      </c>
+      <c r="D197" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E197" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F197" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G197" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="H197" s="71"/>
+      <c r="I197" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K197" s="71" t="s">
+        <v>940</v>
+      </c>
+      <c r="L197" s="70"/>
+      <c r="M197" s="70"/>
+      <c r="N197" s="70"/>
+    </row>
+    <row r="198" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A198" s="67" t="s">
+        <v>942</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C198" s="26" t="s">
+        <v>958</v>
+      </c>
+      <c r="D198" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E198" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F198" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G198" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H198" s="26"/>
+      <c r="I198" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K198" s="26" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A199" s="67" t="s">
+        <v>944</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C199" s="26" t="s">
+        <v>959</v>
+      </c>
+      <c r="D199" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E199" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F199" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G199" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H199" s="26"/>
+      <c r="I199" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K199" s="26" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A200" s="67" t="s">
+        <v>946</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C200" s="26" t="s">
+        <v>962</v>
+      </c>
+      <c r="D200" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E200" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F200" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G200" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H200" s="26"/>
+      <c r="I200" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K200" s="26" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A201" s="67" t="s">
+        <v>948</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C201" s="26" t="s">
+        <v>963</v>
+      </c>
+      <c r="D201" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E201" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F201" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G201" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H201" s="26"/>
+      <c r="I201" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K201" s="26" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A202" s="67" t="s">
+        <v>950</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C202" s="26" t="s">
+        <v>961</v>
+      </c>
+      <c r="D202" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E202" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F202" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G202" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H202" s="26"/>
+      <c r="I202" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K202" s="26" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A203" s="67" t="s">
+        <v>952</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C203" s="26" t="s">
+        <v>960</v>
+      </c>
+      <c r="D203" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E203" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F203" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G203" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H203" s="26"/>
+      <c r="I203" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K203" s="26" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A204" s="67" t="s">
+        <v>954</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C204" s="26" t="s">
+        <v>964</v>
+      </c>
+      <c r="D204" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E204" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F204" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G204" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H204" s="26"/>
+      <c r="I204" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K204" s="26" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A205" s="67" t="s">
+        <v>956</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C205" s="26" t="s">
+        <v>965</v>
+      </c>
+      <c r="D205" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E205" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F205" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G205" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="H205" s="26"/>
+      <c r="I205" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K205" s="26" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A206" s="74" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B206" s="71" t="s">
+        <v>974</v>
+      </c>
+      <c r="C206" s="71" t="s">
+        <v>975</v>
+      </c>
+      <c r="D206" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E206" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F206" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G206" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H206" s="71"/>
+      <c r="I206" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="J206" s="71"/>
+      <c r="K206" s="71" t="s">
+        <v>976</v>
+      </c>
+      <c r="L206" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="M206" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="N206" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="O206" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="P206" s="77" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A207" s="73" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B207" s="70" t="s">
+        <v>977</v>
+      </c>
+      <c r="C207" s="71" t="s">
+        <v>978</v>
+      </c>
+      <c r="D207" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E207" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F207" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G207" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H207" s="71"/>
+      <c r="I207" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="J207" s="71"/>
+      <c r="K207" s="71" t="s">
+        <v>976</v>
+      </c>
+      <c r="L207" s="70"/>
+      <c r="M207" s="70"/>
+      <c r="N207" s="70"/>
+    </row>
+    <row r="208" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A208" s="73" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B208" s="70" t="s">
+        <v>979</v>
+      </c>
+      <c r="C208" s="71" t="s">
+        <v>980</v>
+      </c>
+      <c r="D208" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E208" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F208" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G208" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H208" s="71"/>
+      <c r="I208" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K208" s="71" t="s">
+        <v>981</v>
+      </c>
+      <c r="L208" s="70"/>
+      <c r="M208" s="70"/>
+      <c r="N208" s="70"/>
+    </row>
+    <row r="209" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A209" s="69" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B209" s="70" t="s">
+        <v>982</v>
+      </c>
+      <c r="C209" s="71" t="s">
+        <v>983</v>
+      </c>
+      <c r="D209" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E209" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F209" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G209" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H209" s="71"/>
+      <c r="I209" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K209" s="71" t="s">
+        <v>522</v>
+      </c>
+      <c r="L209" s="70"/>
+      <c r="M209" s="70"/>
+      <c r="N209" s="70"/>
+    </row>
+    <row r="210" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A210" s="73" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B210" s="70" t="s">
+        <v>984</v>
+      </c>
+      <c r="C210" s="71" t="s">
+        <v>985</v>
+      </c>
+      <c r="D210" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E210" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F210" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G210" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H210" s="71"/>
+      <c r="I210" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K210" s="71" t="s">
+        <v>522</v>
+      </c>
+      <c r="L210" s="70"/>
+      <c r="M210" s="70"/>
+      <c r="N210" s="70"/>
+    </row>
+    <row r="211" spans="1:16" s="69" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A211" s="69" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B211" s="70" t="s">
+        <v>986</v>
+      </c>
+      <c r="C211" s="71" t="s">
+        <v>987</v>
+      </c>
+      <c r="D211" s="72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E211" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="F211" s="72" t="s">
+        <v>744</v>
+      </c>
+      <c r="G211" s="71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H211" s="71"/>
+      <c r="I211" s="71" t="s">
+        <v>815</v>
+      </c>
+      <c r="K211" s="71" t="s">
+        <v>988</v>
+      </c>
+      <c r="L211" s="70"/>
+      <c r="M211" s="70"/>
+      <c r="N211" s="70"/>
+    </row>
+    <row r="212" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A212" s="68" t="s">
+        <v>989</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C212" s="26" t="s">
+        <v>992</v>
+      </c>
+      <c r="D212" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E212" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F212" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G212" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="H212" s="26"/>
+      <c r="I212" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K212" s="26" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A213" s="66" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C213" s="26" t="s">
+        <v>994</v>
+      </c>
+      <c r="D213" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E213" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F213" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G213" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="H213" s="26"/>
+      <c r="I213" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K213" s="26" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A214" s="66" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C214" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="D214" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E214" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F214" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G214" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="H214" s="26"/>
+      <c r="I214" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K214" s="26" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A215" s="45" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B215" s="47" t="s">
+        <v>999</v>
+      </c>
+      <c r="C215" s="47" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D215" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E215" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F215" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G215" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H215" s="47"/>
+      <c r="I215" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J215" s="47"/>
+      <c r="K215" s="47" t="s">
+        <v>976</v>
+      </c>
+      <c r="L215" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="M215" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="N215" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="O215" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="P215" s="58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A216" s="67" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B216" s="47" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C216" s="47" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D216" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E216" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F216" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G216" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H216" s="47"/>
+      <c r="I216" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J216" s="47"/>
+      <c r="K216" s="47" t="s">
+        <v>976</v>
+      </c>
+      <c r="L216" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A217" s="67" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B217" s="47" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C217" s="47" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D217" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E217" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F217" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G217" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H217" s="47"/>
+      <c r="I217" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J217" s="47"/>
+      <c r="K217" s="47" t="s">
+        <v>976</v>
+      </c>
+      <c r="L217" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A218" s="67" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C218" s="47" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D218" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E218" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F218" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G218" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H218" s="47"/>
+      <c r="I218" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J218" s="47"/>
+      <c r="K218" s="47" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A219" s="67" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C219" s="47" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D219" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E219" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F219" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G219" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H219" s="47"/>
+      <c r="I219" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J219" s="47"/>
+      <c r="K219" s="47" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A220" s="67" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C220" s="47" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D220" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E220" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F220" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G220" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H220" s="47"/>
+      <c r="I220" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J220" s="47"/>
+      <c r="K220" s="47" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A221" s="67" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C221" s="47" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D221" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E221" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F221" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G221" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H221" s="47"/>
+      <c r="I221" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J221" s="47"/>
+      <c r="K221" s="47" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A222" s="66" t="s">
+        <v>229</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C222" s="47" t="s">
+        <v>997</v>
+      </c>
+      <c r="D222" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E222" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F222" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G222" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H222" s="47"/>
+      <c r="I222" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J222" s="47"/>
+      <c r="K222" s="47" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A223" s="65" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C223" s="47" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D223" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E223" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F223" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G223" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H223" s="47"/>
+      <c r="I223" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J223" s="47"/>
+      <c r="K223" s="47" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A224" s="65" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C224" s="47" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D224" s="47" t="s">
+        <v>733</v>
+      </c>
+      <c r="E224" s="47" t="s">
+        <v>658</v>
+      </c>
+      <c r="F224" s="47" t="s">
+        <v>844</v>
+      </c>
+      <c r="G224" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="H224" s="47"/>
+      <c r="I224" s="47" t="s">
+        <v>815</v>
+      </c>
+      <c r="J224" s="47"/>
+      <c r="K224" s="47" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A225" s="66" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C225" s="26" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D225" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="E225" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="F225" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="G225" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="H225" s="26"/>
+      <c r="I225" s="26" t="s">
+        <v>815</v>
+      </c>
+      <c r="K225" s="26" t="s">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P168">

</xml_diff>

<commit_message>
Updated reference set. Validated build
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCA094A-9CC2-224E-92A5-1025FF751AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B695016-851E-BF44-93B2-346F93963024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="500" windowWidth="45720" windowHeight="25040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="1101">
   <si>
     <t>AY632538</t>
   </si>
@@ -3329,6 +3329,9 @@
   </si>
   <si>
     <t>Podargiformes</t>
+  </si>
+  <si>
+    <t>Perissodactyla</t>
   </si>
 </sst>
 </file>
@@ -5680,9 +5683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L219" sqref="A1:R225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16764,10 +16767,10 @@
         <v>1047</v>
       </c>
       <c r="L215" s="71" t="s">
-        <v>580</v>
+        <v>1100</v>
       </c>
       <c r="M215" s="70" t="s">
-        <v>728</v>
+        <v>518</v>
       </c>
       <c r="N215" s="14" t="s">
         <v>195</v>
@@ -16782,7 +16785,7 @@
         <v>1</v>
       </c>
       <c r="R215" s="58" t="s">
-        <v>728</v>
+        <v>162</v>
       </c>
     </row>
     <row r="216" spans="1:18" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactoring - adding new references - hepaci-pegi sub-genus-level groups
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCA094A-9CC2-224E-92A5-1025FF751AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2DAE12-670C-5B43-BE5F-46AB5796CC77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="500" windowWidth="45720" windowHeight="25040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="1102">
   <si>
     <t>AY632538</t>
   </si>
@@ -3329,6 +3329,12 @@
   </si>
   <si>
     <t>Podargiformes</t>
+  </si>
+  <si>
+    <t>Pegi1</t>
+  </si>
+  <si>
+    <t>Pegi2</t>
   </si>
 </sst>
 </file>
@@ -5680,9 +5686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E219" sqref="A1:R225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16339,7 +16345,9 @@
       <c r="G207" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H207" s="70"/>
+      <c r="H207" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I207" s="70" t="s">
         <v>814</v>
       </c>
@@ -16391,7 +16399,9 @@
       <c r="G208" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H208" s="70"/>
+      <c r="H208" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I208" s="70" t="s">
         <v>814</v>
       </c>
@@ -16443,7 +16453,9 @@
       <c r="G209" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H209" s="70"/>
+      <c r="H209" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I209" s="70" t="s">
         <v>814</v>
       </c>
@@ -16495,7 +16507,9 @@
       <c r="G210" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H210" s="70"/>
+      <c r="H210" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I210" s="70" t="s">
         <v>814</v>
       </c>
@@ -16547,7 +16561,9 @@
       <c r="G211" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H211" s="70"/>
+      <c r="H211" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I211" s="70" t="s">
         <v>814</v>
       </c>
@@ -16599,7 +16615,9 @@
       <c r="G212" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H212" s="70"/>
+      <c r="H212" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I212" s="70" t="s">
         <v>814</v>
       </c>
@@ -16651,7 +16669,9 @@
       <c r="G213" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H213" s="70"/>
+      <c r="H213" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I213" s="70" t="s">
         <v>814</v>
       </c>
@@ -16703,7 +16723,9 @@
       <c r="G214" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H214" s="70"/>
+      <c r="H214" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I214" s="70" t="s">
         <v>814</v>
       </c>
@@ -16755,7 +16777,9 @@
       <c r="G215" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H215" s="70"/>
+      <c r="H215" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I215" s="70" t="s">
         <v>814</v>
       </c>
@@ -16807,7 +16831,9 @@
       <c r="G216" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H216" s="70"/>
+      <c r="H216" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I216" s="70" t="s">
         <v>814</v>
       </c>
@@ -16859,7 +16885,9 @@
       <c r="G217" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H217" s="70"/>
+      <c r="H217" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I217" s="70" t="s">
         <v>814</v>
       </c>
@@ -16905,7 +16933,9 @@
       <c r="G218" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H218" s="70"/>
+      <c r="H218" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I218" s="70" t="s">
         <v>814</v>
       </c>
@@ -16951,7 +16981,9 @@
       <c r="G219" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H219" s="70"/>
+      <c r="H219" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I219" s="70" t="s">
         <v>814</v>
       </c>
@@ -16997,7 +17029,9 @@
       <c r="G220" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H220" s="70"/>
+      <c r="H220" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I220" s="70" t="s">
         <v>814</v>
       </c>
@@ -17043,7 +17077,9 @@
       <c r="G221" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H221" s="70"/>
+      <c r="H221" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I221" s="70" t="s">
         <v>814</v>
       </c>
@@ -17089,7 +17125,9 @@
       <c r="G222" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H222" s="70"/>
+      <c r="H222" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I222" s="70" t="s">
         <v>814</v>
       </c>
@@ -17132,7 +17170,9 @@
       <c r="G223" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H223" s="70"/>
+      <c r="H223" s="70" t="s">
+        <v>1100</v>
+      </c>
       <c r="I223" s="70" t="s">
         <v>814</v>
       </c>
@@ -17175,7 +17215,9 @@
       <c r="G224" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H224" s="70"/>
+      <c r="H224" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I224" s="70" t="s">
         <v>814</v>
       </c>
@@ -17218,7 +17260,9 @@
       <c r="G225" s="70" t="s">
         <v>414</v>
       </c>
-      <c r="H225" s="70"/>
+      <c r="H225" s="70" t="s">
+        <v>1101</v>
+      </c>
       <c r="I225" s="70" t="s">
         <v>814</v>
       </c>

</xml_diff>

<commit_message>
New references for subgenus-level groups. Extensions to alignment tree.
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9BFE16-EECF-A243-905C-BF73403A1B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA386DB5-A6A5-3447-BA7B-B6B8516914D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1100">
   <si>
     <t>AY632538</t>
   </si>
@@ -3326,6 +3326,9 @@
   </si>
   <si>
     <t>Pesti2</t>
+  </si>
+  <si>
+    <t>Hepaci3</t>
   </si>
 </sst>
 </file>
@@ -5678,8 +5681,8 @@
   <dimension ref="A1:R225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C150" sqref="A1:R225"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G181" sqref="A1:R225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14933,7 +14936,7 @@
         <v>365</v>
       </c>
       <c r="H175" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I175" s="26" t="s">
         <v>802</v>
@@ -15025,7 +15028,7 @@
         <v>365</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I177" s="26" t="s">
         <v>802</v>
@@ -15165,7 +15168,7 @@
         <v>365</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I180" s="26" t="s">
         <v>802</v>

</xml_diff>

<commit_message>
Updated reference set and associated side-data
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA386DB5-A6A5-3447-BA7B-B6B8516914D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1D2C9E-58A0-4345-9EA8-44BC0107A064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1101">
   <si>
     <t>AY632538</t>
   </si>
@@ -3329,6 +3329,9 @@
   </si>
   <si>
     <t>Hepaci3</t>
+  </si>
+  <si>
+    <t>Pesti3</t>
   </si>
 </sst>
 </file>
@@ -5681,8 +5684,8 @@
   <dimension ref="A1:R225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G181" sqref="A1:R225"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H143" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13358,7 +13361,7 @@
         <v>322</v>
       </c>
       <c r="H145" s="47" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="I145" s="47" t="s">
         <v>802</v>
@@ -13520,7 +13523,7 @@
         <v>322</v>
       </c>
       <c r="H148" s="47" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="I148" s="47" t="s">
         <v>802</v>

</xml_diff>

<commit_message>
Refactor - label all master refseqs as 'REF_MASTER'
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72717DE-BFCA-C542-B628-97AC3F8B2FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDBFDE5-0132-3A4E-89B8-E1868A075D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -5681,11 +5681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R225"/>
+  <dimension ref="A1:R224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G145" sqref="A1:R225"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C140" sqref="A1:R224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12800,13 +12800,13 @@
     </row>
     <row r="135" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A135" s="45" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B135" s="46" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C135" s="47" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D135" s="47" t="s">
         <v>720</v>
@@ -12834,7 +12834,7 @@
         <v>1069</v>
       </c>
       <c r="M135" s="47" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="N135" s="14" t="s">
         <v>195</v>
@@ -12843,24 +12843,24 @@
         <v>195</v>
       </c>
       <c r="P135" s="57" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="Q135" s="59" t="s">
-        <v>471</v>
+        <v>1</v>
       </c>
       <c r="R135" s="58" t="s">
-        <v>135</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A136" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="B136" s="46" t="s">
-        <v>106</v>
+        <v>642</v>
+      </c>
+      <c r="B136" s="47" t="s">
+        <v>613</v>
       </c>
       <c r="C136" s="47" t="s">
-        <v>348</v>
+        <v>634</v>
       </c>
       <c r="D136" s="47" t="s">
         <v>720</v>
@@ -12875,20 +12875,20 @@
         <v>322</v>
       </c>
       <c r="H136" s="47" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="I136" s="47" t="s">
         <v>802</v>
       </c>
       <c r="J136" s="85"/>
       <c r="K136" s="47" t="s">
-        <v>1034</v>
+        <v>1040</v>
       </c>
       <c r="L136" s="47" t="s">
-        <v>1069</v>
+        <v>1040</v>
       </c>
       <c r="M136" s="47" t="s">
-        <v>521</v>
+        <v>1047</v>
       </c>
       <c r="N136" s="14" t="s">
         <v>195</v>
@@ -12897,24 +12897,24 @@
         <v>195</v>
       </c>
       <c r="P136" s="57" t="s">
-        <v>349</v>
+        <v>1</v>
       </c>
       <c r="Q136" s="59" t="s">
         <v>1</v>
       </c>
       <c r="R136" s="58" t="s">
-        <v>488</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="137" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A137" s="45" t="s">
-        <v>642</v>
-      </c>
-      <c r="B137" s="47" t="s">
-        <v>613</v>
+        <v>229</v>
+      </c>
+      <c r="B137" s="46" t="s">
+        <v>111</v>
       </c>
       <c r="C137" s="47" t="s">
-        <v>634</v>
+        <v>578</v>
       </c>
       <c r="D137" s="47" t="s">
         <v>720</v>
@@ -12929,20 +12929,20 @@
         <v>322</v>
       </c>
       <c r="H137" s="47" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="I137" s="47" t="s">
         <v>802</v>
       </c>
       <c r="J137" s="85"/>
       <c r="K137" s="47" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="L137" s="47" t="s">
-        <v>1040</v>
+        <v>1069</v>
       </c>
       <c r="M137" s="47" t="s">
-        <v>1047</v>
+        <v>515</v>
       </c>
       <c r="N137" s="14" t="s">
         <v>195</v>
@@ -12951,24 +12951,24 @@
         <v>195</v>
       </c>
       <c r="P137" s="57" t="s">
-        <v>1</v>
+        <v>357</v>
       </c>
       <c r="Q137" s="59" t="s">
         <v>1</v>
       </c>
       <c r="R137" s="58" t="s">
-        <v>1047</v>
+        <v>209</v>
       </c>
     </row>
     <row r="138" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A138" s="45" t="s">
-        <v>229</v>
+        <v>283</v>
       </c>
       <c r="B138" s="46" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="C138" s="47" t="s">
-        <v>578</v>
+        <v>419</v>
       </c>
       <c r="D138" s="47" t="s">
         <v>720</v>
@@ -12996,7 +12996,7 @@
         <v>1069</v>
       </c>
       <c r="M138" s="47" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="N138" s="14" t="s">
         <v>195</v>
@@ -13005,24 +13005,24 @@
         <v>195</v>
       </c>
       <c r="P138" s="57" t="s">
-        <v>357</v>
+        <v>1</v>
       </c>
       <c r="Q138" s="59" t="s">
-        <v>1</v>
+        <v>471</v>
       </c>
       <c r="R138" s="58" t="s">
-        <v>209</v>
+        <v>487</v>
       </c>
     </row>
     <row r="139" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A139" s="45" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
       <c r="B139" s="46" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C139" s="47" t="s">
-        <v>419</v>
+        <v>579</v>
       </c>
       <c r="D139" s="47" t="s">
         <v>720</v>
@@ -13050,7 +13050,7 @@
         <v>1069</v>
       </c>
       <c r="M139" s="47" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="N139" s="14" t="s">
         <v>195</v>
@@ -13059,24 +13059,24 @@
         <v>195</v>
       </c>
       <c r="P139" s="57" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="Q139" s="59" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="R139" s="58" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="140" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A140" s="45" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="B140" s="46" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="C140" s="47" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="D140" s="47" t="s">
         <v>720</v>
@@ -13104,7 +13104,7 @@
         <v>1069</v>
       </c>
       <c r="M140" s="47" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N140" s="14" t="s">
         <v>195</v>
@@ -13113,24 +13113,24 @@
         <v>195</v>
       </c>
       <c r="P140" s="57" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="Q140" s="59" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="R140" s="58" t="s">
-        <v>488</v>
+        <v>110</v>
       </c>
     </row>
     <row r="141" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A141" s="45" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="B141" s="46" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C141" s="47" t="s">
-        <v>582</v>
+        <v>406</v>
       </c>
       <c r="D141" s="47" t="s">
         <v>720</v>
@@ -13158,7 +13158,7 @@
         <v>1069</v>
       </c>
       <c r="M141" s="47" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="N141" s="14" t="s">
         <v>195</v>
@@ -13167,24 +13167,24 @@
         <v>195</v>
       </c>
       <c r="P141" s="57" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="Q141" s="59" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="R141" s="58" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="142" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A142" s="45" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B142" s="46" t="s">
-        <v>199</v>
+        <v>142</v>
       </c>
       <c r="C142" s="47" t="s">
-        <v>406</v>
+        <v>580</v>
       </c>
       <c r="D142" s="47" t="s">
         <v>720</v>
@@ -13212,7 +13212,7 @@
         <v>1069</v>
       </c>
       <c r="M142" s="47" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N142" s="14" t="s">
         <v>195</v>
@@ -13227,18 +13227,18 @@
         <v>470</v>
       </c>
       <c r="R142" s="58" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
     </row>
     <row r="143" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A143" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="B143" s="46" t="s">
-        <v>142</v>
+        <v>262</v>
+      </c>
+      <c r="B143" s="47" t="s">
+        <v>166</v>
       </c>
       <c r="C143" s="47" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D143" s="47" t="s">
         <v>720</v>
@@ -13253,7 +13253,7 @@
         <v>322</v>
       </c>
       <c r="H143" s="47" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="I143" s="47" t="s">
         <v>802</v>
@@ -13263,10 +13263,10 @@
         <v>1034</v>
       </c>
       <c r="L143" s="47" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="M143" s="47" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="N143" s="14" t="s">
         <v>195</v>
@@ -13275,24 +13275,24 @@
         <v>195</v>
       </c>
       <c r="P143" s="57" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="Q143" s="59" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="R143" s="58" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
     </row>
     <row r="144" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A144" s="45" t="s">
-        <v>262</v>
+        <v>631</v>
       </c>
       <c r="B144" s="47" t="s">
-        <v>166</v>
+        <v>632</v>
       </c>
       <c r="C144" s="47" t="s">
-        <v>581</v>
+        <v>633</v>
       </c>
       <c r="D144" s="47" t="s">
         <v>720</v>
@@ -13307,7 +13307,7 @@
         <v>322</v>
       </c>
       <c r="H144" s="47" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="I144" s="47" t="s">
         <v>802</v>
@@ -13317,10 +13317,10 @@
         <v>1034</v>
       </c>
       <c r="L144" s="47" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="M144" s="47" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="N144" s="14" t="s">
         <v>195</v>
@@ -13329,24 +13329,24 @@
         <v>195</v>
       </c>
       <c r="P144" s="57" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="Q144" s="59" t="s">
-        <v>471</v>
+        <v>1</v>
       </c>
       <c r="R144" s="58" t="s">
-        <v>164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A145" s="45" t="s">
-        <v>631</v>
+        <v>1008</v>
       </c>
       <c r="B145" s="47" t="s">
-        <v>632</v>
+        <v>979</v>
       </c>
       <c r="C145" s="47" t="s">
-        <v>633</v>
+        <v>980</v>
       </c>
       <c r="D145" s="47" t="s">
         <v>720</v>
@@ -13361,7 +13361,7 @@
         <v>322</v>
       </c>
       <c r="H145" s="47" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="I145" s="47" t="s">
         <v>802</v>
@@ -13371,10 +13371,10 @@
         <v>1034</v>
       </c>
       <c r="L145" s="47" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="M145" s="47" t="s">
-        <v>521</v>
+        <v>956</v>
       </c>
       <c r="N145" s="14" t="s">
         <v>195</v>
@@ -13394,13 +13394,13 @@
     </row>
     <row r="146" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="45" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B146" s="47" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C146" s="47" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="D146" s="47" t="s">
         <v>720</v>
@@ -13448,13 +13448,13 @@
     </row>
     <row r="147" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="45" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B147" s="47" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C147" s="47" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="D147" s="47" t="s">
         <v>720</v>
@@ -13469,7 +13469,7 @@
         <v>322</v>
       </c>
       <c r="H147" s="47" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="I147" s="47" t="s">
         <v>802</v>
@@ -13502,13 +13502,13 @@
     </row>
     <row r="148" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A148" s="45" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B148" s="47" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C148" s="47" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="D148" s="47" t="s">
         <v>720</v>
@@ -13523,7 +13523,7 @@
         <v>322</v>
       </c>
       <c r="H148" s="47" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="I148" s="47" t="s">
         <v>802</v>
@@ -13533,10 +13533,10 @@
         <v>1034</v>
       </c>
       <c r="L148" s="47" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="M148" s="47" t="s">
-        <v>956</v>
+        <v>993</v>
       </c>
       <c r="N148" s="14" t="s">
         <v>195</v>
@@ -13556,13 +13556,13 @@
     </row>
     <row r="149" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A149" s="45" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B149" s="47" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="C149" s="47" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D149" s="47" t="s">
         <v>720</v>
@@ -13605,18 +13605,18 @@
         <v>1</v>
       </c>
       <c r="R149" s="58" t="s">
-        <v>1</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="150" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="45" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B150" s="47" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="C150" s="47" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="D150" s="47" t="s">
         <v>720</v>
@@ -13659,18 +13659,18 @@
         <v>1</v>
       </c>
       <c r="R150" s="58" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="151" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A151" s="45" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B151" s="47" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C151" s="47" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D151" s="47" t="s">
         <v>720</v>
@@ -13713,18 +13713,18 @@
         <v>1</v>
       </c>
       <c r="R151" s="58" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="152" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A152" s="45" t="s">
-        <v>1014</v>
+        <v>228</v>
       </c>
       <c r="B152" s="47" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="C152" s="47" t="s">
-        <v>992</v>
+        <v>977</v>
       </c>
       <c r="D152" s="47" t="s">
         <v>720</v>
@@ -13749,10 +13749,10 @@
         <v>1034</v>
       </c>
       <c r="L152" s="47" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="M152" s="47" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="N152" s="14" t="s">
         <v>195</v>
@@ -13767,18 +13767,18 @@
         <v>1</v>
       </c>
       <c r="R152" s="58" t="s">
-        <v>1057</v>
+        <v>110</v>
       </c>
     </row>
     <row r="153" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A153" s="45" t="s">
-        <v>228</v>
+        <v>996</v>
       </c>
       <c r="B153" s="47" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="C153" s="47" t="s">
-        <v>977</v>
+        <v>998</v>
       </c>
       <c r="D153" s="47" t="s">
         <v>720</v>
@@ -13806,7 +13806,7 @@
         <v>1069</v>
       </c>
       <c r="M153" s="47" t="s">
-        <v>995</v>
+        <v>521</v>
       </c>
       <c r="N153" s="14" t="s">
         <v>195</v>
@@ -13821,18 +13821,18 @@
         <v>1</v>
       </c>
       <c r="R153" s="58" t="s">
-        <v>110</v>
+        <v>488</v>
       </c>
     </row>
     <row r="154" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="45" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="B154" s="47" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
       <c r="C154" s="47" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="D154" s="47" t="s">
         <v>720</v>
@@ -13860,7 +13860,7 @@
         <v>1069</v>
       </c>
       <c r="M154" s="47" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N154" s="14" t="s">
         <v>195</v>
@@ -13875,46 +13875,46 @@
         <v>1</v>
       </c>
       <c r="R154" s="58" t="s">
-        <v>488</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="1:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="A155" s="45" t="s">
-        <v>999</v>
-      </c>
-      <c r="B155" s="47" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C155" s="47" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D155" s="47" t="s">
-        <v>720</v>
-      </c>
-      <c r="E155" s="47" t="s">
-        <v>645</v>
-      </c>
-      <c r="F155" s="47" t="s">
-        <v>831</v>
-      </c>
-      <c r="G155" s="47" t="s">
-        <v>322</v>
-      </c>
-      <c r="H155" s="47" t="s">
-        <v>1098</v>
-      </c>
-      <c r="I155" s="47" t="s">
-        <v>802</v>
-      </c>
-      <c r="J155" s="85"/>
-      <c r="K155" s="47" t="s">
+      <c r="A155" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B155" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C155" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D155" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>731</v>
+      </c>
+      <c r="F155" s="24" t="s">
+        <v>731</v>
+      </c>
+      <c r="G155" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="H155" s="24" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I155" s="24" t="s">
+        <v>802</v>
+      </c>
+      <c r="J155" s="86"/>
+      <c r="K155" s="24" t="s">
         <v>1034</v>
       </c>
-      <c r="L155" s="47" t="s">
-        <v>1069</v>
-      </c>
-      <c r="M155" s="47" t="s">
-        <v>515</v>
+      <c r="L155" s="24" t="s">
+        <v>570</v>
+      </c>
+      <c r="M155" s="24" t="s">
+        <v>601</v>
       </c>
       <c r="N155" s="14" t="s">
         <v>195</v>
@@ -13923,24 +13923,22 @@
         <v>195</v>
       </c>
       <c r="P155" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q155" s="59" t="s">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="Q155" s="59"/>
       <c r="R155" s="58" t="s">
-        <v>209</v>
+        <v>118</v>
       </c>
     </row>
     <row r="156" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="25" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="B156" s="26" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C156" s="24" t="s">
-        <v>205</v>
+        <v>574</v>
       </c>
       <c r="D156" s="24" t="s">
         <v>720</v>
@@ -13955,7 +13953,7 @@
         <v>365</v>
       </c>
       <c r="H156" s="24" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="I156" s="24" t="s">
         <v>802</v>
@@ -13965,10 +13963,10 @@
         <v>1034</v>
       </c>
       <c r="L156" s="24" t="s">
-        <v>570</v>
+        <v>1069</v>
       </c>
       <c r="M156" s="24" t="s">
-        <v>601</v>
+        <v>516</v>
       </c>
       <c r="N156" s="14" t="s">
         <v>195</v>
@@ -13977,22 +13975,24 @@
         <v>195</v>
       </c>
       <c r="P156" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q156" s="59"/>
+        <v>47</v>
+      </c>
+      <c r="Q156" s="59" t="s">
+        <v>473</v>
+      </c>
       <c r="R156" s="58" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="157" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="25" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B157" s="26" t="s">
-        <v>173</v>
+        <v>593</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>720</v>
@@ -14007,7 +14007,7 @@
         <v>365</v>
       </c>
       <c r="H157" s="24" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="I157" s="24" t="s">
         <v>802</v>
@@ -14020,7 +14020,7 @@
         <v>1069</v>
       </c>
       <c r="M157" s="24" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="N157" s="14" t="s">
         <v>195</v>
@@ -14028,25 +14028,25 @@
       <c r="O157" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P157" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q157" s="59" t="s">
-        <v>473</v>
+      <c r="P157" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q157" s="55" t="s">
+        <v>470</v>
       </c>
       <c r="R157" s="58" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="158" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B158" s="26" t="s">
-        <v>593</v>
+        <v>163</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D158" s="24" t="s">
         <v>720</v>
@@ -14061,7 +14061,7 @@
         <v>365</v>
       </c>
       <c r="H158" s="24" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="I158" s="24" t="s">
         <v>802</v>
@@ -14071,10 +14071,10 @@
         <v>1034</v>
       </c>
       <c r="L158" s="24" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="M158" s="24" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N158" s="14" t="s">
         <v>195</v>
@@ -14083,24 +14083,24 @@
         <v>195</v>
       </c>
       <c r="P158" s="55" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="Q158" s="55" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="R158" s="58" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="159" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="25" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B159" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D159" s="24" t="s">
         <v>720</v>
@@ -14137,7 +14137,7 @@
         <v>195</v>
       </c>
       <c r="P159" s="55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q159" s="55" t="s">
         <v>471</v>
@@ -14148,13 +14148,13 @@
     </row>
     <row r="160" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="25" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B160" s="26" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>577</v>
+        <v>32</v>
       </c>
       <c r="D160" s="24" t="s">
         <v>720</v>
@@ -14182,7 +14182,7 @@
         <v>1068</v>
       </c>
       <c r="M160" s="24" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="N160" s="14" t="s">
         <v>195</v>
@@ -14191,24 +14191,24 @@
         <v>195</v>
       </c>
       <c r="P160" s="55" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="Q160" s="55" t="s">
         <v>471</v>
       </c>
       <c r="R160" s="58" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="161" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
-        <v>253</v>
+        <v>651</v>
       </c>
       <c r="B161" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C161" s="24" t="s">
-        <v>32</v>
+      <c r="C161" s="26" t="s">
+        <v>647</v>
       </c>
       <c r="D161" s="24" t="s">
         <v>720</v>
@@ -14219,24 +14219,24 @@
       <c r="F161" s="24" t="s">
         <v>731</v>
       </c>
-      <c r="G161" s="24" t="s">
+      <c r="G161" s="26" t="s">
         <v>365</v>
       </c>
       <c r="H161" s="24" t="s">
         <v>1091</v>
       </c>
-      <c r="I161" s="24" t="s">
-        <v>802</v>
-      </c>
-      <c r="J161" s="86"/>
+      <c r="I161" s="26" t="s">
+        <v>802</v>
+      </c>
+      <c r="J161" s="87"/>
       <c r="K161" s="24" t="s">
         <v>1034</v>
       </c>
       <c r="L161" s="24" t="s">
         <v>1068</v>
       </c>
-      <c r="M161" s="24" t="s">
-        <v>506</v>
+      <c r="M161" s="26" t="s">
+        <v>696</v>
       </c>
       <c r="N161" s="14" t="s">
         <v>195</v>
@@ -14245,24 +14245,24 @@
         <v>195</v>
       </c>
       <c r="P161" s="55" t="s">
-        <v>32</v>
+        <v>695</v>
       </c>
       <c r="Q161" s="55" t="s">
-        <v>471</v>
+        <v>1</v>
       </c>
       <c r="R161" s="58" t="s">
-        <v>147</v>
+        <v>696</v>
       </c>
     </row>
     <row r="162" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>146</v>
+        <v>693</v>
       </c>
       <c r="C162" s="26" t="s">
-        <v>647</v>
+        <v>721</v>
       </c>
       <c r="D162" s="24" t="s">
         <v>720</v>
@@ -14277,20 +14277,20 @@
         <v>365</v>
       </c>
       <c r="H162" s="24" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I162" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J162" s="87"/>
-      <c r="K162" s="24" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L162" s="24" t="s">
-        <v>1068</v>
+      <c r="K162" s="26" t="s">
+        <v>1041</v>
+      </c>
+      <c r="L162" s="26" t="s">
+        <v>1072</v>
       </c>
       <c r="M162" s="26" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="N162" s="14" t="s">
         <v>195</v>
@@ -14299,24 +14299,24 @@
         <v>195</v>
       </c>
       <c r="P162" s="55" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="Q162" s="55" t="s">
         <v>1</v>
       </c>
       <c r="R162" s="58" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="163" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="25" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="C163" s="26" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="D163" s="24" t="s">
         <v>720</v>
@@ -14331,20 +14331,20 @@
         <v>365</v>
       </c>
       <c r="H163" s="24" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="I163" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J163" s="87"/>
       <c r="K163" s="26" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L163" s="26" t="s">
-        <v>1072</v>
+        <v>1040</v>
       </c>
       <c r="M163" s="26" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="N163" s="14" t="s">
         <v>195</v>
@@ -14353,24 +14353,24 @@
         <v>195</v>
       </c>
       <c r="P163" s="55" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="Q163" s="55" t="s">
         <v>1</v>
       </c>
       <c r="R163" s="58" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="164" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="25" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B164" s="26" t="s">
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="C164" s="26" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
       <c r="D164" s="24" t="s">
         <v>720</v>
@@ -14385,20 +14385,20 @@
         <v>365</v>
       </c>
       <c r="H164" s="24" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="I164" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J164" s="87"/>
-      <c r="K164" s="26" t="s">
-        <v>1040</v>
-      </c>
-      <c r="L164" s="26" t="s">
-        <v>1040</v>
+      <c r="K164" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L164" s="24" t="s">
+        <v>1068</v>
       </c>
       <c r="M164" s="26" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="N164" s="14" t="s">
         <v>195</v>
@@ -14407,24 +14407,24 @@
         <v>195</v>
       </c>
       <c r="P164" s="55" t="s">
-        <v>699</v>
+        <v>1</v>
       </c>
       <c r="Q164" s="55" t="s">
         <v>1</v>
       </c>
       <c r="R164" s="58" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
     </row>
     <row r="165" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A165" s="25" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B165" s="26" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="C165" s="26" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D165" s="24" t="s">
         <v>720</v>
@@ -14439,20 +14439,20 @@
         <v>365</v>
       </c>
       <c r="H165" s="24" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="I165" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J165" s="87"/>
-      <c r="K165" s="24" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L165" s="24" t="s">
-        <v>1068</v>
+      <c r="K165" s="26" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L165" s="26" t="s">
+        <v>1040</v>
       </c>
       <c r="M165" s="26" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="N165" s="14" t="s">
         <v>195</v>
@@ -14461,24 +14461,22 @@
         <v>195</v>
       </c>
       <c r="P165" s="55" t="s">
-        <v>1</v>
+        <v>701</v>
       </c>
       <c r="Q165" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="R165" s="58" t="s">
-        <v>681</v>
-      </c>
+      <c r="R165" s="58"/>
     </row>
     <row r="166" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B166" s="26" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C166" s="26" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D166" s="24" t="s">
         <v>720</v>
@@ -14492,21 +14490,21 @@
       <c r="G166" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H166" s="24" t="s">
-        <v>1093</v>
+      <c r="H166" s="26" t="s">
+        <v>1094</v>
       </c>
       <c r="I166" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J166" s="87"/>
       <c r="K166" s="26" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="L166" s="26" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="M166" s="26" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="N166" s="14" t="s">
         <v>195</v>
@@ -14515,22 +14513,24 @@
         <v>195</v>
       </c>
       <c r="P166" s="55" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="Q166" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="R166" s="58"/>
+      <c r="R166" s="58" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="167" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A167" s="25" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B167" s="26" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C167" s="26" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D167" s="24" t="s">
         <v>720</v>
@@ -14544,21 +14544,21 @@
       <c r="G167" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H167" s="26" t="s">
-        <v>1094</v>
+      <c r="H167" s="24" t="s">
+        <v>1093</v>
       </c>
       <c r="I167" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J167" s="87"/>
       <c r="K167" s="26" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="L167" s="26" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="M167" s="26" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="N167" s="14" t="s">
         <v>195</v>
@@ -14567,24 +14567,24 @@
         <v>195</v>
       </c>
       <c r="P167" s="55" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="Q167" s="55" t="s">
         <v>1</v>
       </c>
       <c r="R167" s="58" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="168" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A168" s="25" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B168" s="26" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="C168" s="26" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D168" s="24" t="s">
         <v>720</v>
@@ -14598,21 +14598,19 @@
       <c r="G168" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H168" s="24" t="s">
-        <v>1093</v>
-      </c>
+      <c r="H168" s="26"/>
       <c r="I168" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J168" s="87"/>
       <c r="K168" s="26" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L168" s="26" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="M168" s="26" t="s">
-        <v>687</v>
+        <v>717</v>
       </c>
       <c r="N168" s="14" t="s">
         <v>195</v>
@@ -14621,24 +14619,22 @@
         <v>195</v>
       </c>
       <c r="P168" s="55" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
       <c r="Q168" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="R168" s="58" t="s">
-        <v>687</v>
-      </c>
+      <c r="R168" s="58"/>
     </row>
     <row r="169" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A169" s="25" t="s">
-        <v>660</v>
+        <v>833</v>
       </c>
       <c r="B169" s="26" t="s">
-        <v>691</v>
+        <v>832</v>
       </c>
       <c r="C169" s="26" t="s">
-        <v>726</v>
+        <v>836</v>
       </c>
       <c r="D169" s="24" t="s">
         <v>720</v>
@@ -14652,43 +14648,39 @@
       <c r="G169" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H169" s="26"/>
+      <c r="H169" s="24" t="s">
+        <v>1091</v>
+      </c>
       <c r="I169" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J169" s="87"/>
-      <c r="K169" s="26" t="s">
-        <v>1039</v>
+      <c r="K169" s="24" t="s">
+        <v>1034</v>
       </c>
       <c r="L169" s="26" t="s">
-        <v>1039</v>
+        <v>570</v>
       </c>
       <c r="M169" s="26" t="s">
-        <v>717</v>
+        <v>570</v>
       </c>
       <c r="N169" s="14" t="s">
         <v>195</v>
       </c>
       <c r="O169" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="P169" s="55" t="s">
-        <v>692</v>
-      </c>
-      <c r="Q169" s="55" t="s">
-        <v>1</v>
       </c>
       <c r="R169" s="58"/>
     </row>
     <row r="170" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B170" s="26" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C170" s="26" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="D170" s="24" t="s">
         <v>720</v>
@@ -14712,11 +14704,11 @@
       <c r="K170" s="24" t="s">
         <v>1034</v>
       </c>
-      <c r="L170" s="26" t="s">
-        <v>570</v>
+      <c r="L170" s="24" t="s">
+        <v>1068</v>
       </c>
       <c r="M170" s="26" t="s">
-        <v>570</v>
+        <v>838</v>
       </c>
       <c r="N170" s="14" t="s">
         <v>195</v>
@@ -14724,17 +14716,19 @@
       <c r="O170" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R170" s="58"/>
+      <c r="R170" s="58" t="s">
+        <v>1053</v>
+      </c>
     </row>
     <row r="171" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="C171" s="26" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="D171" s="24" t="s">
         <v>720</v>
@@ -14762,7 +14756,7 @@
         <v>1068</v>
       </c>
       <c r="M171" s="26" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="N171" s="14" t="s">
         <v>195</v>
@@ -14771,18 +14765,18 @@
         <v>195</v>
       </c>
       <c r="R171" s="58" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="172" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A172" s="25" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="B172" s="26" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="C172" s="26" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="D172" s="24" t="s">
         <v>720</v>
@@ -14797,7 +14791,7 @@
         <v>365</v>
       </c>
       <c r="H172" s="24" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c r="I172" s="26" t="s">
         <v>802</v>
@@ -14824,13 +14818,13 @@
     </row>
     <row r="173" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A173" s="25" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B173" s="26" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="C173" s="26" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="D173" s="24" t="s">
         <v>720</v>
@@ -14845,7 +14839,7 @@
         <v>365</v>
       </c>
       <c r="H173" s="24" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="I173" s="26" t="s">
         <v>802</v>
@@ -14858,7 +14852,7 @@
         <v>1068</v>
       </c>
       <c r="M173" s="26" t="s">
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="N173" s="14" t="s">
         <v>195</v>
@@ -14866,19 +14860,17 @@
       <c r="O173" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R173" s="58" t="s">
-        <v>1054</v>
-      </c>
+      <c r="R173" s="58"/>
     </row>
     <row r="174" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A174" s="25" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="B174" s="26" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="C174" s="26" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="D174" s="24" t="s">
         <v>720</v>
@@ -14893,7 +14885,7 @@
         <v>365</v>
       </c>
       <c r="H174" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I174" s="26" t="s">
         <v>802</v>
@@ -14903,10 +14895,10 @@
         <v>1034</v>
       </c>
       <c r="L174" s="24" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="M174" s="26" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="N174" s="14" t="s">
         <v>195</v>
@@ -14918,13 +14910,13 @@
     </row>
     <row r="175" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A175" s="25" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B175" s="26" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="C175" s="26" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="D175" s="24" t="s">
         <v>720</v>
@@ -14939,7 +14931,7 @@
         <v>365</v>
       </c>
       <c r="H175" s="24" t="s">
-        <v>1099</v>
+        <v>1091</v>
       </c>
       <c r="I175" s="26" t="s">
         <v>802</v>
@@ -14949,10 +14941,10 @@
         <v>1034</v>
       </c>
       <c r="L175" s="24" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="M175" s="26" t="s">
-        <v>853</v>
+        <v>516</v>
       </c>
       <c r="N175" s="14" t="s">
         <v>195</v>
@@ -14964,13 +14956,13 @@
     </row>
     <row r="176" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A176" s="25" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C176" s="26" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="D176" s="24" t="s">
         <v>720</v>
@@ -14985,7 +14977,7 @@
         <v>365</v>
       </c>
       <c r="H176" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I176" s="26" t="s">
         <v>802</v>
@@ -14995,10 +14987,10 @@
         <v>1034</v>
       </c>
       <c r="L176" s="24" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="M176" s="26" t="s">
-        <v>516</v>
+        <v>860</v>
       </c>
       <c r="N176" s="14" t="s">
         <v>195</v>
@@ -15010,13 +15002,13 @@
     </row>
     <row r="177" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
       <c r="C177" s="26" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="D177" s="24" t="s">
         <v>720</v>
@@ -15031,7 +15023,7 @@
         <v>365</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>1099</v>
+        <v>1091</v>
       </c>
       <c r="I177" s="26" t="s">
         <v>802</v>
@@ -15041,10 +15033,10 @@
         <v>1034</v>
       </c>
       <c r="L177" s="24" t="s">
-        <v>1067</v>
+        <v>570</v>
       </c>
       <c r="M177" s="26" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="N177" s="14" t="s">
         <v>195</v>
@@ -15056,13 +15048,13 @@
     </row>
     <row r="178" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A178" s="25" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="C178" s="26" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="D178" s="24" t="s">
         <v>720</v>
@@ -15087,10 +15079,10 @@
         <v>1034</v>
       </c>
       <c r="L178" s="24" t="s">
-        <v>570</v>
+        <v>1067</v>
       </c>
       <c r="M178" s="26" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="N178" s="14" t="s">
         <v>195</v>
@@ -15098,17 +15090,19 @@
       <c r="O178" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R178" s="58"/>
+      <c r="R178" s="58" t="s">
+        <v>1058</v>
+      </c>
     </row>
     <row r="179" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C179" s="26" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="D179" s="24" t="s">
         <v>720</v>
@@ -15123,7 +15117,7 @@
         <v>365</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="I179" s="26" t="s">
         <v>802</v>
@@ -15136,7 +15130,7 @@
         <v>1067</v>
       </c>
       <c r="M179" s="26" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="N179" s="14" t="s">
         <v>195</v>
@@ -15145,18 +15139,18 @@
         <v>195</v>
       </c>
       <c r="R179" s="58" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="180" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A180" s="25" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="C180" s="26" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D180" s="24" t="s">
         <v>720</v>
@@ -15171,7 +15165,7 @@
         <v>365</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>1099</v>
+        <v>1091</v>
       </c>
       <c r="I180" s="26" t="s">
         <v>802</v>
@@ -15181,10 +15175,10 @@
         <v>1034</v>
       </c>
       <c r="L180" s="24" t="s">
-        <v>1067</v>
+        <v>570</v>
       </c>
       <c r="M180" s="26" t="s">
-        <v>853</v>
+        <v>863</v>
       </c>
       <c r="N180" s="14" t="s">
         <v>195</v>
@@ -15192,19 +15186,17 @@
       <c r="O180" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R180" s="58" t="s">
-        <v>1059</v>
-      </c>
+      <c r="R180" s="58"/>
     </row>
     <row r="181" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A181" s="25" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="C181" s="26" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="D181" s="24" t="s">
         <v>720</v>
@@ -15229,10 +15221,10 @@
         <v>1034</v>
       </c>
       <c r="L181" s="24" t="s">
-        <v>570</v>
+        <v>1067</v>
       </c>
       <c r="M181" s="26" t="s">
-        <v>863</v>
+        <v>1060</v>
       </c>
       <c r="N181" s="14" t="s">
         <v>195</v>
@@ -15240,17 +15232,19 @@
       <c r="O181" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R181" s="58"/>
+      <c r="R181" s="58" t="s">
+        <v>1060</v>
+      </c>
     </row>
     <row r="182" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A182" s="25" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="C182" s="26" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="D182" s="24" t="s">
         <v>720</v>
@@ -15275,10 +15269,10 @@
         <v>1034</v>
       </c>
       <c r="L182" s="24" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="M182" s="26" t="s">
-        <v>1060</v>
+        <v>877</v>
       </c>
       <c r="N182" s="14" t="s">
         <v>195</v>
@@ -15287,18 +15281,18 @@
         <v>195</v>
       </c>
       <c r="R182" s="58" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="183" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A183" s="25" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="C183" s="26" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="D183" s="24" t="s">
         <v>720</v>
@@ -15323,10 +15317,10 @@
         <v>1034</v>
       </c>
       <c r="L183" s="24" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="M183" s="26" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="N183" s="14" t="s">
         <v>195</v>
@@ -15335,18 +15329,18 @@
         <v>195</v>
       </c>
       <c r="R183" s="58" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="C184" s="26" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="D184" s="24" t="s">
         <v>720</v>
@@ -15360,21 +15354,21 @@
       <c r="G184" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H184" s="24" t="s">
-        <v>1091</v>
+      <c r="H184" s="26" t="s">
+        <v>1090</v>
       </c>
       <c r="I184" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J184" s="87"/>
-      <c r="K184" s="24" t="s">
-        <v>1034</v>
+      <c r="K184" s="26" t="s">
+        <v>1033</v>
       </c>
       <c r="L184" s="24" t="s">
-        <v>1075</v>
+        <v>1086</v>
       </c>
       <c r="M184" s="26" t="s">
-        <v>884</v>
+        <v>1085</v>
       </c>
       <c r="N184" s="14" t="s">
         <v>195</v>
@@ -15382,19 +15376,21 @@
       <c r="O184" s="14" t="s">
         <v>195</v>
       </c>
+      <c r="P184" s="1"/>
+      <c r="Q184"/>
       <c r="R184" s="58" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="185" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A185" s="25" t="s">
-        <v>887</v>
+        <v>1021</v>
       </c>
       <c r="B185" s="26" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="C185" s="26" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="D185" s="24" t="s">
         <v>720</v>
@@ -15408,21 +15404,21 @@
       <c r="G185" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H185" s="26" t="s">
-        <v>1090</v>
+      <c r="H185" s="24" t="s">
+        <v>1091</v>
       </c>
       <c r="I185" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J185" s="87"/>
-      <c r="K185" s="26" t="s">
-        <v>1033</v>
+      <c r="K185" s="24" t="s">
+        <v>1034</v>
       </c>
       <c r="L185" s="24" t="s">
-        <v>1086</v>
+        <v>570</v>
       </c>
       <c r="M185" s="26" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="N185" s="14" t="s">
         <v>195</v>
@@ -15430,21 +15426,19 @@
       <c r="O185" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P185" s="1"/>
-      <c r="Q185"/>
-      <c r="R185" s="58" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="186" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="P185" s="66"/>
+      <c r="Q185" s="65"/>
+      <c r="R185" s="58"/>
+    </row>
+    <row r="186" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A186" s="25" t="s">
-        <v>1021</v>
+        <v>889</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C186" s="26" t="s">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="D186" s="24" t="s">
         <v>720</v>
@@ -15466,13 +15460,13 @@
       </c>
       <c r="J186" s="87"/>
       <c r="K186" s="24" t="s">
-        <v>1034</v>
+        <v>1083</v>
       </c>
       <c r="L186" s="24" t="s">
-        <v>570</v>
+        <v>1037</v>
       </c>
       <c r="M186" s="26" t="s">
-        <v>1082</v>
+        <v>1063</v>
       </c>
       <c r="N186" s="14" t="s">
         <v>195</v>
@@ -15480,19 +15474,21 @@
       <c r="O186" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P186" s="66"/>
-      <c r="Q186" s="65"/>
-      <c r="R186" s="58"/>
+      <c r="P186" s="1"/>
+      <c r="Q186"/>
+      <c r="R186" s="58" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="187" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
-        <v>889</v>
+        <v>1022</v>
       </c>
       <c r="B187" s="26" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="C187" s="26" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="D187" s="24" t="s">
         <v>720</v>
@@ -15514,13 +15510,13 @@
       </c>
       <c r="J187" s="87"/>
       <c r="K187" s="24" t="s">
-        <v>1083</v>
+        <v>1034</v>
       </c>
       <c r="L187" s="24" t="s">
-        <v>1037</v>
+        <v>1075</v>
       </c>
       <c r="M187" s="26" t="s">
-        <v>1063</v>
+        <v>894</v>
       </c>
       <c r="N187" s="14" t="s">
         <v>195</v>
@@ -15528,21 +15524,18 @@
       <c r="O187" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P187" s="1"/>
-      <c r="Q187"/>
-      <c r="R187" s="58" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="188" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="P187" s="66"/>
+      <c r="R187" s="58"/>
+    </row>
+    <row r="188" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="C188" s="26" t="s">
-        <v>893</v>
+        <v>880</v>
       </c>
       <c r="D188" s="24" t="s">
         <v>720</v>
@@ -15567,10 +15560,10 @@
         <v>1034</v>
       </c>
       <c r="L188" s="24" t="s">
-        <v>1075</v>
+        <v>1068</v>
       </c>
       <c r="M188" s="26" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="N188" s="14" t="s">
         <v>195</v>
@@ -15579,17 +15572,20 @@
         <v>195</v>
       </c>
       <c r="P188" s="66"/>
-      <c r="R188" s="58"/>
-    </row>
-    <row r="189" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="Q188" s="65"/>
+      <c r="R188" s="58" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
-        <v>1023</v>
+        <v>898</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C189" s="26" t="s">
-        <v>880</v>
+        <v>899</v>
       </c>
       <c r="D189" s="24" t="s">
         <v>720</v>
@@ -15604,20 +15600,20 @@
         <v>365</v>
       </c>
       <c r="H189" s="24" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c r="I189" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J189" s="87"/>
       <c r="K189" s="24" t="s">
-        <v>1034</v>
+        <v>1041</v>
       </c>
       <c r="L189" s="24" t="s">
-        <v>1068</v>
+        <v>1043</v>
       </c>
       <c r="M189" s="26" t="s">
-        <v>896</v>
+        <v>1049</v>
       </c>
       <c r="N189" s="14" t="s">
         <v>195</v>
@@ -15625,21 +15621,21 @@
       <c r="O189" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P189" s="66"/>
-      <c r="Q189" s="65"/>
+      <c r="P189" s="1"/>
+      <c r="Q189"/>
       <c r="R189" s="58" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="190" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A190" s="25" t="s">
-        <v>898</v>
+        <v>1017</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="C190" s="26" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="D190" s="24" t="s">
         <v>720</v>
@@ -15654,20 +15650,20 @@
         <v>365</v>
       </c>
       <c r="H190" s="24" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="I190" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J190" s="87"/>
       <c r="K190" s="24" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L190" s="24" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="M190" s="26" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="N190" s="14" t="s">
         <v>195</v>
@@ -15675,21 +15671,20 @@
       <c r="O190" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P190" s="1"/>
-      <c r="Q190"/>
+      <c r="P190" s="66"/>
       <c r="R190" s="58" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="191" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A191" s="25" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="C191" s="26" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="D191" s="24" t="s">
         <v>720</v>
@@ -15710,14 +15705,14 @@
         <v>802</v>
       </c>
       <c r="J191" s="87"/>
-      <c r="K191" s="24" t="s">
+      <c r="K191" s="26" t="s">
         <v>1040</v>
       </c>
-      <c r="L191" s="24" t="s">
+      <c r="L191" s="26" t="s">
         <v>1040</v>
       </c>
       <c r="M191" s="26" t="s">
-        <v>1050</v>
+        <v>904</v>
       </c>
       <c r="N191" s="14" t="s">
         <v>195</v>
@@ -15727,18 +15722,18 @@
       </c>
       <c r="P191" s="66"/>
       <c r="R191" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="192" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A192" s="25" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="C192" s="26" t="s">
-        <v>903</v>
+        <v>910</v>
       </c>
       <c r="D192" s="24" t="s">
         <v>720</v>
@@ -15752,21 +15747,21 @@
       <c r="G192" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H192" s="24" t="s">
-        <v>1093</v>
+      <c r="H192" s="26" t="s">
+        <v>1090</v>
       </c>
       <c r="I192" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J192" s="87"/>
       <c r="K192" s="26" t="s">
-        <v>1040</v>
+        <v>1033</v>
       </c>
       <c r="L192" s="26" t="s">
-        <v>1040</v>
+        <v>1081</v>
       </c>
       <c r="M192" s="26" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="N192" s="14" t="s">
         <v>195</v>
@@ -15776,18 +15771,18 @@
       </c>
       <c r="P192" s="66"/>
       <c r="R192" s="58" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="193" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A193" s="25" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B193" s="26" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C193" s="26" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D193" s="24" t="s">
         <v>720</v>
@@ -15812,10 +15807,10 @@
         <v>1033</v>
       </c>
       <c r="L193" s="26" t="s">
-        <v>1081</v>
+        <v>1070</v>
       </c>
       <c r="M193" s="26" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="N193" s="14" t="s">
         <v>195</v>
@@ -15824,19 +15819,17 @@
         <v>195</v>
       </c>
       <c r="P193" s="66"/>
-      <c r="R193" s="58" t="s">
-        <v>1052</v>
-      </c>
+      <c r="R193" s="58"/>
     </row>
     <row r="194" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A194" s="25" t="s">
-        <v>1025</v>
+        <v>656</v>
       </c>
       <c r="B194" s="26" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C194" s="26" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D194" s="24" t="s">
         <v>720</v>
@@ -15851,20 +15844,20 @@
         <v>365</v>
       </c>
       <c r="H194" s="26" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="I194" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J194" s="87"/>
       <c r="K194" s="26" t="s">
-        <v>1033</v>
+        <v>1042</v>
       </c>
       <c r="L194" s="26" t="s">
-        <v>1070</v>
+        <v>1042</v>
       </c>
       <c r="M194" s="26" t="s">
-        <v>908</v>
+        <v>913</v>
       </c>
       <c r="N194" s="14" t="s">
         <v>195</v>
@@ -15877,13 +15870,13 @@
     </row>
     <row r="195" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A195" s="25" t="s">
-        <v>656</v>
+        <v>1015</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
       <c r="C195" s="26" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="D195" s="24" t="s">
         <v>720</v>
@@ -15897,21 +15890,21 @@
       <c r="G195" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H195" s="26" t="s">
-        <v>1094</v>
+      <c r="H195" s="24" t="s">
+        <v>1093</v>
       </c>
       <c r="I195" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J195" s="87"/>
       <c r="K195" s="26" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="L195" s="26" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="M195" s="26" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="N195" s="14" t="s">
         <v>195</v>
@@ -15924,13 +15917,13 @@
     </row>
     <row r="196" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A196" s="25" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="D196" s="24" t="s">
         <v>720</v>
@@ -15945,20 +15938,20 @@
         <v>365</v>
       </c>
       <c r="H196" s="24" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="I196" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J196" s="87"/>
       <c r="K196" s="26" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="L196" s="26" t="s">
-        <v>1040</v>
+        <v>1072</v>
       </c>
       <c r="M196" s="26" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="N196" s="14" t="s">
         <v>195</v>
@@ -15969,15 +15962,15 @@
       <c r="P196" s="66"/>
       <c r="R196" s="58"/>
     </row>
-    <row r="197" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A197" s="25" t="s">
-        <v>1016</v>
+        <v>652</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>917</v>
+        <v>693</v>
       </c>
       <c r="C197" s="26" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="D197" s="24" t="s">
         <v>720</v>
@@ -16005,7 +15998,7 @@
         <v>1072</v>
       </c>
       <c r="M197" s="26" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="N197" s="14" t="s">
         <v>195</v>
@@ -16014,17 +16007,20 @@
         <v>195</v>
       </c>
       <c r="P197" s="66"/>
-      <c r="R197" s="58"/>
+      <c r="Q197" s="65"/>
+      <c r="R197" s="58" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="198" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A198" s="25" t="s">
-        <v>652</v>
+        <v>922</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>693</v>
+        <v>923</v>
       </c>
       <c r="C198" s="26" t="s">
-        <v>921</v>
+        <v>938</v>
       </c>
       <c r="D198" s="24" t="s">
         <v>720</v>
@@ -16039,20 +16035,20 @@
         <v>365</v>
       </c>
       <c r="H198" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="I198" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J198" s="87"/>
-      <c r="K198" s="26" t="s">
-        <v>1041</v>
-      </c>
-      <c r="L198" s="26" t="s">
-        <v>1072</v>
+      <c r="K198" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L198" s="24" t="s">
+        <v>1073</v>
       </c>
       <c r="M198" s="26" t="s">
-        <v>920</v>
+        <v>946</v>
       </c>
       <c r="N198" s="14" t="s">
         <v>195</v>
@@ -16060,21 +16056,19 @@
       <c r="O198" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P198" s="66"/>
-      <c r="Q198" s="65"/>
       <c r="R198" s="58" t="s">
-        <v>697</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="199" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A199" s="25" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="C199" s="26" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="D199" s="24" t="s">
         <v>720</v>
@@ -16088,21 +16082,21 @@
       <c r="G199" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H199" s="24" t="s">
-        <v>1091</v>
+      <c r="H199" s="26" t="s">
+        <v>1090</v>
       </c>
       <c r="I199" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J199" s="87"/>
-      <c r="K199" s="24" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L199" s="24" t="s">
-        <v>1073</v>
+      <c r="K199" s="26" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L199" s="26" t="s">
+        <v>1080</v>
       </c>
       <c r="M199" s="26" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="N199" s="14" t="s">
         <v>195</v>
@@ -16110,19 +16104,17 @@
       <c r="O199" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="R199" s="58" t="s">
-        <v>1064</v>
-      </c>
+      <c r="R199" s="58"/>
     </row>
     <row r="200" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A200" s="25" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="B200" s="26" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C200" s="26" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="D200" s="24" t="s">
         <v>720</v>
@@ -16147,10 +16139,10 @@
         <v>1033</v>
       </c>
       <c r="L200" s="26" t="s">
-        <v>1080</v>
+        <v>1071</v>
       </c>
       <c r="M200" s="26" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="N200" s="14" t="s">
         <v>195</v>
@@ -16162,13 +16154,13 @@
     </row>
     <row r="201" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A201" s="25" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="B201" s="26" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C201" s="26" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="D201" s="24" t="s">
         <v>720</v>
@@ -16182,21 +16174,21 @@
       <c r="G201" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H201" s="26" t="s">
-        <v>1090</v>
+      <c r="H201" s="24" t="s">
+        <v>1091</v>
       </c>
       <c r="I201" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J201" s="87"/>
-      <c r="K201" s="26" t="s">
-        <v>1033</v>
-      </c>
-      <c r="L201" s="26" t="s">
-        <v>1071</v>
+      <c r="K201" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L201" s="24" t="s">
+        <v>1073</v>
       </c>
       <c r="M201" s="26" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="N201" s="14" t="s">
         <v>195</v>
@@ -16208,13 +16200,13 @@
     </row>
     <row r="202" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A202" s="25" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="C202" s="26" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D202" s="24" t="s">
         <v>720</v>
@@ -16229,20 +16221,20 @@
         <v>365</v>
       </c>
       <c r="H202" s="24" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I202" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J202" s="87"/>
-      <c r="K202" s="24" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L202" s="24" t="s">
-        <v>1073</v>
+      <c r="K202" s="26" t="s">
+        <v>1041</v>
+      </c>
+      <c r="L202" s="26" t="s">
+        <v>1072</v>
       </c>
       <c r="M202" s="26" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="N202" s="14" t="s">
         <v>195</v>
@@ -16254,13 +16246,13 @@
     </row>
     <row r="203" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A203" s="25" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="C203" s="26" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D203" s="24" t="s">
         <v>720</v>
@@ -16275,20 +16267,20 @@
         <v>365</v>
       </c>
       <c r="H203" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="I203" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J203" s="87"/>
-      <c r="K203" s="26" t="s">
-        <v>1041</v>
-      </c>
-      <c r="L203" s="26" t="s">
-        <v>1072</v>
+      <c r="K203" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L203" s="24" t="s">
+        <v>570</v>
       </c>
       <c r="M203" s="26" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="N203" s="14" t="s">
         <v>195</v>
@@ -16300,13 +16292,13 @@
     </row>
     <row r="204" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A204" s="25" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="C204" s="26" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="D204" s="24" t="s">
         <v>720</v>
@@ -16320,21 +16312,21 @@
       <c r="G204" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H204" s="24" t="s">
-        <v>1091</v>
+      <c r="H204" s="26" t="s">
+        <v>1090</v>
       </c>
       <c r="I204" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J204" s="87"/>
-      <c r="K204" s="24" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L204" s="24" t="s">
-        <v>570</v>
+      <c r="K204" s="26" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L204" s="26" t="s">
+        <v>1071</v>
       </c>
       <c r="M204" s="26" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="N204" s="14" t="s">
         <v>195</v>
@@ -16344,15 +16336,15 @@
       </c>
       <c r="R204" s="58"/>
     </row>
-    <row r="205" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A205" s="25" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="C205" s="26" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D205" s="24" t="s">
         <v>720</v>
@@ -16366,21 +16358,21 @@
       <c r="G205" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="H205" s="26" t="s">
-        <v>1090</v>
+      <c r="H205" s="24" t="s">
+        <v>1089</v>
       </c>
       <c r="I205" s="26" t="s">
         <v>802</v>
       </c>
       <c r="J205" s="87"/>
       <c r="K205" s="26" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="L205" s="26" t="s">
-        <v>1071</v>
+        <v>570</v>
       </c>
       <c r="M205" s="26" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="N205" s="14" t="s">
         <v>195</v>
@@ -16388,45 +16380,47 @@
       <c r="O205" s="14" t="s">
         <v>195</v>
       </c>
+      <c r="P205" s="1"/>
+      <c r="Q205"/>
       <c r="R205" s="58"/>
     </row>
     <row r="206" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A206" s="25" t="s">
-        <v>936</v>
-      </c>
-      <c r="B206" s="26" t="s">
-        <v>937</v>
-      </c>
-      <c r="C206" s="26" t="s">
-        <v>945</v>
-      </c>
-      <c r="D206" s="24" t="s">
-        <v>720</v>
-      </c>
-      <c r="E206" s="24" t="s">
+      <c r="A206" s="69" t="s">
+        <v>659</v>
+      </c>
+      <c r="B206" s="70" t="s">
+        <v>689</v>
+      </c>
+      <c r="C206" s="70" t="s">
+        <v>728</v>
+      </c>
+      <c r="D206" s="71" t="s">
+        <v>720</v>
+      </c>
+      <c r="E206" s="71" t="s">
         <v>731</v>
       </c>
-      <c r="F206" s="24" t="s">
+      <c r="F206" s="71" t="s">
         <v>731</v>
       </c>
-      <c r="G206" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="H206" s="24" t="s">
-        <v>1089</v>
-      </c>
-      <c r="I206" s="26" t="s">
-        <v>802</v>
-      </c>
-      <c r="J206" s="87"/>
-      <c r="K206" s="26" t="s">
+      <c r="G206" s="70" t="s">
+        <v>413</v>
+      </c>
+      <c r="H206" s="70" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I206" s="70" t="s">
+        <v>802</v>
+      </c>
+      <c r="J206" s="88"/>
+      <c r="K206" s="71" t="s">
         <v>1034</v>
       </c>
-      <c r="L206" s="26" t="s">
+      <c r="L206" s="71" t="s">
         <v>570</v>
       </c>
-      <c r="M206" s="26" t="s">
-        <v>953</v>
+      <c r="M206" s="70" t="s">
+        <v>118</v>
       </c>
       <c r="N206" s="14" t="s">
         <v>195</v>
@@ -16434,19 +16428,25 @@
       <c r="O206" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P206" s="1"/>
-      <c r="Q206"/>
-      <c r="R206" s="58"/>
+      <c r="P206" s="55" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q206" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="R206" s="58" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="207" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A207" s="69" t="s">
-        <v>659</v>
+        <v>251</v>
       </c>
       <c r="B207" s="70" t="s">
-        <v>689</v>
+        <v>143</v>
       </c>
       <c r="C207" s="70" t="s">
-        <v>728</v>
+        <v>586</v>
       </c>
       <c r="D207" s="71" t="s">
         <v>720</v>
@@ -16461,7 +16461,7 @@
         <v>413</v>
       </c>
       <c r="H207" s="70" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I207" s="70" t="s">
         <v>802</v>
@@ -16471,10 +16471,10 @@
         <v>1034</v>
       </c>
       <c r="L207" s="71" t="s">
-        <v>570</v>
+        <v>1069</v>
       </c>
       <c r="M207" s="70" t="s">
-        <v>118</v>
+        <v>517</v>
       </c>
       <c r="N207" s="14" t="s">
         <v>195</v>
@@ -16483,24 +16483,24 @@
         <v>195</v>
       </c>
       <c r="P207" s="55" t="s">
-        <v>690</v>
+        <v>30</v>
       </c>
       <c r="Q207" s="55" t="s">
-        <v>1</v>
+        <v>471</v>
       </c>
       <c r="R207" s="58" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
     </row>
     <row r="208" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A208" s="69" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="B208" s="70" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="C208" s="70" t="s">
-        <v>586</v>
+        <v>343</v>
       </c>
       <c r="D208" s="71" t="s">
         <v>720</v>
@@ -16525,10 +16525,10 @@
         <v>1034</v>
       </c>
       <c r="L208" s="71" t="s">
-        <v>1069</v>
+        <v>570</v>
       </c>
       <c r="M208" s="70" t="s">
-        <v>517</v>
+        <v>570</v>
       </c>
       <c r="N208" s="14" t="s">
         <v>195</v>
@@ -16537,24 +16537,24 @@
         <v>195</v>
       </c>
       <c r="P208" s="55" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="Q208" s="55" t="s">
-        <v>471</v>
+        <v>1</v>
       </c>
       <c r="R208" s="58" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A209" s="69" t="s">
-        <v>218</v>
+        <v>284</v>
       </c>
       <c r="B209" s="70" t="s">
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="C209" s="70" t="s">
-        <v>343</v>
+        <v>434</v>
       </c>
       <c r="D209" s="71" t="s">
         <v>720</v>
@@ -16569,7 +16569,7 @@
         <v>413</v>
       </c>
       <c r="H209" s="70" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="I209" s="70" t="s">
         <v>802</v>
@@ -16591,24 +16591,24 @@
         <v>195</v>
       </c>
       <c r="P209" s="55" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="Q209" s="55" t="s">
-        <v>1</v>
+        <v>471</v>
       </c>
       <c r="R209" s="58" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
     </row>
     <row r="210" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A210" s="69" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="B210" s="70" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C210" s="70" t="s">
-        <v>434</v>
+        <v>585</v>
       </c>
       <c r="D210" s="71" t="s">
         <v>720</v>
@@ -16633,10 +16633,10 @@
         <v>1034</v>
       </c>
       <c r="L210" s="71" t="s">
-        <v>570</v>
+        <v>1068</v>
       </c>
       <c r="M210" s="70" t="s">
-        <v>570</v>
+        <v>518</v>
       </c>
       <c r="N210" s="14" t="s">
         <v>195</v>
@@ -16645,24 +16645,24 @@
         <v>195</v>
       </c>
       <c r="P210" s="55" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q210" s="55" t="s">
         <v>471</v>
       </c>
       <c r="R210" s="58" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="211" spans="1:18" s="65" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A211" s="69" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="B211" s="70" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="C211" s="70" t="s">
-        <v>585</v>
+        <v>345</v>
       </c>
       <c r="D211" s="71" t="s">
         <v>720</v>
@@ -16677,7 +16677,7 @@
         <v>413</v>
       </c>
       <c r="H211" s="70" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I211" s="70" t="s">
         <v>802</v>
@@ -16687,10 +16687,10 @@
         <v>1034</v>
       </c>
       <c r="L211" s="71" t="s">
-        <v>1068</v>
+        <v>570</v>
       </c>
       <c r="M211" s="70" t="s">
-        <v>518</v>
+        <v>118</v>
       </c>
       <c r="N211" s="14" t="s">
         <v>195</v>
@@ -16699,24 +16699,24 @@
         <v>195</v>
       </c>
       <c r="P211" s="55" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="Q211" s="55" t="s">
-        <v>471</v>
+        <v>1</v>
       </c>
       <c r="R211" s="58" t="s">
-        <v>164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A212" s="69" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="B212" s="70" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="C212" s="70" t="s">
-        <v>345</v>
+        <v>584</v>
       </c>
       <c r="D212" s="71" t="s">
         <v>720</v>
@@ -16731,7 +16731,7 @@
         <v>413</v>
       </c>
       <c r="H212" s="70" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="I212" s="70" t="s">
         <v>802</v>
@@ -16741,10 +16741,10 @@
         <v>1034</v>
       </c>
       <c r="L212" s="71" t="s">
-        <v>570</v>
+        <v>1068</v>
       </c>
       <c r="M212" s="70" t="s">
-        <v>118</v>
+        <v>519</v>
       </c>
       <c r="N212" s="14" t="s">
         <v>195</v>
@@ -16753,24 +16753,24 @@
         <v>195</v>
       </c>
       <c r="P212" s="55" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="Q212" s="55" t="s">
-        <v>1</v>
+        <v>471</v>
       </c>
       <c r="R212" s="58" t="s">
-        <v>1</v>
+        <v>149</v>
       </c>
     </row>
     <row r="213" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A213" s="69" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B213" s="70" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="C213" s="70" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D213" s="71" t="s">
         <v>720</v>
@@ -16785,7 +16785,7 @@
         <v>413</v>
       </c>
       <c r="H213" s="70" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I213" s="70" t="s">
         <v>802</v>
@@ -16795,10 +16795,10 @@
         <v>1034</v>
       </c>
       <c r="L213" s="71" t="s">
-        <v>1068</v>
+        <v>570</v>
       </c>
       <c r="M213" s="70" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="N213" s="14" t="s">
         <v>195</v>
@@ -16807,24 +16807,24 @@
         <v>195</v>
       </c>
       <c r="P213" s="55" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Q213" s="55" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="R213" s="58" t="s">
-        <v>149</v>
+        <v>798</v>
       </c>
     </row>
     <row r="214" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A214" s="69" t="s">
-        <v>258</v>
+        <v>658</v>
       </c>
       <c r="B214" s="70" t="s">
-        <v>160</v>
+        <v>688</v>
       </c>
       <c r="C214" s="70" t="s">
-        <v>583</v>
+        <v>727</v>
       </c>
       <c r="D214" s="71" t="s">
         <v>720</v>
@@ -16852,7 +16852,7 @@
         <v>570</v>
       </c>
       <c r="M214" s="70" t="s">
-        <v>520</v>
+        <v>716</v>
       </c>
       <c r="N214" s="14" t="s">
         <v>195</v>
@@ -16861,24 +16861,24 @@
         <v>195</v>
       </c>
       <c r="P214" s="55" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="Q214" s="55" t="s">
-        <v>473</v>
+        <v>1</v>
       </c>
       <c r="R214" s="58" t="s">
-        <v>798</v>
+        <v>716</v>
       </c>
     </row>
     <row r="215" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A215" s="69" t="s">
-        <v>658</v>
+        <v>1026</v>
       </c>
       <c r="B215" s="70" t="s">
-        <v>688</v>
+        <v>954</v>
       </c>
       <c r="C215" s="70" t="s">
-        <v>727</v>
+        <v>955</v>
       </c>
       <c r="D215" s="71" t="s">
         <v>720</v>
@@ -16903,10 +16903,10 @@
         <v>1034</v>
       </c>
       <c r="L215" s="71" t="s">
-        <v>570</v>
+        <v>1067</v>
       </c>
       <c r="M215" s="70" t="s">
-        <v>716</v>
+        <v>956</v>
       </c>
       <c r="N215" s="14" t="s">
         <v>195</v>
@@ -16914,25 +16914,25 @@
       <c r="O215" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P215" s="55" t="s">
+      <c r="P215" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="Q215" s="55" t="s">
+      <c r="Q215" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="R215" s="58" t="s">
+      <c r="R215" s="68" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="216" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A216" s="69" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B216" s="70" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="C216" s="70" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
       <c r="D216" s="71" t="s">
         <v>720</v>
@@ -16968,25 +16968,19 @@
       <c r="O216" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P216" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q216" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="R216" s="68" t="s">
-        <v>716</v>
-      </c>
+      <c r="P216" s="66"/>
+      <c r="Q216" s="65"/>
+      <c r="R216" s="65"/>
     </row>
     <row r="217" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A217" s="69" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B217" s="70" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="C217" s="70" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="D217" s="71" t="s">
         <v>720</v>
@@ -17014,7 +17008,7 @@
         <v>1067</v>
       </c>
       <c r="M217" s="70" t="s">
-        <v>956</v>
+        <v>961</v>
       </c>
       <c r="N217" s="14" t="s">
         <v>195</v>
@@ -17028,13 +17022,13 @@
     </row>
     <row r="218" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A218" s="69" t="s">
-        <v>1028</v>
+        <v>1019</v>
       </c>
       <c r="B218" s="70" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="C218" s="70" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
       <c r="D218" s="71" t="s">
         <v>720</v>
@@ -17059,10 +17053,10 @@
         <v>1034</v>
       </c>
       <c r="L218" s="71" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="M218" s="70" t="s">
-        <v>961</v>
+        <v>521</v>
       </c>
       <c r="N218" s="14" t="s">
         <v>195</v>
@@ -17076,13 +17070,13 @@
     </row>
     <row r="219" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A219" s="69" t="s">
-        <v>1019</v>
+        <v>1029</v>
       </c>
       <c r="B219" s="70" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C219" s="70" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D219" s="71" t="s">
         <v>720</v>
@@ -17124,13 +17118,13 @@
     </row>
     <row r="220" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A220" s="69" t="s">
-        <v>1029</v>
+        <v>1020</v>
       </c>
       <c r="B220" s="70" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C220" s="70" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="D220" s="71" t="s">
         <v>720</v>
@@ -17158,7 +17152,7 @@
         <v>1069</v>
       </c>
       <c r="M220" s="70" t="s">
-        <v>521</v>
+        <v>968</v>
       </c>
       <c r="N220" s="14" t="s">
         <v>195</v>
@@ -17172,13 +17166,13 @@
     </row>
     <row r="221" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A221" s="69" t="s">
-        <v>1020</v>
+        <v>969</v>
       </c>
       <c r="B221" s="70" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="C221" s="70" t="s">
-        <v>967</v>
+        <v>972</v>
       </c>
       <c r="D221" s="71" t="s">
         <v>720</v>
@@ -17193,7 +17187,7 @@
         <v>413</v>
       </c>
       <c r="H221" s="70" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="I221" s="70" t="s">
         <v>802</v>
@@ -17203,10 +17197,10 @@
         <v>1034</v>
       </c>
       <c r="L221" s="71" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="M221" s="70" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="N221" s="14" t="s">
         <v>195</v>
@@ -17214,19 +17208,16 @@
       <c r="O221" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="P221" s="66"/>
-      <c r="Q221" s="65"/>
-      <c r="R221" s="65"/>
     </row>
     <row r="222" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A222" s="69" t="s">
-        <v>969</v>
+        <v>1006</v>
       </c>
       <c r="B222" s="70" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="C222" s="70" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="D222" s="71" t="s">
         <v>720</v>
@@ -17254,7 +17245,7 @@
         <v>1067</v>
       </c>
       <c r="M222" s="70" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c r="N222" s="14" t="s">
         <v>195</v>
@@ -17265,13 +17256,13 @@
     </row>
     <row r="223" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A223" s="69" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B223" s="70" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="C223" s="70" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c r="D223" s="71" t="s">
         <v>720</v>
@@ -17286,20 +17277,20 @@
         <v>413</v>
       </c>
       <c r="H223" s="70" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I223" s="70" t="s">
         <v>802</v>
       </c>
       <c r="J223" s="88"/>
-      <c r="K223" s="71" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L223" s="71" t="s">
-        <v>1067</v>
+      <c r="K223" s="70" t="s">
+        <v>1033</v>
+      </c>
+      <c r="L223" s="70" t="s">
+        <v>1070</v>
       </c>
       <c r="M223" s="70" t="s">
-        <v>975</v>
+        <v>978</v>
       </c>
       <c r="N223" s="14" t="s">
         <v>195</v>
@@ -17310,13 +17301,13 @@
     </row>
     <row r="224" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A224" s="69" t="s">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B224" s="70" t="s">
-        <v>976</v>
+        <v>1003</v>
       </c>
       <c r="C224" s="70" t="s">
-        <v>977</v>
+        <v>1004</v>
       </c>
       <c r="D224" s="71" t="s">
         <v>720</v>
@@ -17336,15 +17327,15 @@
       <c r="I224" s="70" t="s">
         <v>802</v>
       </c>
-      <c r="J224" s="88"/>
-      <c r="K224" s="70" t="s">
-        <v>1033</v>
-      </c>
-      <c r="L224" s="70" t="s">
-        <v>1070</v>
+      <c r="J224" s="89"/>
+      <c r="K224" s="71" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L224" s="71" t="s">
+        <v>570</v>
       </c>
       <c r="M224" s="70" t="s">
-        <v>978</v>
+        <v>1005</v>
       </c>
       <c r="N224" s="14" t="s">
         <v>195</v>
@@ -17353,57 +17344,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A225" s="69" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B225" s="70" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C225" s="70" t="s">
-        <v>1004</v>
-      </c>
-      <c r="D225" s="71" t="s">
-        <v>720</v>
-      </c>
-      <c r="E225" s="71" t="s">
-        <v>731</v>
-      </c>
-      <c r="F225" s="71" t="s">
-        <v>731</v>
-      </c>
-      <c r="G225" s="70" t="s">
-        <v>413</v>
-      </c>
-      <c r="H225" s="70" t="s">
-        <v>1088</v>
-      </c>
-      <c r="I225" s="70" t="s">
-        <v>802</v>
-      </c>
-      <c r="J225" s="89"/>
-      <c r="K225" s="71" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L225" s="71" t="s">
-        <v>570</v>
-      </c>
-      <c r="M225" s="70" t="s">
-        <v>1005</v>
-      </c>
-      <c r="N225" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="O225" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R225">
-    <sortCondition ref="E2:E225"/>
-    <sortCondition ref="F2:F225"/>
-    <sortCondition ref="G2:G225"/>
-    <sortCondition ref="H2:H225"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R224">
+    <sortCondition ref="E2:E224"/>
+    <sortCondition ref="F2:F224"/>
+    <sortCondition ref="G2:G224"/>
+    <sortCondition ref="H2:H224"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B60" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -17420,15 +17366,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>597</v>
       </c>
@@ -17460,7 +17406,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>239</v>
       </c>
@@ -17502,7 +17448,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>614</v>
       </c>
@@ -17546,7 +17492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>667</v>
       </c>
@@ -17589,6 +17535,60 @@
       </c>
       <c r="O8" s="48" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>346</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>720</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>645</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>831</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>802</v>
+      </c>
+      <c r="J9" s="85"/>
+      <c r="K9" s="47" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M9" s="47" t="s">
+        <v>516</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="P9" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q9" s="59" t="s">
+        <v>471</v>
+      </c>
+      <c r="R9" s="58" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated isolation host information
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995ED76E-AEC9-DB4D-A5CB-90E1599D020A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDFE5CD-EBCB-4F44-8019-B74123CDF0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="1940" windowWidth="33480" windowHeight="24020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="1018">
   <si>
     <t>AY632538</t>
   </si>
@@ -3080,6 +3080,9 @@
   </si>
   <si>
     <t>PL3</t>
+  </si>
+  <si>
+    <t>Scorpiones</t>
   </si>
 </sst>
 </file>
@@ -5282,8 +5285,8 @@
   <dimension ref="A1:P252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L143" sqref="A1:N252"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L105" sqref="L105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10568,7 +10571,7 @@
         <v>862</v>
       </c>
       <c r="K120" s="25" t="s">
-        <v>817</v>
+        <v>1017</v>
       </c>
       <c r="L120" s="25" t="s">
         <v>988</v>
@@ -10612,7 +10615,7 @@
         <v>862</v>
       </c>
       <c r="K121" s="25" t="s">
-        <v>817</v>
+        <v>1017</v>
       </c>
       <c r="L121" s="25" t="s">
         <v>988</v>

</xml_diff>

<commit_message>
Refactor - efv trees
</commit_message>
<xml_diff>
--- a/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/flavi-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DBFF61-2CB7-2040-98BE-32F3F9FB1F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993ACC27-948E-2144-BD4D-12E169321764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="680" windowWidth="44860" windowHeight="24800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4709,8 +4709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>